<commit_message>
almost done refactoring (doesn't converge correctly now lol)
</commit_message>
<xml_diff>
--- a/custom sim/two_track_out2.xlsx
+++ b/custom sim/two_track_out2.xlsx
@@ -483,7 +483,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>29.99999739566411</v>
+        <v>0.4025236678718991</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -492,3422 +492,3422 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>-0.2702505563138138</v>
+        <v>-1.923587485323732</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>171.4280177052676</v>
+        <v>171.428573986029</v>
       </c>
       <c r="I2">
-        <v>171.4283835692619</v>
+        <v>-2.557454950492511E-06</v>
       </c>
       <c r="J2">
-        <v>72.59644880647843</v>
+        <v>5.592879920384704</v>
       </c>
       <c r="K2">
-        <v>90.59754701633935</v>
+        <v>107.0518191062842</v>
       </c>
       <c r="L2">
-        <v>-0.0007008544648795109</v>
+        <v>-0.008442906890839983</v>
       </c>
       <c r="M2">
-        <v>449.316120762934</v>
+        <v>0.001849342634680564</v>
       </c>
       <c r="N2">
-        <v>-4.303735218331349E-20</v>
+        <v>-1.188450101141443</v>
       </c>
       <c r="O2">
-        <v>-283.0678199056217</v>
+        <v>-43.42724043924721</v>
       </c>
       <c r="P2">
-        <v>-1.866704920067906</v>
+        <v>-20.80765885514819</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3">
-        <v>0.175148236510452</v>
+        <v>13.50030028985811</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>29.99999983056264</v>
+        <v>0.3758859305097116</v>
       </c>
       <c r="D3">
-        <v>-0.0007553603927464459</v>
+        <v>-0.009146453258830166</v>
       </c>
       <c r="E3">
-        <v>0.005775513476068665</v>
+        <v>-0.002840094275378657</v>
       </c>
       <c r="F3">
-        <v>-0.2700888252871915</v>
+        <v>-2.000000026991795</v>
       </c>
       <c r="G3">
-        <v>0.0008699662100687607</v>
+        <v>-0.01992736453858513</v>
       </c>
       <c r="H3">
-        <v>85.57449085625431</v>
+        <v>171.4285707383771</v>
       </c>
       <c r="I3">
-        <v>86.42261887572441</v>
+        <v>55.45623919978623</v>
       </c>
       <c r="J3">
-        <v>101.911935913443</v>
+        <v>0.03933852893697091</v>
       </c>
       <c r="K3">
-        <v>93.88818366908896</v>
+        <v>101.1940606700598</v>
       </c>
       <c r="L3">
-        <v>-0.02504570173229527</v>
+        <v>0.01350520335297163</v>
       </c>
       <c r="M3">
-        <v>404.2397083497763</v>
+        <v>2.404275986633913</v>
       </c>
       <c r="N3">
-        <v>1.203251192425251E-27</v>
+        <v>0.0001998491605094467</v>
       </c>
       <c r="O3">
-        <v>-245.2490418743137</v>
+        <v>172.6992316535219</v>
       </c>
       <c r="P3">
-        <v>21.29130960883162</v>
+        <v>94.6351032206619</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4">
-        <v>0.3501486729923848</v>
+        <v>27.09410522723888</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>29.9988015889761</v>
+        <v>0.3970776190966772</v>
       </c>
       <c r="D4">
-        <v>-0.00559082339246463</v>
+        <v>0.02416015140907168</v>
       </c>
       <c r="E4">
-        <v>-0.003262681252059567</v>
+        <v>0.007127760551605367</v>
       </c>
       <c r="F4">
-        <v>-0.2827516960506198</v>
+        <v>-1.982222532411391</v>
       </c>
       <c r="G4">
-        <v>0.001092901668211778</v>
+        <v>0.01198207239015201</v>
       </c>
       <c r="H4">
-        <v>85.78825623760189</v>
+        <v>6.910984529323092E-07</v>
       </c>
       <c r="I4">
-        <v>85.09782003942341</v>
+        <v>71.16985477815466</v>
       </c>
       <c r="J4">
-        <v>103.7239749205084</v>
+        <v>35.85645322050225</v>
       </c>
       <c r="K4">
-        <v>93.94209242061122</v>
+        <v>134.642221313657</v>
       </c>
       <c r="L4">
-        <v>-0.05231688253363346</v>
+        <v>-0.007183289095877532</v>
       </c>
       <c r="M4">
-        <v>404.7353104071987</v>
+        <v>0.0007105472821708751</v>
       </c>
       <c r="N4">
-        <v>-1.940005093046536E-27</v>
+        <v>-2.611588034178653</v>
       </c>
       <c r="O4">
-        <v>-263.9921329831768</v>
+        <v>-209.5803358827978</v>
       </c>
       <c r="P4">
-        <v>39.06927319012095</v>
+        <v>-110.327168194697</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5">
-        <v>0.5251595317725035</v>
+        <v>41.21219702908144</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>29.99999963866599</v>
+        <v>0.3480958008756005</v>
       </c>
       <c r="D5">
-        <v>-0.01079945548171086</v>
+        <v>-0.03112138228219068</v>
       </c>
       <c r="E5">
-        <v>-0.02050228251169342</v>
+        <v>-0.003701259158805437</v>
       </c>
       <c r="F5">
-        <v>-0.3264813428942182</v>
+        <v>-1.982028185292249</v>
       </c>
       <c r="G5">
-        <v>-0.0009704810072043052</v>
+        <v>-0.004283101064455341</v>
       </c>
       <c r="H5">
-        <v>85.4605259126847</v>
+        <v>171.4285734857922</v>
       </c>
       <c r="I5">
-        <v>86.10894944589667</v>
+        <v>171.4285735952785</v>
       </c>
       <c r="J5">
-        <v>103.4894607824712</v>
+        <v>18.5048155206608</v>
       </c>
       <c r="K5">
-        <v>94.13056251564815</v>
+        <v>112.6749464594002</v>
       </c>
       <c r="L5">
-        <v>-0.04653400602082683</v>
+        <v>0.01199820563138037</v>
       </c>
       <c r="M5">
-        <v>397.1658166988021</v>
+        <v>1.524565923907109</v>
       </c>
       <c r="N5">
-        <v>-2.943282834618596E-26</v>
+        <v>0.0001999828067136122</v>
       </c>
       <c r="O5">
-        <v>-250.7120530595055</v>
+        <v>282.9648999281249</v>
       </c>
       <c r="P5">
-        <v>33.50820073452412</v>
+        <v>172.286353954202</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6">
-        <v>0.7002007032934222</v>
+        <v>55.50499235808775</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>29.99244363851315</v>
+        <v>0.3873166245431029</v>
       </c>
       <c r="D6">
-        <v>-0.01116894665144502</v>
+        <v>0.04471729166097636</v>
       </c>
       <c r="E6">
-        <v>-0.0368260356533487</v>
+        <v>0.007221939080635714</v>
       </c>
       <c r="F6">
-        <v>-0.4024800883557253</v>
+        <v>-1.896014082180723</v>
       </c>
       <c r="G6">
-        <v>-0.005992750146944469</v>
+        <v>0.02395347815962818</v>
       </c>
       <c r="H6">
-        <v>85.67282798612499</v>
+        <v>-2.557669447712158E-06</v>
       </c>
       <c r="I6">
-        <v>85.41484272524832</v>
+        <v>152.9130860348284</v>
       </c>
       <c r="J6">
-        <v>103.3698978150644</v>
+        <v>46.4689003087034</v>
       </c>
       <c r="K6">
-        <v>93.84390508083925</v>
+        <v>134.3430030187501</v>
       </c>
       <c r="L6">
-        <v>-0.0523431534041934</v>
+        <v>-0.0131341041674196</v>
       </c>
       <c r="M6">
-        <v>402.994166745402</v>
+        <v>0.0003711714419971881</v>
       </c>
       <c r="N6">
-        <v>4.581089132841495E-27</v>
+        <v>-4.6852767963984</v>
       </c>
       <c r="O6">
-        <v>-264.3889453881312</v>
+        <v>-299.294826222171</v>
       </c>
       <c r="P6">
-        <v>43.24325580077888</v>
+        <v>-176.6703432633724</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7">
-        <v>0.8752634688893306</v>
+        <v>70.6289001077414</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>29.99999524687372</v>
+        <v>0.309872689562307</v>
       </c>
       <c r="D7">
-        <v>-0.009708194299310373</v>
+        <v>-0.05764679377913462</v>
       </c>
       <c r="E7">
-        <v>-0.05411581826598051</v>
+        <v>-0.004125766939543165</v>
       </c>
       <c r="F7">
-        <v>-0.5093286506710499</v>
+        <v>-1.886468028810635</v>
       </c>
       <c r="G7">
-        <v>-0.01396053627372621</v>
+        <v>-0.006335240316035612</v>
       </c>
       <c r="H7">
-        <v>85.41117144742898</v>
+        <v>171.4285740170393</v>
       </c>
       <c r="I7">
-        <v>86.01299583954764</v>
+        <v>171.4285673992215</v>
       </c>
       <c r="J7">
-        <v>101.7448627247406</v>
+        <v>26.65330585028306</v>
       </c>
       <c r="K7">
-        <v>94.09250860909573</v>
+        <v>108.0286805605204</v>
       </c>
       <c r="L7">
-        <v>-0.08464046098628504</v>
+        <v>0.01093248834956401</v>
       </c>
       <c r="M7">
-        <v>383.5780761218104</v>
+        <v>1.08666001613401</v>
       </c>
       <c r="N7">
-        <v>-8.96348007022494E-28</v>
+        <v>0.0001999860629717998</v>
       </c>
       <c r="O7">
-        <v>-252.1065821221995</v>
+        <v>306.8692648324996</v>
       </c>
       <c r="P7">
-        <v>67.67169328388906</v>
+        <v>205.3954407046986</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8">
-        <v>1.050354612257053</v>
+        <v>86.1260661012579</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>29.99999876022166</v>
+        <v>0.3683472034671609</v>
       </c>
       <c r="D8">
-        <v>-0.009076291498923411</v>
+        <v>0.07002561595617632</v>
       </c>
       <c r="E8">
-        <v>-0.07791734757747674</v>
+        <v>0.007068801122846744</v>
       </c>
       <c r="F8">
-        <v>-0.6622771227168154</v>
+        <v>-1.820963208326224</v>
       </c>
       <c r="G8">
-        <v>-0.02550188823884381</v>
+        <v>0.01935618492382619</v>
       </c>
       <c r="H8">
-        <v>85.2629277737649</v>
+        <v>-2.611226585013112E-06</v>
       </c>
       <c r="I8">
-        <v>85.37113961025112</v>
+        <v>124.2263322672908</v>
       </c>
       <c r="J8">
-        <v>92.37855644397554</v>
+        <v>50.78558340361215</v>
       </c>
       <c r="K8">
-        <v>94.22601207606471</v>
+        <v>124.1584662633507</v>
       </c>
       <c r="L8">
-        <v>-0.04841882778277753</v>
+        <v>-0.01363906414830139</v>
       </c>
       <c r="M8">
-        <v>391.8888313349107</v>
+        <v>0.0003635789449264077</v>
       </c>
       <c r="N8">
-        <v>1.445655997706762E-24</v>
+        <v>-4.773140342545753</v>
       </c>
       <c r="O8">
-        <v>-258.0479333907703</v>
+        <v>-314.6825223289686</v>
       </c>
       <c r="P8">
-        <v>64.76934810977976</v>
+        <v>-205.2401566963525</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9">
-        <v>1.225499757483865</v>
+        <v>102.5586452878137</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>29.98629861262248</v>
+        <v>0.2741733946274609</v>
       </c>
       <c r="D9">
-        <v>-0.00256449402259163</v>
+        <v>-0.0835073737620311</v>
       </c>
       <c r="E9">
-        <v>-0.0925764795562182</v>
+        <v>-0.003968759051152925</v>
       </c>
       <c r="F9">
-        <v>-0.8644275401994517</v>
+        <v>-1.840376654937489</v>
       </c>
       <c r="G9">
-        <v>-0.04050788773798109</v>
+        <v>-0.01221631890677186</v>
       </c>
       <c r="H9">
-        <v>85.52810541603233</v>
+        <v>171.4285740774316</v>
       </c>
       <c r="I9">
-        <v>86.20621549735269</v>
+        <v>100.9676512674029</v>
       </c>
       <c r="J9">
-        <v>90.05345733001154</v>
+        <v>32.14046123258811</v>
       </c>
       <c r="K9">
-        <v>94.89804494969685</v>
+        <v>99.10458882919917</v>
       </c>
       <c r="L9">
-        <v>0.04141014888834691</v>
+        <v>0.01028717453065245</v>
       </c>
       <c r="M9">
-        <v>435.6938360112447</v>
+        <v>0.8125498385202237</v>
       </c>
       <c r="N9">
-        <v>3.397690724693333E-28</v>
+        <v>0.0001999884421727933</v>
       </c>
       <c r="O9">
-        <v>-252.4305730012158</v>
+        <v>295.6488980037444</v>
       </c>
       <c r="P9">
-        <v>-2.55878366849068</v>
+        <v>207.3508081258908</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10">
-        <v>1.400688136228056</v>
+        <v>119.4372438025613</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>30.00000007969707</v>
+        <v>0.348446407457455</v>
       </c>
       <c r="D10">
-        <v>0.01670841275708275</v>
+        <v>0.09500605982315469</v>
       </c>
       <c r="E10">
-        <v>-0.07404306037784376</v>
+        <v>0.006550475281539251</v>
       </c>
       <c r="F10">
-        <v>-1.074194612272204</v>
+        <v>-1.811515325952283</v>
       </c>
       <c r="G10">
-        <v>-0.05513820570028236</v>
+        <v>0.01199838432866765</v>
       </c>
       <c r="H10">
-        <v>85.36326045051545</v>
+        <v>-2.648850144351273E-06</v>
       </c>
       <c r="I10">
-        <v>85.54569530579924</v>
+        <v>42.11953792437455</v>
       </c>
       <c r="J10">
-        <v>94.95612502138002</v>
+        <v>52.07720324443369</v>
       </c>
       <c r="K10">
-        <v>98.68606607510506</v>
+        <v>112.3939510164194</v>
       </c>
       <c r="L10">
-        <v>0.03499138696120417</v>
+        <v>-0.01276187022363004</v>
       </c>
       <c r="M10">
-        <v>419.8284899575024</v>
+        <v>0.0004657674008989858</v>
       </c>
       <c r="N10">
-        <v>-8.498488252749848E-28</v>
+        <v>-3.810925854385568</v>
       </c>
       <c r="O10">
-        <v>-260.2069833423311</v>
+        <v>-300.638014615855</v>
       </c>
       <c r="P10">
-        <v>31.20546562955481</v>
+        <v>-206.2067003091486</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11">
-        <v>1.575807398538395</v>
+        <v>137.2956881221491</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>29.99999935710484</v>
+        <v>0.2432973981317768</v>
       </c>
       <c r="D11">
-        <v>0.02474974397563092</v>
+        <v>-0.1077259475834896</v>
       </c>
       <c r="E11">
-        <v>-0.05839563646757716</v>
+        <v>-0.003178181679021966</v>
       </c>
       <c r="F11">
-        <v>-1.283714728661302</v>
+        <v>-1.862095585250477</v>
       </c>
       <c r="G11">
-        <v>-0.06671870525157461</v>
+        <v>-0.01763443214393483</v>
       </c>
       <c r="H11">
-        <v>85.6783545595397</v>
+        <v>171.428574089508</v>
       </c>
       <c r="I11">
-        <v>86.11039198869005</v>
+        <v>39.75443197357352</v>
       </c>
       <c r="J11">
-        <v>93.58315209973553</v>
+        <v>35.92085714001773</v>
       </c>
       <c r="K11">
-        <v>106.1526174173784</v>
+        <v>90.54014521880822</v>
       </c>
       <c r="L11">
-        <v>0.06612957526612506</v>
+        <v>0.01034660684897255</v>
       </c>
       <c r="M11">
-        <v>602.5223596407133</v>
+        <v>0.5867728999864386</v>
       </c>
       <c r="N11">
-        <v>-1.003094263682719E-26</v>
+        <v>0.0001999897121510085</v>
       </c>
       <c r="O11">
-        <v>-156.4814604077547</v>
+        <v>279.8518285477558</v>
       </c>
       <c r="P11">
-        <v>-35.85592561121008</v>
+        <v>200.403803047832</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12">
-        <v>1.751514699071341</v>
+        <v>155.6058664413082</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>29.78046720144491</v>
+        <v>0.3306704419765834</v>
       </c>
       <c r="D12">
-        <v>0.03963229130727886</v>
+        <v>0.1190956446651706</v>
       </c>
       <c r="E12">
-        <v>-0.03692606382483118</v>
+        <v>0.005652149574822848</v>
       </c>
       <c r="F12">
-        <v>-1.48682977130751</v>
+        <v>-1.860896014627843</v>
       </c>
       <c r="G12">
-        <v>-0.07494811591239135</v>
+        <v>0.006838408287800813</v>
       </c>
       <c r="H12">
-        <v>84.80847347443027</v>
+        <v>-2.644852230977505E-06</v>
       </c>
       <c r="I12">
-        <v>84.87367933722267</v>
+        <v>4.4939003124283E-06</v>
       </c>
       <c r="J12">
-        <v>144.1261167807237</v>
+        <v>49.58864315989902</v>
       </c>
       <c r="K12">
-        <v>155.2172238812166</v>
+        <v>100.9450379392323</v>
       </c>
       <c r="L12">
-        <v>0.1080290974616526</v>
+        <v>-0.01118138088745468</v>
       </c>
       <c r="M12">
-        <v>-4.02182987857733E-26</v>
+        <v>0.0007276294021526524</v>
       </c>
       <c r="N12">
-        <v>-0.0002382656986221379</v>
+        <v>-2.504703120999076</v>
       </c>
       <c r="O12">
-        <v>-212.6353441050444</v>
+        <v>-283.4349036461788</v>
       </c>
       <c r="P12">
-        <v>-2.115484282094079</v>
+        <v>-198.347993369127</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13">
-        <v>1.928533916696793</v>
+        <v>174.8705402406503</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>29.58636800451441</v>
+        <v>0.2181416187822255</v>
       </c>
       <c r="D13">
-        <v>0.05198737876893288</v>
+        <v>-0.1303072562652417</v>
       </c>
       <c r="E13">
-        <v>-0.009316364016207605</v>
+        <v>-0.002811659095833143</v>
       </c>
       <c r="F13">
-        <v>-1.646705559141833</v>
+        <v>-1.924758861120675</v>
       </c>
       <c r="G13">
-        <v>-0.079189460141976</v>
+        <v>-0.01919774733012335</v>
       </c>
       <c r="H13">
-        <v>84.36464466957358</v>
+        <v>171.4285740670998</v>
       </c>
       <c r="I13">
-        <v>84.50027406909025</v>
+        <v>32.89205036648492</v>
       </c>
       <c r="J13">
-        <v>92.39613089078176</v>
+        <v>37.32033605657825</v>
       </c>
       <c r="K13">
-        <v>105.9985875005506</v>
+        <v>84.21569039773586</v>
       </c>
       <c r="L13">
-        <v>0.125055788493705</v>
+        <v>0.01014406456756129</v>
       </c>
       <c r="M13">
-        <v>358.7102237865072</v>
+        <v>0.04884707979865765</v>
       </c>
       <c r="N13">
-        <v>1.763242668763301E-27</v>
+        <v>0.0001999898061446215</v>
       </c>
       <c r="O13">
-        <v>-198.1511343810747</v>
+        <v>265.7252839472441</v>
       </c>
       <c r="P13">
-        <v>-25.67060757642481</v>
+        <v>192.0209892855251</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14">
-        <v>2.106471973778904</v>
+        <v>194.5708491398933</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>29.44312662709868</v>
+        <v>0.3153452456384909</v>
       </c>
       <c r="D14">
-        <v>0.05392145412454036</v>
+        <v>0.1413529311354088</v>
       </c>
       <c r="E14">
-        <v>0.02951284708389866</v>
+        <v>0.005102029399164593</v>
       </c>
       <c r="F14">
-        <v>-1.780294036945668</v>
+        <v>-1.933491280951562</v>
       </c>
       <c r="G14">
-        <v>-0.07733963114756436</v>
+        <v>0.004849643679055799</v>
       </c>
       <c r="H14">
-        <v>83.93184197797147</v>
+        <v>-2.634802071011128E-06</v>
       </c>
       <c r="I14">
-        <v>83.72652645860553</v>
+        <v>3.259514865542934E-05</v>
       </c>
       <c r="J14">
-        <v>95.4105724811533</v>
+        <v>40.09997527399352</v>
       </c>
       <c r="K14">
-        <v>109.3552215878401</v>
+        <v>85.45314163150074</v>
       </c>
       <c r="L14">
-        <v>0.1399931318186446</v>
+        <v>-0.01028656772373162</v>
       </c>
       <c r="M14">
-        <v>332.4299846781488</v>
+        <v>0.0009849736797253276</v>
       </c>
       <c r="N14">
-        <v>1.742212466640867E-26</v>
+        <v>-1.733198907526684</v>
       </c>
       <c r="O14">
-        <v>-201.9918137635009</v>
+        <v>-266.8581442464447</v>
       </c>
       <c r="P14">
-        <v>-32.03204122763687</v>
+        <v>-188.6696935025203</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15">
-        <v>2.285254239181182</v>
+        <v>215.241035636062</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>29.3029106111724</v>
+        <v>0.2172318002830219</v>
       </c>
       <c r="D15">
-        <v>0.0506311188972042</v>
+        <v>-0.1517266841022214</v>
       </c>
       <c r="E15">
-        <v>0.06772207249900106</v>
+        <v>-0.001359309453988036</v>
       </c>
       <c r="F15">
-        <v>-1.88922668367108</v>
+        <v>-2.000000047124283</v>
       </c>
       <c r="G15">
-        <v>-0.06864072030209249</v>
+        <v>-0.01915642205621851</v>
       </c>
       <c r="H15">
-        <v>83.55584881772363</v>
+        <v>171.4285740656412</v>
       </c>
       <c r="I15">
-        <v>83.28289370661173</v>
+        <v>60.34250758024622</v>
       </c>
       <c r="J15">
-        <v>93.79356953687916</v>
+        <v>30.17447759289516</v>
       </c>
       <c r="K15">
-        <v>108.1983496077264</v>
+        <v>71.83643069055907</v>
       </c>
       <c r="L15">
-        <v>0.1423112275103812</v>
+        <v>0.01105248700126392</v>
       </c>
       <c r="M15">
-        <v>329.907777830612</v>
+        <v>0.00466052912367589</v>
       </c>
       <c r="N15">
-        <v>2.76763683728454E-27</v>
+        <v>0.0001999893984333511</v>
       </c>
       <c r="O15">
-        <v>-209.7973436063861</v>
+        <v>254.4952117319014</v>
       </c>
       <c r="P15">
-        <v>-35.79826427394634</v>
+        <v>185.1235313495935</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16">
-        <v>2.464797532383591</v>
+        <v>234.2600612864648</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>29.18972401618702</v>
+        <v>0.3355937445858249</v>
       </c>
       <c r="D16">
-        <v>0.04077829581824167</v>
+        <v>0.1635592339564484</v>
       </c>
       <c r="E16">
-        <v>0.1054925840237673</v>
+        <v>0.004025959163593364</v>
       </c>
       <c r="F16">
-        <v>-1.969198158422217</v>
+        <v>-2.000000049238839</v>
       </c>
       <c r="G16">
-        <v>-0.05308098356623071</v>
+        <v>0.007181053429153064</v>
       </c>
       <c r="H16">
-        <v>83.27617455107935</v>
+        <v>-2.63705673708372E-06</v>
       </c>
       <c r="I16">
-        <v>82.73570952619457</v>
+        <v>60.82563948865756</v>
       </c>
       <c r="J16">
-        <v>90.23952510250032</v>
+        <v>26.85014957610545</v>
       </c>
       <c r="K16">
-        <v>104.5485520835698</v>
+        <v>71.16344417470708</v>
       </c>
       <c r="L16">
-        <v>0.5734386587331688</v>
+        <v>0.0005381018871598624</v>
       </c>
       <c r="M16">
-        <v>412.5678104075254</v>
+        <v>0.002593121483481037</v>
       </c>
       <c r="N16">
-        <v>2.279472509395758E-27</v>
+        <v>-0.1334470676374061</v>
       </c>
       <c r="O16">
-        <v>-23.39852531058329</v>
+        <v>-258.8158308891711</v>
       </c>
       <c r="P16">
-        <v>-71.71965438736433</v>
+        <v>-184.8240808970149</v>
       </c>
     </row>
     <row r="17" spans="1:16">
       <c r="A17">
-        <v>2.646304900532903</v>
+        <v>253.5832688564677</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>28.64392812222416</v>
+        <v>0.2618695535562728</v>
       </c>
       <c r="D17">
-        <v>0.03254825729389917</v>
+        <v>-0.1622469234658728</v>
       </c>
       <c r="E17">
-        <v>0.1349440177524654</v>
+        <v>-0.002487856170210536</v>
       </c>
       <c r="F17">
-        <v>-1.999999810693658</v>
+        <v>-1.956241394345466</v>
       </c>
       <c r="G17">
-        <v>-0.03113979509410816</v>
+        <v>0.008770027441980318</v>
       </c>
       <c r="H17">
-        <v>65.71787633436971</v>
+        <v>171.428574344364</v>
       </c>
       <c r="I17">
-        <v>66.16579388110144</v>
+        <v>120.5437313802238</v>
       </c>
       <c r="J17">
-        <v>121.5395205622169</v>
+        <v>25.29774045053272</v>
       </c>
       <c r="K17">
-        <v>128.4402575183722</v>
+        <v>68.82992519743624</v>
       </c>
       <c r="L17">
-        <v>0.1321209100411237</v>
+        <v>0.008960281225997589</v>
       </c>
       <c r="M17">
-        <v>0.001939280818943257</v>
+        <v>0.00271460981676947</v>
       </c>
       <c r="N17">
-        <v>7.66398330006273E-25</v>
+        <v>0.0001999970018960722</v>
       </c>
       <c r="O17">
-        <v>-68.40302639663129</v>
+        <v>250.0632659773441</v>
       </c>
       <c r="P17">
-        <v>-57.67629934326195</v>
+        <v>181.6915601401241</v>
       </c>
     </row>
     <row r="18" spans="1:16">
       <c r="A18">
-        <v>2.830603326154852</v>
+        <v>269.1871442783465</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>28.34394403757355</v>
+        <v>0.4114353482725129</v>
       </c>
       <c r="D18">
-        <v>0.02286746195829881</v>
+        <v>0.1717321646737955</v>
       </c>
       <c r="E18">
-        <v>0.1716769414562861</v>
+        <v>0.004978138829117581</v>
       </c>
       <c r="F18">
-        <v>-1.941931444187555</v>
+        <v>-1.829222331675156</v>
       </c>
       <c r="G18">
-        <v>-0.003014252561297861</v>
+        <v>0.02992207522772276</v>
       </c>
       <c r="H18">
-        <v>94.09696873531539</v>
+        <v>-2.849877287823442E-06</v>
       </c>
       <c r="I18">
-        <v>91.87932625864471</v>
+        <v>-2.13884299098005E-06</v>
       </c>
       <c r="J18">
-        <v>79.99472038654166</v>
+        <v>26.73780922235307</v>
       </c>
       <c r="K18">
-        <v>79.80041194766807</v>
+        <v>69.20319530570514</v>
       </c>
       <c r="L18">
-        <v>0.121119769646981</v>
+        <v>0.00815364843837431</v>
       </c>
       <c r="M18">
-        <v>-3.279916929011744E-24</v>
+        <v>0.002636220285335493</v>
       </c>
       <c r="N18">
-        <v>-0.00294914023710311</v>
+        <v>0.000199991225148401</v>
       </c>
       <c r="O18">
-        <v>256.187546612053</v>
+        <v>-253.6365632449449</v>
       </c>
       <c r="P18">
-        <v>-100.8695702955812</v>
+        <v>-182.4214296008324</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19">
-        <v>3.018736632587401</v>
+        <v>284.8086591298096</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>27.52529179726817</v>
+        <v>0.3702912562479955</v>
       </c>
       <c r="D19">
-        <v>0.02043185750597484</v>
+        <v>-0.1618283944874649</v>
       </c>
       <c r="E19">
-        <v>0.2209513005327868</v>
+        <v>0.00169021460883954</v>
       </c>
       <c r="F19">
-        <v>-1.74833029082763</v>
+        <v>-1.595913021717977</v>
       </c>
       <c r="G19">
-        <v>0.03393054705061835</v>
+        <v>0.0498148844357296</v>
       </c>
       <c r="H19">
-        <v>67.32405371162919</v>
+        <v>171.4285743461716</v>
       </c>
       <c r="I19">
-        <v>67.77763150691243</v>
+        <v>88.78309554005817</v>
       </c>
       <c r="J19">
-        <v>78.52319294319351</v>
+        <v>26.11769188959753</v>
       </c>
       <c r="K19">
-        <v>79.54585574299591</v>
+        <v>68.20060876669073</v>
       </c>
       <c r="L19">
-        <v>0.1191978778303996</v>
+        <v>0.0117873395639554</v>
       </c>
       <c r="M19">
-        <v>503.9356604045615</v>
+        <v>0.004295489607545928</v>
       </c>
       <c r="N19">
-        <v>5.318210895122265E-28</v>
+        <v>0.0001999968699617555</v>
       </c>
       <c r="O19">
-        <v>-332.7536131185527</v>
+        <v>250.0615280100172</v>
       </c>
       <c r="P19">
-        <v>-103.0542606003206</v>
+        <v>182.4272166150001</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20">
-        <v>3.209489361479243</v>
+        <v>295.7725276897305</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>27.64652984520336</v>
+        <v>0.656522460249566</v>
       </c>
       <c r="D20">
-        <v>-0.008330811044512188</v>
+        <v>0.1734211685786633</v>
       </c>
       <c r="E20">
-        <v>0.2380682547519472</v>
+        <v>0.00669865785399826</v>
       </c>
       <c r="F20">
-        <v>-1.428809801732096</v>
+        <v>-1.226376666578598</v>
       </c>
       <c r="G20">
-        <v>0.07796339368739101</v>
+        <v>0.0781407524891182</v>
       </c>
       <c r="H20">
-        <v>87.52022694410493</v>
+        <v>-2.889993843088816E-06</v>
       </c>
       <c r="I20">
-        <v>83.43484896976381</v>
+        <v>-2.686520688912521E-06</v>
       </c>
       <c r="J20">
-        <v>102.2377175346772</v>
+        <v>15.72786600503182</v>
       </c>
       <c r="K20">
-        <v>85.58423591373686</v>
+        <v>65.78688326562006</v>
       </c>
       <c r="L20">
-        <v>0.09087146402773645</v>
+        <v>0.01492236708512812</v>
       </c>
       <c r="M20">
-        <v>4.129029810154228E-30</v>
+        <v>0.00605690987693816</v>
       </c>
       <c r="N20">
-        <v>-340.5057285290218</v>
+        <v>0.0001999853523934024</v>
       </c>
       <c r="O20">
-        <v>262.4399918949118</v>
+        <v>-254.7295076785167</v>
       </c>
       <c r="P20">
-        <v>-171.8350549962871</v>
+        <v>-183.9055357435065</v>
       </c>
     </row>
     <row r="21" spans="1:16">
       <c r="A21">
-        <v>3.40324726950419</v>
+        <v>305.4770220440475</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>26.75426692319439</v>
+        <v>0.4587012334363274</v>
       </c>
       <c r="D21">
-        <v>-0.01524613692329107</v>
+        <v>-0.1550155039255171</v>
       </c>
       <c r="E21">
-        <v>0.2760300333001882</v>
+        <v>0.003356509518256488</v>
       </c>
       <c r="F21">
-        <v>-0.9511877451839259</v>
+        <v>-0.6745565889967078</v>
       </c>
       <c r="G21">
-        <v>0.1279110609036712</v>
+        <v>0.1146179938937624</v>
       </c>
       <c r="H21">
-        <v>68.32492373140883</v>
+        <v>171.4285743590031</v>
       </c>
       <c r="I21">
-        <v>69.4524457427579</v>
+        <v>113.6141856175414</v>
       </c>
       <c r="J21">
-        <v>85.56676236461699</v>
+        <v>18.59209596466039</v>
       </c>
       <c r="K21">
-        <v>75.72387214062176</v>
+        <v>70.26780160428</v>
       </c>
       <c r="L21">
-        <v>0.106271284886993</v>
+        <v>0.01200226614513192</v>
       </c>
       <c r="M21">
-        <v>7.00789265528821E-05</v>
+        <v>0.01100641330067549</v>
       </c>
       <c r="N21">
-        <v>-1.17434611415472E-24</v>
+        <v>0.0001999966264942684</v>
       </c>
       <c r="O21">
-        <v>-106.3855923017031</v>
+        <v>253.419809273886</v>
       </c>
       <c r="P21">
-        <v>-207.2497389191921</v>
+        <v>184.6751269290639</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="A22">
-        <v>3.604119813775911</v>
+        <v>314.4846013004699</v>
       </c>
       <c r="B22">
         <v>0.003183098861837901</v>
       </c>
       <c r="C22">
-        <v>26.00634421883393</v>
+        <v>0.888680728703259</v>
       </c>
       <c r="D22">
-        <v>-0.028085495899735</v>
+        <v>0.1661144116921349</v>
       </c>
       <c r="E22">
-        <v>0.2764568842117314</v>
+        <v>0.01033063794965093</v>
       </c>
       <c r="F22">
-        <v>-0.2760139041835133</v>
+        <v>0.01230785083917473</v>
       </c>
       <c r="G22">
-        <v>0.1666787013563632</v>
+        <v>0.1271137204221079</v>
       </c>
       <c r="H22">
-        <v>81.43306235505052</v>
+        <v>-2.921930451875139E-06</v>
       </c>
       <c r="I22">
-        <v>77.1717678403068</v>
+        <v>-2.777202218570391E-06</v>
       </c>
       <c r="J22">
-        <v>72.85539721410859</v>
+        <v>4.596166679722756</v>
       </c>
       <c r="K22">
-        <v>75.59838168285037</v>
+        <v>67.19869455017742</v>
       </c>
       <c r="L22">
-        <v>0.07135646548253842</v>
+        <v>0.02188793713707414</v>
       </c>
       <c r="M22">
-        <v>-9.544694409049545E-30</v>
+        <v>0.02649208092763519</v>
       </c>
       <c r="N22">
-        <v>-1335.892709540615</v>
+        <v>0.0001999194820420282</v>
       </c>
       <c r="O22">
-        <v>327.0166767702015</v>
+        <v>-261.0023984752552</v>
       </c>
       <c r="P22">
-        <v>-169.2842546171157</v>
+        <v>-188.7108235847481</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="A23">
-        <v>3.813986636381685</v>
+        <v>321.4890358289551</v>
       </c>
       <c r="B23">
         <v>0.009708451528605597</v>
       </c>
       <c r="C23">
-        <v>24.45368675157986</v>
+        <v>0.6154758125602243</v>
       </c>
       <c r="D23">
-        <v>-0.03880062472196966</v>
+        <v>-0.138666585104283</v>
       </c>
       <c r="E23">
-        <v>0.3122155920487815</v>
+        <v>0.006388057961833128</v>
       </c>
       <c r="F23">
-        <v>0.46861965900346</v>
+        <v>0.7686169701497171</v>
       </c>
       <c r="G23">
-        <v>0.1775396088560895</v>
+        <v>0.1297141077183976</v>
       </c>
       <c r="H23">
-        <v>60.42025166434669</v>
+        <v>171.4285743805366</v>
       </c>
       <c r="I23">
-        <v>59.92394348416438</v>
+        <v>134.3447457761123</v>
       </c>
       <c r="J23">
-        <v>46.18691910975839</v>
+        <v>9.327762002679201</v>
       </c>
       <c r="K23">
-        <v>67.49396245266546</v>
+        <v>74.57505498767885</v>
       </c>
       <c r="L23">
-        <v>0.08093771193798818</v>
+        <v>0.01282677856362168</v>
       </c>
       <c r="M23">
-        <v>4.177142603132374E-05</v>
+        <v>1.684952743416839</v>
       </c>
       <c r="N23">
-        <v>-2.047357458758156E-25</v>
+        <v>0.0001999962208929666</v>
       </c>
       <c r="O23">
-        <v>-137.4727861493442</v>
+        <v>261.3313800531331</v>
       </c>
       <c r="P23">
-        <v>-223.9283384094417</v>
+        <v>189.966028143527</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24">
-        <v>4.031927964921906</v>
+        <v>328.2314819470565</v>
       </c>
       <c r="B24">
         <v>0.01639295913846519</v>
       </c>
       <c r="C24">
-        <v>23.54491119809519</v>
+        <v>1.033089376885512</v>
       </c>
       <c r="D24">
-        <v>-0.04880884224298262</v>
+        <v>0.149180665874344</v>
       </c>
       <c r="E24">
-        <v>0.306428747886173</v>
+        <v>0.01815686256805184</v>
       </c>
       <c r="F24">
-        <v>1.1270084947225</v>
+        <v>1.348164390776472</v>
       </c>
       <c r="G24">
-        <v>0.1594283793624685</v>
+        <v>0.07461102117586228</v>
       </c>
       <c r="H24">
-        <v>76.05838811512807</v>
+        <v>-2.951966116626071E-06</v>
       </c>
       <c r="I24">
-        <v>72.31711816135441</v>
+        <v>-1.871614698420237E-06</v>
       </c>
       <c r="J24">
-        <v>64.88454155099977</v>
+        <v>0.09678923606466314</v>
       </c>
       <c r="K24">
-        <v>69.35343767710854</v>
+        <v>81.1227813880764</v>
       </c>
       <c r="L24">
-        <v>0.06217117779341732</v>
+        <v>0.03291373387411867</v>
       </c>
       <c r="M24">
-        <v>-1.121288683062752E-28</v>
+        <v>0.03558776008919132</v>
       </c>
       <c r="N24">
-        <v>-339.9507502921666</v>
+        <v>0.0001989843292765865</v>
       </c>
       <c r="O24">
-        <v>275.3206488217727</v>
+        <v>-275.3045187253791</v>
       </c>
       <c r="P24">
-        <v>-193.6760403331835</v>
+        <v>-198.7228724399485</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c r="A25">
-        <v>4.254212962298838</v>
+        <v>333.7952521358886</v>
       </c>
       <c r="B25">
         <v>0.01986760647169749</v>
       </c>
       <c r="C25">
-        <v>22.59126197695183</v>
+        <v>0.79381099390087</v>
       </c>
       <c r="D25">
-        <v>-0.05467298210836744</v>
+        <v>-0.1081914460731947</v>
       </c>
       <c r="E25">
-        <v>0.3435125175454988</v>
+        <v>0.01253052892215573</v>
       </c>
       <c r="F25">
-        <v>1.594959641935798</v>
+        <v>1.757522423515591</v>
       </c>
       <c r="G25">
-        <v>0.1273950904415034</v>
+        <v>0.04854325114322183</v>
       </c>
       <c r="H25">
-        <v>56.388549796456</v>
+        <v>171.428574386137</v>
       </c>
       <c r="I25">
-        <v>56.63439290133422</v>
+        <v>171.4285714467678</v>
       </c>
       <c r="J25">
-        <v>60.96788944995595</v>
+        <v>1.301308841704538</v>
       </c>
       <c r="K25">
-        <v>64.51840229927424</v>
+        <v>82.91764999928708</v>
       </c>
       <c r="L25">
-        <v>0.07148982424466999</v>
+        <v>0.01765796195142317</v>
       </c>
       <c r="M25">
-        <v>4.124450162148068E-05</v>
+        <v>16.84390559239931</v>
       </c>
       <c r="N25">
-        <v>-4.964718211583831E-24</v>
+        <v>0.0001999956203532667</v>
       </c>
       <c r="O25">
-        <v>-144.333003941144</v>
+        <v>269.779755455377</v>
       </c>
       <c r="P25">
-        <v>-237.1809739169186</v>
+        <v>193.3878960471683</v>
       </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26">
-        <v>4.482652804149417</v>
+        <v>339.0810327987595</v>
       </c>
       <c r="B26">
         <v>0.02</v>
       </c>
       <c r="C26">
-        <v>21.85315022846399</v>
+        <v>1.118019419921428</v>
       </c>
       <c r="D26">
-        <v>-0.05990869498501382</v>
+        <v>0.1222204094400906</v>
       </c>
       <c r="E26">
-        <v>0.3261467804699089</v>
+        <v>0.05244359118300083</v>
       </c>
       <c r="F26">
-        <v>1.876354003335981</v>
+        <v>1.891270765280587</v>
       </c>
       <c r="G26">
-        <v>0.09894187404917255</v>
+        <v>-0.01422445674307088</v>
       </c>
       <c r="H26">
-        <v>70.34173864295875</v>
+        <v>-2.958332313885664E-06</v>
       </c>
       <c r="I26">
-        <v>66.02293561445649</v>
+        <v>103.428846709922</v>
       </c>
       <c r="J26">
-        <v>62.22500730921784</v>
+        <v>54.99045067199155</v>
       </c>
       <c r="K26">
-        <v>63.58001218990383</v>
+        <v>159.8264313210843</v>
       </c>
       <c r="L26">
-        <v>0.05567684862949855</v>
+        <v>0.04858570872906419</v>
       </c>
       <c r="M26">
-        <v>-2.669437567255827E-28</v>
+        <v>1.393607267550474E-05</v>
       </c>
       <c r="N26">
-        <v>-285.8759741480189</v>
+        <v>-50.59488761407561</v>
       </c>
       <c r="O26">
-        <v>258.0428116068421</v>
+        <v>-305.9030366082042</v>
       </c>
       <c r="P26">
-        <v>-204.0327083042688</v>
+        <v>-211.6377623197678</v>
       </c>
     </row>
     <row r="27" spans="1:16">
       <c r="A27">
-        <v>4.718413167775238</v>
+        <v>343.6838936747593</v>
       </c>
       <c r="B27">
         <v>0.02</v>
       </c>
       <c r="C27">
-        <v>20.9587226103786</v>
+        <v>1.058329766453057</v>
       </c>
       <c r="D27">
-        <v>-0.06397206409210804</v>
+        <v>-0.05690972704156464</v>
       </c>
       <c r="E27">
-        <v>0.3616505122086126</v>
+        <v>0.01802489696765177</v>
       </c>
       <c r="F27">
-        <v>1.999999890945066</v>
+        <v>2.000000049198159</v>
       </c>
       <c r="G27">
-        <v>0.07501339881310645</v>
+        <v>0.0003179395310395035</v>
       </c>
       <c r="H27">
-        <v>52.74375469392419</v>
+        <v>171.428574392333</v>
       </c>
       <c r="I27">
-        <v>53.36088471995214</v>
+        <v>-1.130636519702664E-06</v>
       </c>
       <c r="J27">
-        <v>57.17252085368987</v>
+        <v>0.02520905350446062</v>
       </c>
       <c r="K27">
-        <v>60.13441786971049</v>
+        <v>87.79389609971304</v>
       </c>
       <c r="L27">
-        <v>0.06298101072657836</v>
+        <v>0.02259688567885212</v>
       </c>
       <c r="M27">
-        <v>1.568764306202474E-25</v>
+        <v>15.75325024294949</v>
       </c>
       <c r="N27">
-        <v>-5.367531465370823E-05</v>
+        <v>0.0001999951357830614</v>
       </c>
       <c r="O27">
-        <v>-138.9509047335262</v>
+        <v>298.1243837404094</v>
       </c>
       <c r="P27">
-        <v>-240.9259860860476</v>
+        <v>203.8595111834251</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28">
-        <v>4.963023535182331</v>
+        <v>347.9048297120319</v>
       </c>
       <c r="B28">
         <v>0.02</v>
       </c>
       <c r="C28">
-        <v>20.25710807129565</v>
+        <v>1.327017432663145</v>
       </c>
       <c r="D28">
-        <v>-0.06617149478998177</v>
+        <v>0.07589798474770515</v>
       </c>
       <c r="E28">
-        <v>0.3421130304013377</v>
+        <v>0.04002605094503976</v>
       </c>
       <c r="F28">
-        <v>1.999999498710614</v>
+        <v>1.933563927507374</v>
       </c>
       <c r="G28">
-        <v>0.05611899938720128</v>
+        <v>-0.05057406156855061</v>
       </c>
       <c r="H28">
-        <v>65.15825179911336</v>
+        <v>-2.961310528341408E-06</v>
       </c>
       <c r="I28">
-        <v>60.6424258199774</v>
+        <v>-2.175712204485554E-06</v>
       </c>
       <c r="J28">
-        <v>57.4461050429945</v>
+        <v>32.48018507158981</v>
       </c>
       <c r="K28">
-        <v>58.92615039693928</v>
+        <v>146.1378839056372</v>
       </c>
       <c r="L28">
-        <v>0.05132264680241373</v>
+        <v>0.03368323206949987</v>
       </c>
       <c r="M28">
-        <v>2.830983595433104E-28</v>
+        <v>3.47787717596384E-05</v>
       </c>
       <c r="N28">
-        <v>-28.62000192897993</v>
+        <v>-29.28021047089428</v>
       </c>
       <c r="O28">
-        <v>224.1530884898876</v>
+        <v>-301.3860848256655</v>
       </c>
       <c r="P28">
-        <v>-215.3147127432239</v>
+        <v>-184.6913196339694</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c r="A29">
-        <v>5.216391358850169</v>
+        <v>351.7838196390722</v>
       </c>
       <c r="B29">
         <v>0.02</v>
       </c>
       <c r="C29">
-        <v>19.56986153668406</v>
+        <v>1.276641886751603</v>
       </c>
       <c r="D29">
-        <v>-0.0666321352467568</v>
+        <v>-0.03026005628584125</v>
       </c>
       <c r="E29">
-        <v>0.3755668045678391</v>
+        <v>0.01883992507947921</v>
       </c>
       <c r="F29">
-        <v>1.909801751400547</v>
+        <v>1.723839738318365</v>
       </c>
       <c r="G29">
-        <v>0.04204554436509146</v>
+        <v>0.05968003560393236</v>
       </c>
       <c r="H29">
-        <v>50.04380040419706</v>
+        <v>171.4285743897674</v>
       </c>
       <c r="I29">
-        <v>51.01071316721705</v>
+        <v>-2.594230685574422E-06</v>
       </c>
       <c r="J29">
-        <v>55.19162123256464</v>
+        <v>0.1943252489873309</v>
       </c>
       <c r="K29">
-        <v>56.66425996408394</v>
+        <v>103.850073730754</v>
       </c>
       <c r="L29">
-        <v>0.06332210453117473</v>
+        <v>0.02427553839522184</v>
       </c>
       <c r="M29">
-        <v>1.59989329059248E-26</v>
+        <v>15.63296892205036</v>
       </c>
       <c r="N29">
-        <v>2.426879561172013E-07</v>
+        <v>0.0001999934466598271</v>
       </c>
       <c r="O29">
-        <v>-118.7746998057287</v>
+        <v>282.0032639314232</v>
       </c>
       <c r="P29">
-        <v>-244.3834921872013</v>
+        <v>176.0627292231166</v>
       </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30">
-        <v>5.479401382938831</v>
+        <v>355.4215195172922</v>
       </c>
       <c r="B30">
         <v>0.02</v>
       </c>
       <c r="C30">
-        <v>18.90566457868778</v>
+        <v>1.502300650304962</v>
       </c>
       <c r="D30">
-        <v>-0.0656040060246442</v>
+        <v>0.05225687843390924</v>
       </c>
       <c r="E30">
-        <v>0.3568248022896389</v>
+        <v>0.03652927614555809</v>
       </c>
       <c r="F30">
-        <v>1.763105826308185</v>
+        <v>1.971801869695252</v>
       </c>
       <c r="G30">
-        <v>0.03335066998658347</v>
+        <v>0.01245174436666112</v>
       </c>
       <c r="H30">
-        <v>60.35793359666894</v>
+        <v>-2.953260079981019E-06</v>
       </c>
       <c r="I30">
-        <v>55.66827258623834</v>
+        <v>-2.476691795817937E-06</v>
       </c>
       <c r="J30">
-        <v>53.10798433878568</v>
+        <v>31.16980258046534</v>
       </c>
       <c r="K30">
-        <v>54.87485800965162</v>
+        <v>151.9245538799877</v>
       </c>
       <c r="L30">
-        <v>0.0522304813512872</v>
+        <v>0.02427849587366249</v>
       </c>
       <c r="M30">
-        <v>91.41256820290248</v>
+        <v>3.963478217760007E-05</v>
       </c>
       <c r="N30">
-        <v>2.236481725476671E-24</v>
+        <v>-26.95479607823283</v>
       </c>
       <c r="O30">
-        <v>127.3548453895466</v>
+        <v>-255.7835745633932</v>
       </c>
       <c r="P30">
-        <v>-217.4153173629903</v>
+        <v>-142.2748380888008</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31">
-        <v>5.750999871292233</v>
+        <v>358.8171772747159</v>
       </c>
       <c r="B31">
         <v>0.02</v>
       </c>
       <c r="C31">
-        <v>18.49700693031129</v>
+        <v>1.461633913731184</v>
       </c>
       <c r="D31">
-        <v>-0.06329929296912493</v>
+        <v>-0.01856597247728323</v>
       </c>
       <c r="E31">
-        <v>0.3800973215982708</v>
+        <v>0.01701379535939716</v>
       </c>
       <c r="F31">
-        <v>1.591762018829999</v>
+        <v>2.000000049641876</v>
       </c>
       <c r="G31">
-        <v>0.02841764661952779</v>
+        <v>-0.03144914128015154</v>
       </c>
       <c r="H31">
-        <v>48.01169906866211</v>
+        <v>171.4285743718356</v>
       </c>
       <c r="I31">
-        <v>49.07286240900848</v>
+        <v>57.46679067473682</v>
       </c>
       <c r="J31">
-        <v>58.09786346314313</v>
+        <v>0.1542633083456333</v>
       </c>
       <c r="K31">
-        <v>54.94336917923483</v>
+        <v>112.6619578987169</v>
       </c>
       <c r="L31">
-        <v>0.06939279321942551</v>
+        <v>0.02348097546284098</v>
       </c>
       <c r="M31">
-        <v>-5.957587782203527E-29</v>
+        <v>7.158342810607756</v>
       </c>
       <c r="N31">
-        <v>1.677535141814168E-05</v>
+        <v>0.0001999902651772596</v>
       </c>
       <c r="O31">
-        <v>-66.04634201202123</v>
+        <v>244.6562394080815</v>
       </c>
       <c r="P31">
-        <v>-244.3730092245467</v>
+        <v>139.2720250617973</v>
       </c>
     </row>
     <row r="32" spans="1:16">
       <c r="A32">
-        <v>6.030808714007093</v>
+        <v>362.0551415401488</v>
       </c>
       <c r="B32">
         <v>0.02</v>
       </c>
       <c r="C32">
-        <v>17.90056985576439</v>
+        <v>1.659464663848217</v>
       </c>
       <c r="D32">
-        <v>-0.05867408132330796</v>
+        <v>0.04092789256184379</v>
       </c>
       <c r="E32">
-        <v>0.3682562603721562</v>
+        <v>0.02832343158355989</v>
       </c>
       <c r="F32">
-        <v>1.42129742159429</v>
+        <v>1.776863818126263</v>
       </c>
       <c r="G32">
-        <v>0.02802251492798536</v>
+        <v>-0.08149317204961917</v>
       </c>
       <c r="H32">
-        <v>56.69189764168556</v>
+        <v>-2.938688058958549E-06</v>
       </c>
       <c r="I32">
-        <v>52.00463748034964</v>
+        <v>14.45191930055176</v>
       </c>
       <c r="J32">
-        <v>49.12241722812717</v>
+        <v>8.307570489194399</v>
       </c>
       <c r="K32">
-        <v>51.33806932408342</v>
+        <v>129.2083313462189</v>
       </c>
       <c r="L32">
-        <v>0.06197848919785732</v>
+        <v>0.02181167886918744</v>
       </c>
       <c r="M32">
-        <v>68.92316978135646</v>
+        <v>7.977459785151058</v>
       </c>
       <c r="N32">
-        <v>3.11855260816492E-25</v>
+        <v>0.000199864075601082</v>
       </c>
       <c r="O32">
-        <v>121.056377388412</v>
+        <v>-213.9240847723869</v>
       </c>
       <c r="P32">
-        <v>-222.0389915312417</v>
+        <v>-113.7610134748317</v>
       </c>
     </row>
     <row r="33" spans="1:16">
       <c r="A33">
-        <v>6.320028452627537</v>
+        <v>365.1638489836643</v>
       </c>
       <c r="B33">
         <v>0.02</v>
       </c>
       <c r="C33">
-        <v>17.45987373387959</v>
+        <v>1.625582917253973</v>
       </c>
       <c r="D33">
-        <v>-0.05271370901780061</v>
+        <v>-0.01273038082837005</v>
       </c>
       <c r="E33">
-        <v>0.3905904597524811</v>
+        <v>0.01472717558567554</v>
       </c>
       <c r="F33">
-        <v>1.290376152413829</v>
+        <v>1.297372152897303</v>
       </c>
       <c r="G33">
-        <v>0.03280378142384666</v>
+        <v>-0.1323918098790651</v>
       </c>
       <c r="H33">
-        <v>45.86854625080127</v>
+        <v>171.4285742934214</v>
       </c>
       <c r="I33">
-        <v>46.80838075915286</v>
+        <v>171.4285741221187</v>
       </c>
       <c r="J33">
-        <v>51.8006688142414</v>
+        <v>17.68033896057787</v>
       </c>
       <c r="K33">
-        <v>51.9675529646732</v>
+        <v>134.2326690355763</v>
       </c>
       <c r="L33">
-        <v>0.07501908524007181</v>
+        <v>0.02152180303315001</v>
       </c>
       <c r="M33">
-        <v>261.7167072585108</v>
+        <v>1.581620754370884</v>
       </c>
       <c r="N33">
-        <v>-9.598535298243677E-31</v>
+        <v>0.0001999847464276984</v>
       </c>
       <c r="O33">
-        <v>-247.3352899442067</v>
+        <v>203.4016984827308</v>
       </c>
       <c r="P33">
-        <v>-221.0784672431397</v>
+        <v>109.2483861128341</v>
       </c>
     </row>
     <row r="34" spans="1:16">
       <c r="A34">
-        <v>6.611466678105559</v>
+        <v>368.2045912450644</v>
       </c>
       <c r="B34">
         <v>0.02</v>
       </c>
       <c r="C34">
-        <v>17.68452854028479</v>
+        <v>1.801506079998902</v>
       </c>
       <c r="D34">
-        <v>-0.05277535762174398</v>
+        <v>0.03374411492090467</v>
       </c>
       <c r="E34">
-        <v>0.3598096460151987</v>
+        <v>0.02189995110211204</v>
       </c>
       <c r="F34">
-        <v>1.203009380508814</v>
+        <v>0.5274608441792159</v>
       </c>
       <c r="G34">
-        <v>0.03704144584465612</v>
+        <v>-0.1862692065447703</v>
       </c>
       <c r="H34">
-        <v>55.3170429663875</v>
+        <v>-2.883323264055616E-06</v>
       </c>
       <c r="I34">
-        <v>50.67718014078041</v>
+        <v>87.72442731358301</v>
       </c>
       <c r="J34">
-        <v>56.83232653198873</v>
+        <v>14.39861538125679</v>
       </c>
       <c r="K34">
-        <v>53.18848044892403</v>
+        <v>134.7382593024339</v>
       </c>
       <c r="L34">
-        <v>0.06866613363868762</v>
+        <v>0.02058822699095207</v>
       </c>
       <c r="M34">
-        <v>43.3831044343839</v>
+        <v>0.3208649184350714</v>
       </c>
       <c r="N34">
-        <v>-1.651680962403308E-26</v>
+        <v>0.000199945536750804</v>
       </c>
       <c r="O34">
-        <v>171.3099134863379</v>
+        <v>-183.8144761536342</v>
       </c>
       <c r="P34">
-        <v>-225.9957916261661</v>
+        <v>-95.39638960489245</v>
       </c>
     </row>
     <row r="35" spans="1:16">
       <c r="A35">
-        <v>6.905138940281997</v>
+        <v>371.1984544463602</v>
       </c>
       <c r="B35">
         <v>0.02</v>
       </c>
       <c r="C35">
-        <v>17.23401778798979</v>
+        <v>1.777658155516802</v>
       </c>
       <c r="D35">
-        <v>-0.04580828679797188</v>
+        <v>-0.008665054664186964</v>
       </c>
       <c r="E35">
-        <v>0.3915808318291374</v>
+        <v>0.01652353012017592</v>
       </c>
       <c r="F35">
-        <v>1.151114730230537</v>
+        <v>-0.5440211802652701</v>
       </c>
       <c r="G35">
-        <v>0.04242575900457433</v>
+        <v>-0.2394817762118191</v>
       </c>
       <c r="H35">
-        <v>45.92504654053485</v>
+        <v>48.32547105896449</v>
       </c>
       <c r="I35">
-        <v>46.83243496698204</v>
+        <v>171.4285742023826</v>
       </c>
       <c r="J35">
-        <v>51.47095802622008</v>
+        <v>8.283212327689206</v>
       </c>
       <c r="K35">
-        <v>49.92742206220482</v>
+        <v>126.6720054807343</v>
       </c>
       <c r="L35">
-        <v>0.08329081763892782</v>
+        <v>0.01513165157237306</v>
       </c>
       <c r="M35">
-        <v>280.1664486362501</v>
+        <v>20.07256326739708</v>
       </c>
       <c r="N35">
-        <v>2.567646184633904E-29</v>
+        <v>0.0001999765356002858</v>
       </c>
       <c r="O35">
-        <v>-265.7739080861951</v>
+        <v>31.47237693223547</v>
       </c>
       <c r="P35">
-        <v>-213.8737271608356</v>
+        <v>25.68974933550225</v>
       </c>
     </row>
     <row r="36" spans="1:16">
       <c r="A36">
-        <v>7.200296208691094</v>
+        <v>374.2239507181678</v>
       </c>
       <c r="B36">
         <v>0.02</v>
       </c>
       <c r="C36">
-        <v>17.53188097188578</v>
+        <v>1.902121033193476</v>
       </c>
       <c r="D36">
-        <v>-0.04720362886079962</v>
+        <v>0.02299553303131527</v>
       </c>
       <c r="E36">
-        <v>0.3589701590505832</v>
+        <v>0.4772008638492212</v>
       </c>
       <c r="F36">
-        <v>1.149069956547078</v>
+        <v>-2.000000049768825</v>
       </c>
       <c r="G36">
-        <v>0.04804723048819105</v>
+        <v>-0.3048187110169432</v>
       </c>
       <c r="H36">
-        <v>54.22641023152722</v>
+        <v>-2.902631722834846E-06</v>
       </c>
       <c r="I36">
-        <v>49.72164211795151</v>
+        <v>171.4285740033698</v>
       </c>
       <c r="J36">
-        <v>56.59770943834998</v>
+        <v>51.7215908871168</v>
       </c>
       <c r="K36">
-        <v>53.5163566059118</v>
+        <v>171.4285706970392</v>
       </c>
       <c r="L36">
-        <v>0.07150070286149632</v>
+        <v>0.118695261913302</v>
       </c>
       <c r="M36">
-        <v>59.16893691467783</v>
+        <v>264.7336158699712</v>
       </c>
       <c r="N36">
-        <v>-1.453888720114538E-25</v>
+        <v>-491.7553598311159</v>
       </c>
       <c r="O36">
-        <v>154.8998612278962</v>
+        <v>-221.0228088134109</v>
       </c>
       <c r="P36">
-        <v>-227.1009672237715</v>
+        <v>-128.2331304978224</v>
       </c>
     </row>
     <row r="37" spans="1:16">
       <c r="A37">
-        <v>7.496085728932864</v>
+        <v>376.0546544168142</v>
       </c>
       <c r="B37">
         <v>0.02</v>
       </c>
       <c r="C37">
-        <v>17.1431139479808</v>
+        <v>3.977888568276782</v>
       </c>
       <c r="D37">
-        <v>-0.04082649287382356</v>
+        <v>0.03834973784790086</v>
       </c>
       <c r="E37">
-        <v>0.3900412960272182</v>
+        <v>0.2148393726893207</v>
       </c>
       <c r="F37">
-        <v>1.182521595426026</v>
+        <v>-1.805915678483411</v>
       </c>
       <c r="G37">
-        <v>0.05388224042737847</v>
+        <v>0.1209905938377209</v>
       </c>
       <c r="H37">
-        <v>46.31727679658388</v>
+        <v>171.42857426433</v>
       </c>
       <c r="I37">
-        <v>47.09303475600134</v>
+        <v>-2.834215377080956E-06</v>
       </c>
       <c r="J37">
-        <v>52.73515869816585</v>
+        <v>152.0069759107495</v>
       </c>
       <c r="K37">
-        <v>49.45763745343412</v>
+        <v>171.4285515947262</v>
       </c>
       <c r="L37">
-        <v>0.1830028358104935</v>
+        <v>0.04143753457643821</v>
       </c>
       <c r="M37">
-        <v>238.5727406092965</v>
+        <v>34.47948396533056</v>
       </c>
       <c r="N37">
-        <v>-3.786883064217709E-29</v>
+        <v>-388.8832265075421</v>
       </c>
       <c r="O37">
-        <v>-191.6909737606789</v>
+        <v>-118.7594280774801</v>
       </c>
       <c r="P37">
-        <v>-220.1070107144204</v>
+        <v>-60.50391698307328</v>
       </c>
     </row>
     <row r="38" spans="1:16">
       <c r="A38">
-        <v>7.793938959118723</v>
+        <v>377.2989801105899</v>
       </c>
       <c r="B38">
         <v>0.02</v>
       </c>
       <c r="C38">
-        <v>17.2569442584117</v>
+        <v>4.754166510182819</v>
       </c>
       <c r="D38">
-        <v>-0.04450722972638575</v>
+        <v>0.01105672481320672</v>
       </c>
       <c r="E38">
-        <v>0.3647261767296222</v>
+        <v>0.1025970988266143</v>
       </c>
       <c r="F38">
-        <v>1.260403551929532</v>
+        <v>-0.7760956436413973</v>
       </c>
       <c r="G38">
-        <v>0.06122746719624157</v>
+        <v>0.1872238157825133</v>
       </c>
       <c r="H38">
-        <v>51.3643419549745</v>
+        <v>171.428574368873</v>
       </c>
       <c r="I38">
-        <v>47.30676760082309</v>
+        <v>-2.919701165139602E-06</v>
       </c>
       <c r="J38">
-        <v>54.88863585206523</v>
+        <v>1.039546254646192</v>
       </c>
       <c r="K38">
-        <v>52.54830344708554</v>
+        <v>2.081270048997986E-07</v>
       </c>
       <c r="L38">
-        <v>0.06497434698849419</v>
+        <v>0.0295173129475529</v>
       </c>
       <c r="M38">
-        <v>141.005231303369</v>
+        <v>221.5369485367968</v>
       </c>
       <c r="N38">
-        <v>4.115314585031116E-25</v>
+        <v>0.0001998753840946112</v>
       </c>
       <c r="O38">
-        <v>-3.721436148868396</v>
+        <v>-22.52059033976505</v>
       </c>
       <c r="P38">
-        <v>-232.7946857549203</v>
+        <v>-11.06638168497132</v>
       </c>
     </row>
     <row r="39" spans="1:16">
       <c r="A39">
-        <v>8.091122931133524</v>
+        <v>378.3702587848759</v>
       </c>
       <c r="B39">
         <v>0.02</v>
       </c>
       <c r="C39">
-        <v>17.15579617263688</v>
+        <v>5.254159172433778</v>
       </c>
       <c r="D39">
-        <v>-0.04030892298840084</v>
+        <v>0.01395247005557099</v>
       </c>
       <c r="E39">
-        <v>0.3724066999441362</v>
+        <v>0.0757927419418279</v>
       </c>
       <c r="F39">
-        <v>1.368312054915998</v>
+        <v>0.2732431060815674</v>
       </c>
       <c r="G39">
-        <v>0.06578103394254267</v>
+        <v>0.1730869302551418</v>
       </c>
       <c r="H39">
-        <v>48.38540008525107</v>
+        <v>171.4285737283847</v>
       </c>
       <c r="I39">
-        <v>48.7111656481016</v>
+        <v>76.52673769605225</v>
       </c>
       <c r="J39">
-        <v>54.2810219180784</v>
+        <v>166.0554239689108</v>
       </c>
       <c r="K39">
-        <v>50.12603376177968</v>
+        <v>164.4678350515972</v>
       </c>
       <c r="L39">
-        <v>0.08554277063520478</v>
+        <v>0.02147626711792422</v>
       </c>
       <c r="M39">
-        <v>231.1489103499916</v>
+        <v>25.88335224619073</v>
       </c>
       <c r="N39">
-        <v>4.228808392912525E-30</v>
+        <v>0.0001998994722095968</v>
       </c>
       <c r="O39">
-        <v>-187.4406879674974</v>
+        <v>-43.17984304639459</v>
       </c>
       <c r="P39">
-        <v>-224.8106749389978</v>
+        <v>-21.26991846151348</v>
       </c>
     </row>
     <row r="40" spans="1:16">
       <c r="A40">
-        <v>8.386889961011637</v>
+        <v>379.3429533001744</v>
       </c>
       <c r="B40">
         <v>0.02</v>
       </c>
       <c r="C40">
-        <v>17.33977792713401</v>
+        <v>5.526152435038922</v>
       </c>
       <c r="D40">
-        <v>-0.03835916300840144</v>
+        <v>0.007568644962309433</v>
       </c>
       <c r="E40">
-        <v>0.3530006922999765</v>
+        <v>0.05903805790634745</v>
       </c>
       <c r="F40">
-        <v>1.510366809876015</v>
+        <v>1.127986440594383</v>
       </c>
       <c r="G40">
-        <v>0.06803105745413768</v>
+        <v>0.1314970836254192</v>
       </c>
       <c r="H40">
-        <v>51.24712558420509</v>
+        <v>171.4285736709441</v>
       </c>
       <c r="I40">
-        <v>47.66051586194631</v>
+        <v>110.7119989847646</v>
       </c>
       <c r="J40">
-        <v>54.21574631735587</v>
+        <v>155.848686232725</v>
       </c>
       <c r="K40">
-        <v>52.25928490430933</v>
+        <v>152.4974943205549</v>
       </c>
       <c r="L40">
-        <v>0.05894958667273837</v>
+        <v>0.01538534438478167</v>
       </c>
       <c r="M40">
-        <v>178.9547673504247</v>
+        <v>38.13335607332485</v>
       </c>
       <c r="N40">
-        <v>-1.26899371976994E-30</v>
+        <v>0.0001999128852347269</v>
       </c>
       <c r="O40">
-        <v>-58.39929240621525</v>
+        <v>-25.57193255483217</v>
       </c>
       <c r="P40">
-        <v>-222.4604197367706</v>
+        <v>-12.34065099612679</v>
       </c>
     </row>
     <row r="41" spans="1:16">
       <c r="A41">
-        <v>8.679912998813574</v>
+        <v>380.2547684225888</v>
       </c>
       <c r="B41">
         <v>0.02</v>
       </c>
       <c r="C41">
-        <v>17.37181633112408</v>
+        <v>5.717419241253554</v>
       </c>
       <c r="D41">
-        <v>-0.03565586879593829</v>
+        <v>0.006059370227518984</v>
       </c>
       <c r="E41">
-        <v>0.3532485738191174</v>
+        <v>0.06024880258579402</v>
       </c>
       <c r="F41">
-        <v>1.665432468019806</v>
+        <v>1.690711245448674</v>
       </c>
       <c r="G41">
-        <v>0.06649472865838951</v>
+        <v>0.07275638098365574</v>
       </c>
       <c r="H41">
-        <v>49.35596465950109</v>
+        <v>171.428573926316</v>
       </c>
       <c r="I41">
-        <v>49.37339572028718</v>
+        <v>128.5495886312783</v>
       </c>
       <c r="J41">
-        <v>54.98363176134757</v>
+        <v>160.7097053986691</v>
       </c>
       <c r="K41">
-        <v>51.2147836187531</v>
+        <v>156.5968356754166</v>
       </c>
       <c r="L41">
-        <v>0.07010805522273364</v>
+        <v>0.02032316487778606</v>
       </c>
       <c r="M41">
-        <v>232.8721175334108</v>
+        <v>27.16577487064418</v>
       </c>
       <c r="N41">
-        <v>8.75580444618351E-30</v>
+        <v>0.0001999285238911662</v>
       </c>
       <c r="O41">
-        <v>-175.3403837717839</v>
+        <v>-18.5132944883605</v>
       </c>
       <c r="P41">
-        <v>-218.5827306315371</v>
+        <v>-8.611321593481827</v>
       </c>
     </row>
     <row r="42" spans="1:16">
       <c r="A42">
-        <v>8.970032173345627</v>
+        <v>381.1193026107814</v>
       </c>
       <c r="B42">
         <v>0.02</v>
       </c>
       <c r="C42">
-        <v>17.57525092731254</v>
+        <v>5.981907658553395</v>
       </c>
       <c r="D42">
-        <v>-0.03373530975851145</v>
+        <v>0.009478465703786841</v>
       </c>
       <c r="E42">
-        <v>0.3380644137788796</v>
+        <v>0.1001419930353323</v>
       </c>
       <c r="F42">
-        <v>1.816043997584537</v>
+        <v>1.965344683833926</v>
       </c>
       <c r="G42">
-        <v>0.06176038018371807</v>
+        <v>0.01775191993219125</v>
       </c>
       <c r="H42">
-        <v>51.69476284908245</v>
+        <v>16.56482213723607</v>
       </c>
       <c r="I42">
-        <v>48.51230848719851</v>
+        <v>-2.674605207773841E-06</v>
       </c>
       <c r="J42">
-        <v>54.78041270453804</v>
+        <v>162.5804756510469</v>
       </c>
       <c r="K42">
-        <v>52.62006601679167</v>
+        <v>158.1948540565109</v>
       </c>
       <c r="L42">
-        <v>0.0460562270289034</v>
+        <v>0.01675487733444195</v>
       </c>
       <c r="M42">
-        <v>204.9067526621295</v>
+        <v>73.28694592025991</v>
       </c>
       <c r="N42">
-        <v>1.042014786473643E-30</v>
+        <v>0.0001998846137043633</v>
       </c>
       <c r="O42">
-        <v>-96.28246823869799</v>
+        <v>-45.04224645676251</v>
       </c>
       <c r="P42">
-        <v>-210.0498392475159</v>
+        <v>-22.08878878410075</v>
       </c>
     </row>
     <row r="43" spans="1:16">
       <c r="A43">
-        <v>9.256564707387838</v>
+        <v>381.9370155204589</v>
       </c>
       <c r="B43">
         <v>0.02</v>
       </c>
       <c r="C43">
-        <v>17.70055364537248</v>
+        <v>6.330431678887159</v>
       </c>
       <c r="D43">
-        <v>-0.03405187191906311</v>
+        <v>0.0051170627011792</v>
       </c>
       <c r="E43">
-        <v>0.3315416378786687</v>
+        <v>0.08779113903198772</v>
       </c>
       <c r="F43">
-        <v>1.934703061322355</v>
+        <v>2.000000049471945</v>
       </c>
       <c r="G43">
-        <v>0.05268192102089887</v>
+        <v>-0.02143753089946938</v>
       </c>
       <c r="H43">
-        <v>50.52265550655499</v>
+        <v>171.4285735604942</v>
       </c>
       <c r="I43">
-        <v>50.33060267106741</v>
+        <v>171.4285738647595</v>
       </c>
       <c r="J43">
-        <v>55.57729762065753</v>
+        <v>164.4092968314938</v>
       </c>
       <c r="K43">
-        <v>52.44158949040104</v>
+        <v>157.1127758461759</v>
       </c>
       <c r="L43">
-        <v>0.05012939732648833</v>
+        <v>0.02348423847781038</v>
       </c>
       <c r="M43">
-        <v>239.2709021790526</v>
+        <v>55.87574092098637</v>
       </c>
       <c r="N43">
-        <v>1.107546326902022E-26</v>
+        <v>0.0001999182603059054</v>
       </c>
       <c r="O43">
-        <v>-171.7392613533504</v>
+        <v>0.7154276828146691</v>
       </c>
       <c r="P43">
-        <v>-208.1299181206844</v>
+        <v>-1.676288888033395</v>
       </c>
     </row>
     <row r="44" spans="1:16">
       <c r="A44">
-        <v>9.539675302571187</v>
+        <v>382.7073812169757</v>
       </c>
       <c r="B44">
         <v>0.02</v>
       </c>
       <c r="C44">
-        <v>17.92702921776986</v>
+        <v>6.752369202727333</v>
       </c>
       <c r="D44">
-        <v>-0.03265342238335223</v>
+        <v>0.009849008413409145</v>
       </c>
       <c r="E44">
-        <v>0.316265148381986</v>
+        <v>0.3012305668534642</v>
       </c>
       <c r="F44">
-        <v>1.999999864931711</v>
+        <v>1.834190011641778</v>
       </c>
       <c r="G44">
-        <v>0.03936629053902025</v>
+        <v>-0.0632777622729922</v>
       </c>
       <c r="H44">
-        <v>52.53312949785076</v>
+        <v>-2.887083871084747E-06</v>
       </c>
       <c r="I44">
-        <v>49.71993067741214</v>
+        <v>30.86810830068822</v>
       </c>
       <c r="J44">
-        <v>55.68799698598681</v>
+        <v>171.4201995094965</v>
       </c>
       <c r="K44">
-        <v>53.48212057534185</v>
+        <v>164.6005763717414</v>
       </c>
       <c r="L44">
-        <v>0.03379423605154323</v>
+        <v>0.03745068456376621</v>
       </c>
       <c r="M44">
-        <v>223.5503920599814</v>
+        <v>3.263872276429288E-06</v>
       </c>
       <c r="N44">
-        <v>2.352401576515773E-31</v>
+        <v>-108.9857890138413</v>
       </c>
       <c r="O44">
-        <v>-120.0131847962945</v>
+        <v>-127.4587917401681</v>
       </c>
       <c r="P44">
-        <v>-197.2597895081246</v>
+        <v>-66.4428057494016</v>
       </c>
     </row>
     <row r="45" spans="1:16">
       <c r="A45">
-        <v>9.819407762522172</v>
+        <v>383.3919308562669</v>
       </c>
       <c r="B45">
         <v>0.02</v>
       </c>
       <c r="C45">
-        <v>18.10547760821647</v>
+        <v>8.055989276549292</v>
       </c>
       <c r="D45">
-        <v>-0.03396394063563473</v>
+        <v>0.008608498043274019</v>
       </c>
       <c r="E45">
-        <v>0.3043746259104375</v>
+        <v>0.2176023916043388</v>
       </c>
       <c r="F45">
-        <v>1.984962779664668</v>
+        <v>1.7672614527405</v>
       </c>
       <c r="G45">
-        <v>0.02115319309012525</v>
+        <v>0.005308992473549387</v>
       </c>
       <c r="H45">
-        <v>51.78285227705366</v>
+        <v>88.98680437041249</v>
       </c>
       <c r="I45">
-        <v>51.47577498699793</v>
+        <v>171.4285739642258</v>
       </c>
       <c r="J45">
-        <v>56.55507094433766</v>
+        <v>35.51508616904943</v>
       </c>
       <c r="K45">
-        <v>53.76339575335403</v>
+        <v>5.393714556615848</v>
       </c>
       <c r="L45">
-        <v>0.02756209752023485</v>
+        <v>0.02863371391730217</v>
       </c>
       <c r="M45">
-        <v>255.0793967543425</v>
+        <v>405.1222665474241</v>
       </c>
       <c r="N45">
-        <v>-1.216987510771085E-30</v>
+        <v>0.0001994820815969802</v>
       </c>
       <c r="O45">
-        <v>-180.4669891039564</v>
+        <v>-115.323038554969</v>
       </c>
       <c r="P45">
-        <v>-190.0125905030407</v>
+        <v>-58.52872855414194</v>
       </c>
     </row>
     <row r="46" spans="1:16">
       <c r="A46">
-        <v>10.09617809614165</v>
+        <v>383.9845267389514</v>
       </c>
       <c r="B46">
         <v>0.02</v>
       </c>
       <c r="C46">
-        <v>18.37587661309</v>
+        <v>9.028602572064788</v>
       </c>
       <c r="D46">
-        <v>-0.03444662946367001</v>
+        <v>0.004889796292154015</v>
       </c>
       <c r="E46">
-        <v>0.2840196943296125</v>
+        <v>0.1738396328522046</v>
       </c>
       <c r="F46">
-        <v>1.860194615692348</v>
+        <v>1.861824344012618</v>
       </c>
       <c r="G46">
-        <v>-0.002449160335722087</v>
+        <v>0.01473537134974662</v>
       </c>
       <c r="H46">
-        <v>53.68630402839651</v>
+        <v>37.87585709231951</v>
       </c>
       <c r="I46">
-        <v>51.23899152109929</v>
+        <v>171.4285733652439</v>
       </c>
       <c r="J46">
-        <v>57.24831629396588</v>
+        <v>171.3645108788047</v>
       </c>
       <c r="K46">
-        <v>54.79040116336819</v>
+        <v>127.7242671851465</v>
       </c>
       <c r="L46">
-        <v>0.0105274321386805</v>
+        <v>0.01758619282455282</v>
       </c>
       <c r="M46">
-        <v>244.5411071237461</v>
+        <v>137.4568833783262</v>
       </c>
       <c r="N46">
-        <v>-9.30583052841991E-30</v>
+        <v>0.0001996529719345974</v>
       </c>
       <c r="O46">
-        <v>-141.0928793981904</v>
+        <v>-100.3212393374474</v>
       </c>
       <c r="P46">
-        <v>-174.5798692089672</v>
+        <v>-50.40392103546151</v>
       </c>
     </row>
     <row r="47" spans="1:16">
       <c r="A47">
-        <v>10.37058164915373</v>
+        <v>384.5236715130082</v>
       </c>
       <c r="B47">
         <v>0.02</v>
       </c>
       <c r="C47">
-        <v>18.61104172838906</v>
+        <v>9.725713536445353</v>
       </c>
       <c r="D47">
-        <v>-0.03789585827521252</v>
+        <v>0.0003698205632270834</v>
       </c>
       <c r="E47">
-        <v>0.2622089044107401</v>
+        <v>0.1383874013566217</v>
       </c>
       <c r="F47">
-        <v>1.586827175290384</v>
+        <v>1.89633036154025</v>
       </c>
       <c r="G47">
-        <v>-0.03255404080890677</v>
+        <v>-0.006953650377699439</v>
       </c>
       <c r="H47">
-        <v>53.24441312161098</v>
+        <v>16.65149387051026</v>
       </c>
       <c r="I47">
-        <v>52.95110200559144</v>
+        <v>171.4285731657336</v>
       </c>
       <c r="J47">
-        <v>58.26542181642778</v>
+        <v>171.1894133134</v>
       </c>
       <c r="K47">
-        <v>55.3661261253029</v>
+        <v>117.8126710842341</v>
       </c>
       <c r="L47">
-        <v>0.005360065039212361</v>
+        <v>0.01050199670059428</v>
       </c>
       <c r="M47">
-        <v>272.1752115071617</v>
+        <v>121.7760529062457</v>
       </c>
       <c r="N47">
-        <v>-9.437179747590532E-31</v>
+        <v>0.0001997093264230432</v>
       </c>
       <c r="O47">
-        <v>-190.0481416090455</v>
+        <v>-83.56828454328904</v>
       </c>
       <c r="P47">
-        <v>-165.6302451048647</v>
+        <v>-41.59461881304307</v>
       </c>
     </row>
     <row r="48" spans="1:16">
       <c r="A48">
-        <v>10.64375626276973</v>
+        <v>385.0307635338429</v>
       </c>
       <c r="B48">
         <v>0.01991830220998726</v>
       </c>
       <c r="C48">
-        <v>18.91926512013778</v>
+        <v>10.23258814852241</v>
       </c>
       <c r="D48">
-        <v>-0.03720035898949309</v>
+        <v>-0.00189341310996009</v>
       </c>
       <c r="E48">
-        <v>0.23470033260237</v>
+        <v>0.1089926021670921</v>
       </c>
       <c r="F48">
-        <v>1.134233650033034</v>
+        <v>1.751320840640777</v>
       </c>
       <c r="G48">
-        <v>-0.06929197920200716</v>
+        <v>-0.04934821295063403</v>
       </c>
       <c r="H48">
-        <v>55.06600667091554</v>
+        <v>7.601835771059378</v>
       </c>
       <c r="I48">
-        <v>53.02558516164466</v>
+        <v>171.4285727235387</v>
       </c>
       <c r="J48">
-        <v>59.14145391038939</v>
+        <v>171.2563094115709</v>
       </c>
       <c r="K48">
-        <v>56.4042149913326</v>
+        <v>111.0120448500262</v>
       </c>
       <c r="L48">
-        <v>-0.0077463281846291</v>
+        <v>0.006246432045545776</v>
       </c>
       <c r="M48">
-        <v>271.9467120228146</v>
+        <v>103.5285300361086</v>
       </c>
       <c r="N48">
-        <v>7.294076685247619E-30</v>
+        <v>0.0001997418775560964</v>
       </c>
       <c r="O48">
-        <v>-164.486285531264</v>
+        <v>-67.97649481127708</v>
       </c>
       <c r="P48">
-        <v>-145.5832846930768</v>
+        <v>-33.54496094159587</v>
       </c>
     </row>
     <row r="49" spans="1:16">
       <c r="A49">
-        <v>10.91728605354176</v>
+        <v>385.5231693221205</v>
       </c>
       <c r="B49">
         <v>0.01649435061504471</v>
       </c>
       <c r="C49">
-        <v>19.22058985590987</v>
+        <v>10.5838560986007</v>
       </c>
       <c r="D49">
-        <v>-0.03859596754771999</v>
+        <v>-0.002781462428249359</v>
       </c>
       <c r="E49">
-        <v>0.2045581682624821</v>
+        <v>0.08481473246016291</v>
       </c>
       <c r="F49">
-        <v>0.4915141992219205</v>
+        <v>1.372507159837443</v>
       </c>
       <c r="G49">
-        <v>-0.09586886879412186</v>
+        <v>-0.08861207917973049</v>
       </c>
       <c r="H49">
-        <v>54.9355867617726</v>
+        <v>3.613384762751696</v>
       </c>
       <c r="I49">
-        <v>54.76806918576017</v>
+        <v>171.4285719898419</v>
       </c>
       <c r="J49">
-        <v>60.28574355370315</v>
+        <v>171.172971775934</v>
       </c>
       <c r="K49">
-        <v>57.29226541078476</v>
+        <v>106.2382889625225</v>
       </c>
       <c r="L49">
-        <v>-0.01145590098799235</v>
+        <v>0.003720060442982321</v>
       </c>
       <c r="M49">
-        <v>302.382786048038</v>
+        <v>83.62357939964056</v>
       </c>
       <c r="N49">
-        <v>-7.413824476071486E-31</v>
+        <v>0.0001997627473227951</v>
       </c>
       <c r="O49">
-        <v>-206.7726729348484</v>
+        <v>-53.93265230056954</v>
       </c>
       <c r="P49">
-        <v>-131.301250648508</v>
+        <v>-26.42388440454391</v>
       </c>
     </row>
     <row r="50" spans="1:16">
       <c r="A50">
-        <v>11.18979201538024</v>
+        <v>386.0109212494555</v>
       </c>
       <c r="B50">
         <v>0.009809843005185111</v>
       </c>
       <c r="C50">
-        <v>19.60062225845789</v>
+        <v>10.80251214440495</v>
       </c>
       <c r="D50">
-        <v>-0.03551467540361967</v>
+        <v>-0.002894853749762275</v>
       </c>
       <c r="E50">
-        <v>0.1713465552052831</v>
+        <v>0.06519857980062542</v>
       </c>
       <c r="F50">
-        <v>-0.2233307246219464</v>
+        <v>0.8432682463758998</v>
       </c>
       <c r="G50">
-        <v>-0.09619850324199698</v>
+        <v>-0.1038154187969173</v>
       </c>
       <c r="H50">
-        <v>56.81260921575408</v>
+        <v>1.817437972777156</v>
       </c>
       <c r="I50">
-        <v>55.21912616879638</v>
+        <v>171.4285704780864</v>
       </c>
       <c r="J50">
-        <v>61.41483650969563</v>
+        <v>170.2908036876566</v>
       </c>
       <c r="K50">
-        <v>58.5178634365199</v>
+        <v>102.2812029480785</v>
       </c>
       <c r="L50">
-        <v>-0.02193531581744311</v>
+        <v>0.002262226864125965</v>
       </c>
       <c r="M50">
-        <v>313.5115482953804</v>
+        <v>57.82534271762061</v>
       </c>
       <c r="N50">
-        <v>2.428808427027646E-31</v>
+        <v>0.0001997745287455976</v>
       </c>
       <c r="O50">
-        <v>-194.7837204811747</v>
+        <v>-41.86865787479469</v>
       </c>
       <c r="P50">
-        <v>-106.4830237513414</v>
+        <v>-20.40180903239728</v>
       </c>
     </row>
     <row r="51" spans="1:16">
       <c r="A51">
-        <v>11.45734382909261</v>
+        <v>386.4959033344862</v>
       </c>
       <c r="B51">
         <v>0.003233794600127655</v>
       </c>
       <c r="C51">
-        <v>19.99378005686687</v>
+        <v>10.90775409613783</v>
       </c>
       <c r="D51">
-        <v>-0.03455940870307408</v>
+        <v>-0.002611252663796164</v>
       </c>
       <c r="E51">
-        <v>0.1362198362502424</v>
+        <v>0.04966362439551574</v>
       </c>
       <c r="F51">
-        <v>-0.866589804777582</v>
+        <v>0.2982196609155605</v>
       </c>
       <c r="G51">
-        <v>-0.07209005550940069</v>
+        <v>-0.0931538123689617</v>
       </c>
       <c r="H51">
-        <v>57.05344889906311</v>
+        <v>0.9898575977976396</v>
       </c>
       <c r="I51">
-        <v>57.08606609375592</v>
+        <v>171.4285660541739</v>
       </c>
       <c r="J51">
-        <v>62.78037732534976</v>
+        <v>165.4813939015812</v>
       </c>
       <c r="K51">
-        <v>59.80607084570988</v>
+        <v>95.55260585199477</v>
       </c>
       <c r="L51">
-        <v>-0.02340240964807794</v>
+        <v>0.001450095435172325</v>
       </c>
       <c r="M51">
-        <v>344.8597562577993</v>
+        <v>43.34927383714518</v>
       </c>
       <c r="N51">
-        <v>-6.572276610274761E-30</v>
+        <v>0.0001997792276190203</v>
       </c>
       <c r="O51">
-        <v>-229.3808801869622</v>
+        <v>-31.96765559778959</v>
       </c>
       <c r="P51">
-        <v>-88.69013583422591</v>
+        <v>-15.51828735437315</v>
       </c>
     </row>
     <row r="52" spans="1:16">
       <c r="A52">
-        <v>11.71797598337239</v>
+        <v>386.9784472961992</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52">
-        <v>20.45153614189159</v>
+        <v>10.92076081929019</v>
       </c>
       <c r="D52">
-        <v>-0.02980111408246361</v>
+        <v>-0.002166861164070132</v>
       </c>
       <c r="E52">
-        <v>0.1023881967446281</v>
+        <v>0.03761935623202067</v>
       </c>
       <c r="F52">
-        <v>-1.330283582595182</v>
+        <v>-0.1477303146634473</v>
       </c>
       <c r="G52">
-        <v>-0.0410563103650491</v>
+        <v>-0.07225410287297838</v>
       </c>
       <c r="H52">
-        <v>59.02630543832731</v>
+        <v>0.5878311635972819</v>
       </c>
       <c r="I52">
-        <v>57.89317031525459</v>
+        <v>171.4284854879963</v>
       </c>
       <c r="J52">
-        <v>64.15931887715459</v>
+        <v>160.8784359337548</v>
       </c>
       <c r="K52">
-        <v>61.28380372892499</v>
+        <v>89.80045186901765</v>
       </c>
       <c r="L52">
-        <v>-0.0296431275454726</v>
+        <v>0.001025179005282881</v>
       </c>
       <c r="M52">
-        <v>362.9837397638042</v>
+        <v>33.5216254755444</v>
       </c>
       <c r="N52">
-        <v>1.553884969042059E-29</v>
+        <v>0.0001997802964525157</v>
       </c>
       <c r="O52">
-        <v>-227.8503562528336</v>
+        <v>-24.11188566969494</v>
       </c>
       <c r="P52">
-        <v>-63.65573791435528</v>
+        <v>-11.67571992858589</v>
       </c>
     </row>
     <row r="53" spans="1:16">
       <c r="A53">
-        <v>11.97214748785181</v>
+        <v>387.4613426542454</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53">
-        <v>20.92891599224533</v>
+        <v>10.86233879859392</v>
       </c>
       <c r="D53">
-        <v>-0.02675311687018086</v>
+        <v>-0.001689320628887865</v>
       </c>
       <c r="E53">
-        <v>0.06953685504965307</v>
+        <v>0.02840862272140857</v>
       </c>
       <c r="F53">
-        <v>-1.635005788406454</v>
+        <v>-0.494593342608816</v>
       </c>
       <c r="G53">
-        <v>-0.01927449436217221</v>
+        <v>-0.05643139062821931</v>
       </c>
       <c r="H53">
-        <v>59.6266075985923</v>
+        <v>1.054233932755379E-05</v>
       </c>
       <c r="I53">
-        <v>59.86082576464671</v>
+        <v>171.0689628100801</v>
       </c>
       <c r="J53">
-        <v>65.72881313786736</v>
+        <v>157.443452151944</v>
       </c>
       <c r="K53">
-        <v>62.96952920945337</v>
+        <v>85.69632134516318</v>
       </c>
       <c r="L53">
-        <v>-0.02608121989660552</v>
+        <v>0.0007646463787985297</v>
       </c>
       <c r="M53">
-        <v>390.6272278688153</v>
+        <v>26.51595291811233</v>
       </c>
       <c r="N53">
-        <v>1.754837716188897E-29</v>
+        <v>0.0001997790584360903</v>
       </c>
       <c r="O53">
-        <v>-254.0555690094482</v>
+        <v>-18.00062019867099</v>
       </c>
       <c r="P53">
-        <v>-47.30003107700363</v>
+        <v>-8.703171236428629</v>
       </c>
     </row>
     <row r="54" spans="1:16">
       <c r="A54">
-        <v>12.22006230863698</v>
+        <v>387.9476983486949</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54">
-        <v>21.45086250124922</v>
+        <v>10.74940455838039</v>
       </c>
       <c r="D54">
-        <v>-0.02084018743828562</v>
+        <v>-0.001273509830267965</v>
       </c>
       <c r="E54">
-        <v>0.04239728626678527</v>
+        <v>0.02137001379297698</v>
       </c>
       <c r="F54">
-        <v>-1.821084291450236</v>
+        <v>-0.7660984240537432</v>
       </c>
       <c r="G54">
-        <v>-0.005477968580721022</v>
+        <v>-0.04441804797409896</v>
       </c>
       <c r="H54">
-        <v>61.67863659980172</v>
+        <v>3.905913536239828E-06</v>
       </c>
       <c r="I54">
-        <v>60.95624172203545</v>
+        <v>171.1902715275834</v>
       </c>
       <c r="J54">
-        <v>67.32495865425422</v>
+        <v>155.3032416594431</v>
       </c>
       <c r="K54">
-        <v>64.72162965213079</v>
+        <v>83.17349368215338</v>
       </c>
       <c r="L54">
-        <v>-0.02549734842109723</v>
+        <v>0.0006242295439325173</v>
       </c>
       <c r="M54">
-        <v>407.7695549652397</v>
+        <v>21.61862917967242</v>
       </c>
       <c r="N54">
-        <v>2.138316141107261E-29</v>
+        <v>0.0001997756266513288</v>
       </c>
       <c r="O54">
-        <v>-257.1210426905168</v>
+        <v>-13.33094574457206</v>
       </c>
       <c r="P54">
-        <v>-27.98035286826806</v>
+        <v>-6.43950264548321</v>
       </c>
     </row>
     <row r="55" spans="1:16">
       <c r="A55">
-        <v>12.4618641413827</v>
+        <v>388.439902728492</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55">
-        <v>21.98102523013781</v>
+        <v>10.59633005167963</v>
       </c>
       <c r="D55">
-        <v>-0.01632475671977554</v>
+        <v>-0.0009194054039673202</v>
       </c>
       <c r="E55">
-        <v>0.02003675377682059</v>
+        <v>0.01604220419506138</v>
       </c>
       <c r="F55">
-        <v>-1.924829173039639</v>
+        <v>-0.9801867607194868</v>
       </c>
       <c r="G55">
-        <v>0.001994820734094132</v>
+        <v>-0.03528172045530424</v>
       </c>
       <c r="H55">
-        <v>62.57403605493435</v>
+        <v>1.895729608163532E-06</v>
       </c>
       <c r="I55">
-        <v>62.93356289575028</v>
+        <v>171.2672268842661</v>
       </c>
       <c r="J55">
-        <v>69.04403538169329</v>
+        <v>154.47553741282</v>
       </c>
       <c r="K55">
-        <v>66.74689690956677</v>
+        <v>82.13092140428995</v>
       </c>
       <c r="L55">
-        <v>-0.01796466441569363</v>
+        <v>0.0005352667094880269</v>
       </c>
       <c r="M55">
-        <v>426.1651608657469</v>
+        <v>16.8641398886169</v>
       </c>
       <c r="N55">
-        <v>-6.624582539336354E-29</v>
+        <v>0.0001997699855437323</v>
       </c>
       <c r="O55">
-        <v>-273.9243793050162</v>
+        <v>-9.823416271014077</v>
       </c>
       <c r="P55">
-        <v>-16.95334649250927</v>
+        <v>-4.742690815982626</v>
       </c>
     </row>
     <row r="56" spans="1:16">
       <c r="A56">
-        <v>12.69780102770439</v>
+        <v>388.9398426543783</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56">
-        <v>22.52282477820338</v>
+        <v>10.41419329716213</v>
       </c>
       <c r="D56">
-        <v>-0.01077731604276446</v>
+        <v>-0.000641254732964019</v>
       </c>
       <c r="E56">
-        <v>0.005091053568056193</v>
+        <v>0.01203065834577294</v>
       </c>
       <c r="F56">
-        <v>-1.974623342200836</v>
+        <v>-1.150521440806501</v>
       </c>
       <c r="G56">
-        <v>0.00488581305245185</v>
+        <v>-0.02831959598955932</v>
       </c>
       <c r="H56">
-        <v>64.59154998711496</v>
+        <v>9.383162734491275E-07</v>
       </c>
       <c r="I56">
-        <v>64.16249780497749</v>
+        <v>171.3186808947778</v>
       </c>
       <c r="J56">
-        <v>70.78371992988001</v>
+        <v>154.2304371166763</v>
       </c>
       <c r="K56">
-        <v>68.75421185934624</v>
+        <v>81.76668310681198</v>
       </c>
       <c r="L56">
-        <v>-0.01589649410062524</v>
+        <v>0.0004683507003417708</v>
       </c>
       <c r="M56">
-        <v>436.5805068569553</v>
+        <v>13.70726701677308</v>
       </c>
       <c r="N56">
-        <v>1.537391592796668E-27</v>
+        <v>0.0001997618083345029</v>
       </c>
       <c r="O56">
-        <v>-275.7730645575422</v>
+        <v>-7.215808033424183</v>
       </c>
       <c r="P56">
-        <v>-4.318040816968792</v>
+        <v>-3.482728399756915</v>
       </c>
     </row>
     <row r="57" spans="1:16">
       <c r="A57">
-        <v>12.92820008680493</v>
+        <v>389.4490399866193</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
       <c r="C57">
-        <v>23.04876388770719</v>
+        <v>10.21175428861547</v>
       </c>
       <c r="D57">
-        <v>-0.007254018003740477</v>
+        <v>-0.000432851353353996</v>
       </c>
       <c r="E57">
-        <v>-0.005741199020544688</v>
+        <v>0.009020077754621715</v>
       </c>
       <c r="F57">
-        <v>-1.994620451105244</v>
+        <v>-1.287504645593823</v>
       </c>
       <c r="G57">
-        <v>0.004755735290799788</v>
+        <v>-0.02300347003089997</v>
       </c>
       <c r="H57">
-        <v>65.62154947119235</v>
+        <v>3.84113850708343E-07</v>
       </c>
       <c r="I57">
-        <v>66.00181693176427</v>
+        <v>171.3538938989614</v>
       </c>
       <c r="J57">
-        <v>72.64410300182259</v>
+        <v>154.6427913556667</v>
       </c>
       <c r="K57">
-        <v>71.23148013850066</v>
+        <v>82.11353761754978</v>
       </c>
       <c r="L57">
-        <v>-0.007644599035413526</v>
+        <v>0.0004110237084717464</v>
       </c>
       <c r="M57">
-        <v>443.0433176791869</v>
+        <v>10.47720131606968</v>
       </c>
       <c r="N57">
-        <v>1.084809255320042E-28</v>
+        <v>0.0001997507128386661</v>
       </c>
       <c r="O57">
-        <v>-283.0594031137477</v>
+        <v>-5.291341242239641</v>
       </c>
       <c r="P57">
-        <v>-0.4392686744444267</v>
+        <v>-2.55347139176565</v>
       </c>
     </row>
     <row r="58" spans="1:16">
       <c r="A58">
-        <v>13.15348202580292</v>
+        <v>389.9687470974291</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58">
-        <v>23.55598631415235</v>
+        <v>9.995753403456565</v>
       </c>
       <c r="D58">
-        <v>-0.003204549737869117</v>
+        <v>-0.0002821446417660446</v>
       </c>
       <c r="E58">
-        <v>-0.01058228958997999</v>
+        <v>0.006765103456664595</v>
       </c>
       <c r="F58">
-        <v>-1.99999946949124</v>
+        <v>-1.399045488322683</v>
       </c>
       <c r="G58">
-        <v>0.002877153098402982</v>
+        <v>-0.01893588395654465</v>
       </c>
       <c r="H58">
-        <v>67.44982549663361</v>
+        <v>2.703544833358558E-08</v>
       </c>
       <c r="I58">
-        <v>67.19564481840062</v>
+        <v>171.3781308645132</v>
       </c>
       <c r="J58">
-        <v>74.39803962934799</v>
+        <v>155.1498187859613</v>
       </c>
       <c r="K58">
-        <v>73.32689799248394</v>
+        <v>82.58474692368466</v>
       </c>
       <c r="L58">
-        <v>-0.0009191491256197496</v>
+        <v>0.0003586436656713179</v>
       </c>
       <c r="M58">
-        <v>441.4123915148464</v>
+        <v>9.308304849218029</v>
       </c>
       <c r="N58">
-        <v>3.578564923998964E-29</v>
+        <v>0.000199735861223443</v>
       </c>
       <c r="O58">
-        <v>-280.1324257312623</v>
+        <v>-3.877896021660475</v>
       </c>
       <c r="P58">
-        <v>2.239121827019806</v>
+        <v>-1.871217866220606</v>
       </c>
     </row>
     <row r="59" spans="1:16">
       <c r="A59">
-        <v>13.37413336798776</v>
+        <v>390.5000169499079</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
       <c r="C59">
-        <v>24.02649350523733</v>
+        <v>9.77129267316943</v>
       </c>
       <c r="D59">
-        <v>4.405031059662506E-05</v>
+        <v>-0.0001763478095069599</v>
       </c>
       <c r="E59">
-        <v>-0.01095113528741443</v>
+        <v>0.005077634176713114</v>
       </c>
       <c r="F59">
-        <v>-1.997995329610591</v>
+        <v>-1.49115539982555</v>
       </c>
       <c r="G59">
-        <v>0.0004784570750179082</v>
+        <v>-0.01581723797702659</v>
       </c>
       <c r="H59">
-        <v>68.4561102559819</v>
+        <v>-2.176000434619272E-07</v>
       </c>
       <c r="I59">
-        <v>68.77283412519076</v>
+        <v>171.3947595608326</v>
       </c>
       <c r="J59">
-        <v>75.73425010866306</v>
+        <v>156.3284418691475</v>
       </c>
       <c r="K59">
-        <v>75.21427560366803</v>
+        <v>83.74384007102272</v>
       </c>
       <c r="L59">
-        <v>0.007027812333839</v>
+        <v>0.0003100361929419782</v>
       </c>
       <c r="M59">
-        <v>442.252938730777</v>
+        <v>8.404986337823424</v>
       </c>
       <c r="N59">
-        <v>2.191776469345094E-30</v>
+        <v>0.0001997162200303187</v>
       </c>
       <c r="O59">
-        <v>-282.9434481013639</v>
+        <v>-2.842783032315081</v>
       </c>
       <c r="P59">
-        <v>0.8022067544612832</v>
+        <v>-1.371678821845765</v>
       </c>
     </row>
     <row r="60" spans="1:16">
       <c r="A60">
-        <v>13.5906368690226</v>
+        <v>391.0437547542587</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
       <c r="C60">
-        <v>24.46761562216563</v>
+        <v>9.542185160218212</v>
       </c>
       <c r="D60">
-        <v>0.002819398856350751</v>
+        <v>-0.0001040576466395266</v>
       </c>
       <c r="E60">
-        <v>-0.00697825805773308</v>
+        <v>0.003814991261665513</v>
       </c>
       <c r="F60">
-        <v>-1.991915840225344</v>
+        <v>-1.568404325568113</v>
       </c>
       <c r="G60">
-        <v>-0.001476632088750429</v>
+        <v>-0.01342131266299415</v>
       </c>
       <c r="H60">
-        <v>70.01351034320673</v>
+        <v>-3.895385580098317E-07</v>
       </c>
       <c r="I60">
-        <v>69.82217409422954</v>
+        <v>171.4060894700621</v>
       </c>
       <c r="J60">
-        <v>77.06231528739983</v>
+        <v>158.0092911519104</v>
       </c>
       <c r="K60">
-        <v>76.71743044463342</v>
+        <v>85.41405181126223</v>
       </c>
       <c r="L60">
-        <v>0.008126363465820035</v>
+        <v>0.0002653131898195549</v>
       </c>
       <c r="M60">
-        <v>440.3382749522</v>
+        <v>7.232496905739414</v>
       </c>
       <c r="N60">
-        <v>1.377542464860059E-29</v>
+        <v>0.0001996900955445323</v>
       </c>
       <c r="O60">
-        <v>-280.5187919297882</v>
+        <v>-2.085826436919751</v>
       </c>
       <c r="P60">
-        <v>1.662760382008889</v>
+        <v>-1.006414101369191</v>
       </c>
     </row>
     <row r="61" spans="1:16">
       <c r="A61">
-        <v>13.80341810626703</v>
+        <v>391.6007564176062</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="C61">
-        <v>24.87521503496018</v>
+        <v>9.3112500561269</v>
       </c>
       <c r="D61">
-        <v>0.003543112282022477</v>
+        <v>-5.597786537648866E-05</v>
       </c>
       <c r="E61">
-        <v>-0.002313108320789624</v>
+        <v>0.002869775765872218</v>
       </c>
       <c r="F61">
-        <v>-1.985297196179395</v>
+        <v>-1.634268855483865</v>
       </c>
       <c r="G61">
-        <v>-0.002465031085992346</v>
+        <v>-0.01157699030132441</v>
       </c>
       <c r="H61">
-        <v>70.94535293757322</v>
+        <v>-5.082780520796796E-07</v>
       </c>
       <c r="I61">
-        <v>71.14887505158923</v>
+        <v>171.4137483967926</v>
       </c>
       <c r="J61">
-        <v>78.17084037526534</v>
+        <v>159.8254556877939</v>
       </c>
       <c r="K61">
-        <v>78.16785417738534</v>
+        <v>87.22442044955559</v>
       </c>
       <c r="L61">
-        <v>0.007716898444950014</v>
+        <v>0.0002248575064516223</v>
       </c>
       <c r="M61">
-        <v>441.2140416227772</v>
+        <v>7.816262441656634</v>
       </c>
       <c r="N61">
-        <v>2.155968690372191E-30</v>
+        <v>0.0001996545838521818</v>
       </c>
       <c r="O61">
-        <v>-282.6656477069695</v>
+        <v>-1.532481511433951</v>
       </c>
       <c r="P61">
-        <v>0.5524195406049585</v>
+        <v>-0.7394153097146714</v>
       </c>
     </row>
     <row r="62" spans="1:16">
       <c r="A62">
-        <v>14.01284566600077</v>
+        <v>392.1717373846776</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="C62">
-        <v>25.25806698070437</v>
+        <v>9.080551401623079</v>
       </c>
       <c r="D62">
-        <v>0.003151679616284214</v>
+        <v>-2.494462106945585E-05</v>
       </c>
       <c r="E62">
-        <v>0.001936889933207007</v>
+        <v>0.002161562881917182</v>
       </c>
       <c r="F62">
-        <v>-1.98094711372665</v>
+        <v>-1.691396914352508</v>
       </c>
       <c r="G62">
-        <v>-0.002498123699927706</v>
+        <v>-0.01015457848468331</v>
       </c>
       <c r="H62">
-        <v>72.25773869875196</v>
+        <v>-5.823621552858303E-07</v>
       </c>
       <c r="I62">
-        <v>72.08578514915888</v>
+        <v>171.4188868335516</v>
       </c>
       <c r="J62">
-        <v>79.31966045630027</v>
+        <v>162.5133873914778</v>
       </c>
       <c r="K62">
-        <v>79.42812534255813</v>
+        <v>89.90919011771156</v>
       </c>
       <c r="L62">
-        <v>0.003984338939220324</v>
+        <v>0.0001889236247864851</v>
       </c>
       <c r="M62">
-        <v>440.2218583029254</v>
+        <v>10.4910320464884</v>
       </c>
       <c r="N62">
-        <v>-4.418836325438934E-29</v>
+        <v>0.0001996049599964377</v>
       </c>
       <c r="O62">
-        <v>-281.2314556765193</v>
+        <v>-1.127810932579923</v>
       </c>
       <c r="P62">
-        <v>0.6271506802736259</v>
+        <v>-0.5441599616818351</v>
       </c>
     </row>
     <row r="63" spans="1:16">
       <c r="A63">
-        <v>14.21923162541453</v>
+        <v>392.7573544005883</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="C63">
-        <v>25.61434011708347</v>
+        <v>8.851585524261271</v>
       </c>
       <c r="D63">
-        <v>0.001760153631069652</v>
+        <v>-5.646993185429463E-06</v>
       </c>
       <c r="E63">
-        <v>0.004158240509543088</v>
+        <v>0.001630317959076604</v>
       </c>
       <c r="F63">
-        <v>-1.980065096117542</v>
+        <v>-1.741808361599838</v>
       </c>
       <c r="G63">
-        <v>-0.001858931070325327</v>
+        <v>-0.009055571004820819</v>
       </c>
       <c r="H63">
-        <v>73.10693578129042</v>
+        <v>-6.127360462332639E-07</v>
       </c>
       <c r="I63">
-        <v>73.22403316458468</v>
+        <v>171.4223112663841</v>
       </c>
       <c r="J63">
-        <v>80.37793374019853</v>
+        <v>167.0985304221826</v>
       </c>
       <c r="K63">
-        <v>80.61156602101046</v>
+        <v>94.4926046109792</v>
       </c>
       <c r="L63">
-        <v>0.001209228178324576</v>
+        <v>0.0001575363143056968</v>
       </c>
       <c r="M63">
-        <v>440.7849745155056</v>
+        <v>8.181244610761585</v>
       </c>
       <c r="N63">
-        <v>-5.297878702402491E-30</v>
+        <v>0.0001995341108780757</v>
       </c>
       <c r="O63">
-        <v>-282.6993987681153</v>
+        <v>-0.8315786841067161</v>
       </c>
       <c r="P63">
-        <v>-0.4635818549206762</v>
+        <v>-0.4012286358433014</v>
       </c>
     </row>
     <row r="64" spans="1:16">
       <c r="A64">
-        <v>14.42285139068643</v>
+        <v>393.3582220216385</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
       <c r="C64">
-        <v>25.949387934466</v>
+        <v>8.625425098893372</v>
       </c>
       <c r="D64">
-        <v>0.0004163902762145762</v>
+        <v>5.74213086144677E-06</v>
       </c>
       <c r="E64">
-        <v>0.004767708811659001</v>
+        <v>0.001231299726642224</v>
       </c>
       <c r="F64">
-        <v>-1.982229727911674</v>
+        <v>-1.787046680340905</v>
       </c>
       <c r="G64">
-        <v>-0.0009419263301016941</v>
+        <v>-0.008204979862981963</v>
       </c>
       <c r="H64">
-        <v>74.21283367017635</v>
+        <v>-5.928441409179228E-07</v>
       </c>
       <c r="I64">
-        <v>74.07448620573456</v>
+        <v>171.4245804701144</v>
       </c>
       <c r="J64">
-        <v>81.47474165363556</v>
+        <v>170.8192393054927</v>
       </c>
       <c r="K64">
-        <v>81.61787564299281</v>
+        <v>98.21236625036269</v>
       </c>
       <c r="L64">
-        <v>-0.001963827259961594</v>
+        <v>0.0001305140869346155</v>
       </c>
       <c r="M64">
-        <v>439.8754243026239</v>
+        <v>1.909988756214035</v>
       </c>
       <c r="N64">
-        <v>-2.961536548127957E-30</v>
+        <v>0.0001994272530047032</v>
       </c>
       <c r="O64">
-        <v>-281.5575462053598</v>
+        <v>-0.6144265338082043</v>
       </c>
       <c r="P64">
-        <v>-0.3285367685865132</v>
+        <v>-0.2964540540581682</v>
       </c>
     </row>
     <row r="65" spans="1:16">
       <c r="A65">
-        <v>14.62394765235881</v>
+        <v>393.9749252113708</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="C65">
-        <v>26.26162163751965</v>
+        <v>8.402828228634046</v>
       </c>
       <c r="D65">
-        <v>-0.0007950274280725685</v>
+        <v>1.19202139149539E-05</v>
       </c>
       <c r="E65">
-        <v>0.00373024822120531</v>
+        <v>0.0009311807337273499</v>
       </c>
       <c r="F65">
-        <v>-1.986361849852085</v>
+        <v>-1.828293562124868</v>
       </c>
       <c r="G65">
-        <v>-8.14858420235277E-05</v>
+        <v>-0.007545588942431365</v>
       </c>
       <c r="H65">
-        <v>74.97953087159206</v>
+        <v>-5.052588358815846E-07</v>
       </c>
       <c r="I65">
-        <v>75.05760147901722</v>
+        <v>171.4260770743564</v>
       </c>
       <c r="J65">
-        <v>82.48447334663639</v>
+        <v>171.3028513515576</v>
       </c>
       <c r="K65">
-        <v>82.56403194703815</v>
+        <v>98.69545775755171</v>
       </c>
       <c r="L65">
-        <v>-0.003008505676550867</v>
+        <v>0.000107531351706215</v>
       </c>
       <c r="M65">
-        <v>440.0529158358166</v>
+        <v>0.878598996686098</v>
       </c>
       <c r="N65">
-        <v>7.239456466319677E-31</v>
+        <v>0.000199251683531927</v>
       </c>
       <c r="O65">
-        <v>-282.4967468467839</v>
+        <v>-0.4549764558209604</v>
       </c>
       <c r="P65">
-        <v>-0.8685256198183162</v>
+        <v>-0.2195206974945897</v>
       </c>
     </row>
     <row r="66" spans="1:16">
       <c r="A66">
-        <v>14.82273851727173</v>
+        <v>394.6080290086285</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66">
-        <v>26.55508450395694</v>
+        <v>8.184320217448974</v>
       </c>
       <c r="D66">
-        <v>-0.001354133202986988</v>
+        <v>1.475342967888158E-05</v>
       </c>
       <c r="E66">
-        <v>0.00210608957344559</v>
+        <v>0.0007051279545345824</v>
       </c>
       <c r="F66">
-        <v>-1.991098758059789</v>
+        <v>-1.866455467089181</v>
       </c>
       <c r="G66">
-        <v>0.0005003984128530284</v>
+        <v>-0.007033642363963323</v>
       </c>
       <c r="H66">
-        <v>75.91701046340093</v>
+        <v>-3.109246577817797E-07</v>
       </c>
       <c r="I66">
-        <v>75.82659446642462</v>
+        <v>171.4270603640373</v>
       </c>
       <c r="J66">
-        <v>83.4807390392009</v>
+        <v>171.3630306959952</v>
       </c>
       <c r="K66">
-        <v>83.39388859602673</v>
+        <v>98.75535019423418</v>
       </c>
       <c r="L66">
-        <v>-0.003558207949539017</v>
+        <v>8.818135453328694E-05</v>
       </c>
       <c r="M66">
-        <v>439.3727165189503</v>
+        <v>0.5936882724959863</v>
       </c>
       <c r="N66">
-        <v>2.003180276175655E-25</v>
+        <v>0.0001989337014573517</v>
       </c>
       <c r="O66">
-        <v>-281.720427899179</v>
+        <v>-0.3376738781746061</v>
       </c>
       <c r="P66">
-        <v>-0.4623981423582945</v>
+        <v>-0.1629233199467273</v>
       </c>
     </row>
     <row r="67" spans="1:16">
       <c r="A67">
-        <v>15.01941638397542</v>
+        <v>395.2580859984504</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67">
-        <v>26.8292556215936</v>
+        <v>7.970254482932585</v>
       </c>
       <c r="D67">
-        <v>-0.001491840966995927</v>
+        <v>1.551093441176104E-05</v>
       </c>
       <c r="E67">
-        <v>0.0002549100499349298</v>
+        <v>0.0005346220957941419</v>
       </c>
       <c r="F67">
-        <v>-1.995372416725188</v>
+        <v>-1.902229071863976</v>
       </c>
       <c r="G67">
-        <v>0.0007319230745700741</v>
+        <v>-0.006635603505619162</v>
       </c>
       <c r="H67">
-        <v>76.61083517407528</v>
+        <v>8.398746372076246E-08</v>
       </c>
       <c r="I67">
-        <v>76.67591228483252</v>
+        <v>171.4277045237287</v>
       </c>
       <c r="J67">
-        <v>84.38182869155985</v>
+        <v>171.3775219643343</v>
       </c>
       <c r="K67">
-        <v>84.20825876198447</v>
+        <v>98.76968283265738</v>
       </c>
       <c r="L67">
-        <v>-0.002423878090414986</v>
+        <v>7.20263745884902E-05</v>
       </c>
       <c r="M67">
-        <v>439.5034026761299</v>
+        <v>0.420562868038233</v>
       </c>
       <c r="N67">
-        <v>-2.771650830179325E-30</v>
+        <v>0.0001982604817998707</v>
       </c>
       <c r="O67">
-        <v>-282.3991618850509</v>
+        <v>-0.2512006972994641</v>
       </c>
       <c r="P67">
-        <v>-0.6583232212184169</v>
+        <v>-0.1212009196221042</v>
       </c>
     </row>
     <row r="68" spans="1:16">
       <c r="A68">
-        <v>15.21415356732201</v>
+        <v>395.9256421285528</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="C68">
-        <v>27.08726181182552</v>
+        <v>7.76085776165798</v>
       </c>
       <c r="D68">
-        <v>-0.00111611589486981</v>
+        <v>1.504102035925825E-05</v>
       </c>
       <c r="E68">
-        <v>-0.001029550424399625</v>
+        <v>0.0004058358640371129</v>
       </c>
       <c r="F68">
-        <v>-1.998439550382097</v>
+        <v>-1.936150828262598</v>
       </c>
       <c r="G68">
-        <v>0.0006535240976610539</v>
+        <v>-0.006325713448382566</v>
       </c>
       <c r="H68">
-        <v>77.41591893271378</v>
+        <v>9.716438521626506E-07</v>
       </c>
       <c r="I68">
-        <v>77.36604057434529</v>
+        <v>171.4281258878046</v>
       </c>
       <c r="J68">
-        <v>85.25225262628889</v>
+        <v>171.3785875974138</v>
       </c>
       <c r="K68">
-        <v>84.95703433454239</v>
+        <v>98.77066047965519</v>
       </c>
       <c r="L68">
-        <v>-0.001240881674720904</v>
+        <v>5.863277957634517E-05</v>
       </c>
       <c r="M68">
-        <v>439.0300490728508</v>
+        <v>0.3058680980261133</v>
       </c>
       <c r="N68">
-        <v>1.574780678346522E-29</v>
+        <v>0.0001964599286752743</v>
       </c>
       <c r="O68">
-        <v>-281.8996399718433</v>
+        <v>-0.1873159399746704</v>
       </c>
       <c r="P68">
-        <v>-0.3343038851291994</v>
+        <v>-0.09037725187354977</v>
       </c>
     </row>
     <row r="69" spans="1:16">
       <c r="A69">
-        <v>15.40710306629226</v>
+        <v>396.6112412756376</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69">
-        <v>27.32895537111682</v>
+        <v>7.556263593442317</v>
       </c>
       <c r="D69">
-        <v>-0.0005858524395284717</v>
+        <v>1.389979795403131E-05</v>
       </c>
       <c r="E69">
-        <v>-0.001679553049499067</v>
+        <v>0.000308430666867994</v>
       </c>
       <c r="F69">
-        <v>-1.999981877029894</v>
+        <v>-1.968634560728888</v>
       </c>
       <c r="G69">
-        <v>0.0003889392242223858</v>
+        <v>-0.00608414715965624</v>
       </c>
       <c r="H69">
-        <v>78.04686464195264</v>
+        <v>3.221765016341848E-06</v>
       </c>
       <c r="I69">
-        <v>78.10011496271376</v>
+        <v>171.4284022068507</v>
       </c>
       <c r="J69">
-        <v>86.04696404102258</v>
+        <v>171.3769697587052</v>
       </c>
       <c r="K69">
-        <v>85.69178015169136</v>
+        <v>98.76899368055834</v>
       </c>
       <c r="L69">
-        <v>0.00047885976984989</v>
+        <v>4.759327134020422E-05</v>
       </c>
       <c r="M69">
-        <v>439.0291929333104</v>
+        <v>0.2265361824668302</v>
       </c>
       <c r="N69">
-        <v>-3.829987378389947E-31</v>
+        <v>0.0001893392485850571</v>
       </c>
       <c r="O69">
-        <v>-282.3165693347185</v>
+        <v>-0.1400124910182405</v>
       </c>
       <c r="P69">
-        <v>-0.5395691786072626</v>
+        <v>-0.06755391564618882</v>
       </c>
     </row>
     <row r="70" spans="1:16">
       <c r="A70">
-        <v>15.59840362962104</v>
+        <v>397.3154288634393</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="C70">
-        <v>27.55644293163924</v>
+        <v>7.356537110463023</v>
       </c>
       <c r="D70">
-        <v>3.199070130129252E-05</v>
+        <v>1.244348670121387E-05</v>
       </c>
       <c r="E70">
-        <v>-0.00149072459056563</v>
+        <v>0.0002346651002253361</v>
       </c>
       <c r="F70">
-        <v>-1.999986857351332</v>
+        <v>-2.000000048262731</v>
       </c>
       <c r="G70">
-        <v>8.264284133753508E-05</v>
+        <v>-0.005895617306052557</v>
       </c>
       <c r="H70">
-        <v>78.74533055573271</v>
+        <v>-2.952691669241955E-06</v>
       </c>
       <c r="I70">
-        <v>78.71558281461846</v>
+        <v>171.4285743810969</v>
       </c>
       <c r="J70">
-        <v>86.81777224625216</v>
+        <v>171.3763995832639</v>
       </c>
       <c r="K70">
-        <v>86.36455145499291</v>
+        <v>98.76839617254761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doesn't optimize on this version
</commit_message>
<xml_diff>
--- a/custom sim/two_track_out2.xlsx
+++ b/custom sim/two_track_out2.xlsx
@@ -483,7 +483,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.4025236678718991</v>
+        <v>29.99999739566411</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -492,3422 +492,3422 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>-1.923587485323732</v>
+        <v>-0.2702505563138138</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>171.428573986029</v>
+        <v>171.4280177052676</v>
       </c>
       <c r="I2">
-        <v>-2.557454950492511E-06</v>
+        <v>171.4283835692619</v>
       </c>
       <c r="J2">
-        <v>5.592879920384704</v>
+        <v>72.59644880647843</v>
       </c>
       <c r="K2">
-        <v>107.0518191062842</v>
+        <v>90.59754701633935</v>
       </c>
       <c r="L2">
-        <v>-0.008442906890839983</v>
+        <v>-0.0007008544648795109</v>
       </c>
       <c r="M2">
-        <v>0.001849342634680564</v>
+        <v>449.316120762934</v>
       </c>
       <c r="N2">
-        <v>-1.188450101141443</v>
+        <v>-4.303735218331349E-20</v>
       </c>
       <c r="O2">
-        <v>-43.42724043924721</v>
+        <v>-283.0678199056217</v>
       </c>
       <c r="P2">
-        <v>-20.80765885514819</v>
+        <v>-1.866704920067906</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3">
-        <v>13.50030028985811</v>
+        <v>0.175148236510452</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.3758859305097116</v>
+        <v>29.99999983056264</v>
       </c>
       <c r="D3">
-        <v>-0.009146453258830166</v>
+        <v>-0.0007553603927464459</v>
       </c>
       <c r="E3">
-        <v>-0.002840094275378657</v>
+        <v>0.005775513476068665</v>
       </c>
       <c r="F3">
-        <v>-2.000000026991795</v>
+        <v>-0.2700888252871915</v>
       </c>
       <c r="G3">
-        <v>-0.01992736453858513</v>
+        <v>0.0008699662100687607</v>
       </c>
       <c r="H3">
-        <v>171.4285707383771</v>
+        <v>85.57449085625431</v>
       </c>
       <c r="I3">
-        <v>55.45623919978623</v>
+        <v>86.42261887572441</v>
       </c>
       <c r="J3">
-        <v>0.03933852893697091</v>
+        <v>101.911935913443</v>
       </c>
       <c r="K3">
-        <v>101.1940606700598</v>
+        <v>93.88818366908896</v>
       </c>
       <c r="L3">
-        <v>0.01350520335297163</v>
+        <v>-0.02504570173229527</v>
       </c>
       <c r="M3">
-        <v>2.404275986633913</v>
+        <v>404.2397083497763</v>
       </c>
       <c r="N3">
-        <v>0.0001998491605094467</v>
+        <v>1.203251192425251E-27</v>
       </c>
       <c r="O3">
-        <v>172.6992316535219</v>
+        <v>-245.2490418743137</v>
       </c>
       <c r="P3">
-        <v>94.6351032206619</v>
+        <v>21.29130960883162</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4">
-        <v>27.09410522723888</v>
+        <v>0.3501486729923848</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.3970776190966772</v>
+        <v>29.9988015889761</v>
       </c>
       <c r="D4">
-        <v>0.02416015140907168</v>
+        <v>-0.00559082339246463</v>
       </c>
       <c r="E4">
-        <v>0.007127760551605367</v>
+        <v>-0.003262681252059567</v>
       </c>
       <c r="F4">
-        <v>-1.982222532411391</v>
+        <v>-0.2827516960506198</v>
       </c>
       <c r="G4">
-        <v>0.01198207239015201</v>
+        <v>0.001092901668211778</v>
       </c>
       <c r="H4">
-        <v>6.910984529323092E-07</v>
+        <v>85.78825623760189</v>
       </c>
       <c r="I4">
-        <v>71.16985477815466</v>
+        <v>85.09782003942341</v>
       </c>
       <c r="J4">
-        <v>35.85645322050225</v>
+        <v>103.7239749205084</v>
       </c>
       <c r="K4">
-        <v>134.642221313657</v>
+        <v>93.94209242061122</v>
       </c>
       <c r="L4">
-        <v>-0.007183289095877532</v>
+        <v>-0.05231688253363346</v>
       </c>
       <c r="M4">
-        <v>0.0007105472821708751</v>
+        <v>404.7353104071987</v>
       </c>
       <c r="N4">
-        <v>-2.611588034178653</v>
+        <v>-1.940005093046536E-27</v>
       </c>
       <c r="O4">
-        <v>-209.5803358827978</v>
+        <v>-263.9921329831768</v>
       </c>
       <c r="P4">
-        <v>-110.327168194697</v>
+        <v>39.06927319012095</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5">
-        <v>41.21219702908144</v>
+        <v>0.5251595317725035</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0.3480958008756005</v>
+        <v>29.99999963866599</v>
       </c>
       <c r="D5">
-        <v>-0.03112138228219068</v>
+        <v>-0.01079945548171086</v>
       </c>
       <c r="E5">
-        <v>-0.003701259158805437</v>
+        <v>-0.02050228251169342</v>
       </c>
       <c r="F5">
-        <v>-1.982028185292249</v>
+        <v>-0.3264813428942182</v>
       </c>
       <c r="G5">
-        <v>-0.004283101064455341</v>
+        <v>-0.0009704810072043052</v>
       </c>
       <c r="H5">
-        <v>171.4285734857922</v>
+        <v>85.4605259126847</v>
       </c>
       <c r="I5">
-        <v>171.4285735952785</v>
+        <v>86.10894944589667</v>
       </c>
       <c r="J5">
-        <v>18.5048155206608</v>
+        <v>103.4894607824712</v>
       </c>
       <c r="K5">
-        <v>112.6749464594002</v>
+        <v>94.13056251564815</v>
       </c>
       <c r="L5">
-        <v>0.01199820563138037</v>
+        <v>-0.04653400602082683</v>
       </c>
       <c r="M5">
-        <v>1.524565923907109</v>
+        <v>397.1658166988021</v>
       </c>
       <c r="N5">
-        <v>0.0001999828067136122</v>
+        <v>-2.943282834618596E-26</v>
       </c>
       <c r="O5">
-        <v>282.9648999281249</v>
+        <v>-250.7120530595055</v>
       </c>
       <c r="P5">
-        <v>172.286353954202</v>
+        <v>33.50820073452412</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6">
-        <v>55.50499235808775</v>
+        <v>0.7002007032934222</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.3873166245431029</v>
+        <v>29.99244363851315</v>
       </c>
       <c r="D6">
-        <v>0.04471729166097636</v>
+        <v>-0.01116894665144502</v>
       </c>
       <c r="E6">
-        <v>0.007221939080635714</v>
+        <v>-0.0368260356533487</v>
       </c>
       <c r="F6">
-        <v>-1.896014082180723</v>
+        <v>-0.4024800883557253</v>
       </c>
       <c r="G6">
-        <v>0.02395347815962818</v>
+        <v>-0.005992750146944469</v>
       </c>
       <c r="H6">
-        <v>-2.557669447712158E-06</v>
+        <v>85.67282798612499</v>
       </c>
       <c r="I6">
-        <v>152.9130860348284</v>
+        <v>85.41484272524832</v>
       </c>
       <c r="J6">
-        <v>46.4689003087034</v>
+        <v>103.3698978150644</v>
       </c>
       <c r="K6">
-        <v>134.3430030187501</v>
+        <v>93.84390508083925</v>
       </c>
       <c r="L6">
-        <v>-0.0131341041674196</v>
+        <v>-0.0523431534041934</v>
       </c>
       <c r="M6">
-        <v>0.0003711714419971881</v>
+        <v>402.994166745402</v>
       </c>
       <c r="N6">
-        <v>-4.6852767963984</v>
+        <v>4.581089132841495E-27</v>
       </c>
       <c r="O6">
-        <v>-299.294826222171</v>
+        <v>-264.3889453881312</v>
       </c>
       <c r="P6">
-        <v>-176.6703432633724</v>
+        <v>43.24325580077888</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7">
-        <v>70.6289001077414</v>
+        <v>0.8752634688893306</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.309872689562307</v>
+        <v>29.99999524687372</v>
       </c>
       <c r="D7">
-        <v>-0.05764679377913462</v>
+        <v>-0.009708194299310373</v>
       </c>
       <c r="E7">
-        <v>-0.004125766939543165</v>
+        <v>-0.05411581826598051</v>
       </c>
       <c r="F7">
-        <v>-1.886468028810635</v>
+        <v>-0.5093286506710499</v>
       </c>
       <c r="G7">
-        <v>-0.006335240316035612</v>
+        <v>-0.01396053627372621</v>
       </c>
       <c r="H7">
-        <v>171.4285740170393</v>
+        <v>85.41117144742898</v>
       </c>
       <c r="I7">
-        <v>171.4285673992215</v>
+        <v>86.01299583954764</v>
       </c>
       <c r="J7">
-        <v>26.65330585028306</v>
+        <v>101.7448627247406</v>
       </c>
       <c r="K7">
-        <v>108.0286805605204</v>
+        <v>94.09250860909573</v>
       </c>
       <c r="L7">
-        <v>0.01093248834956401</v>
+        <v>-0.08464046098628504</v>
       </c>
       <c r="M7">
-        <v>1.08666001613401</v>
+        <v>383.5780761218104</v>
       </c>
       <c r="N7">
-        <v>0.0001999860629717998</v>
+        <v>-8.96348007022494E-28</v>
       </c>
       <c r="O7">
-        <v>306.8692648324996</v>
+        <v>-252.1065821221995</v>
       </c>
       <c r="P7">
-        <v>205.3954407046986</v>
+        <v>67.67169328388906</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8">
-        <v>86.1260661012579</v>
+        <v>1.050354612257053</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0.3683472034671609</v>
+        <v>29.99999876022166</v>
       </c>
       <c r="D8">
-        <v>0.07002561595617632</v>
+        <v>-0.009076291498923411</v>
       </c>
       <c r="E8">
-        <v>0.007068801122846744</v>
+        <v>-0.07791734757747674</v>
       </c>
       <c r="F8">
-        <v>-1.820963208326224</v>
+        <v>-0.6622771227168154</v>
       </c>
       <c r="G8">
-        <v>0.01935618492382619</v>
+        <v>-0.02550188823884381</v>
       </c>
       <c r="H8">
-        <v>-2.611226585013112E-06</v>
+        <v>85.2629277737649</v>
       </c>
       <c r="I8">
-        <v>124.2263322672908</v>
+        <v>85.37113961025112</v>
       </c>
       <c r="J8">
-        <v>50.78558340361215</v>
+        <v>92.37855644397554</v>
       </c>
       <c r="K8">
-        <v>124.1584662633507</v>
+        <v>94.22601207606471</v>
       </c>
       <c r="L8">
-        <v>-0.01363906414830139</v>
+        <v>-0.04841882778277753</v>
       </c>
       <c r="M8">
-        <v>0.0003635789449264077</v>
+        <v>391.8888313349107</v>
       </c>
       <c r="N8">
-        <v>-4.773140342545753</v>
+        <v>1.445655997706762E-24</v>
       </c>
       <c r="O8">
-        <v>-314.6825223289686</v>
+        <v>-258.0479333907703</v>
       </c>
       <c r="P8">
-        <v>-205.2401566963525</v>
+        <v>64.76934810977976</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9">
-        <v>102.5586452878137</v>
+        <v>1.225499757483865</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0.2741733946274609</v>
+        <v>29.98629861262248</v>
       </c>
       <c r="D9">
-        <v>-0.0835073737620311</v>
+        <v>-0.00256449402259163</v>
       </c>
       <c r="E9">
-        <v>-0.003968759051152925</v>
+        <v>-0.0925764795562182</v>
       </c>
       <c r="F9">
-        <v>-1.840376654937489</v>
+        <v>-0.8644275401994517</v>
       </c>
       <c r="G9">
-        <v>-0.01221631890677186</v>
+        <v>-0.04050788773798109</v>
       </c>
       <c r="H9">
-        <v>171.4285740774316</v>
+        <v>85.52810541603233</v>
       </c>
       <c r="I9">
-        <v>100.9676512674029</v>
+        <v>86.20621549735269</v>
       </c>
       <c r="J9">
-        <v>32.14046123258811</v>
+        <v>90.05345733001154</v>
       </c>
       <c r="K9">
-        <v>99.10458882919917</v>
+        <v>94.89804494969685</v>
       </c>
       <c r="L9">
-        <v>0.01028717453065245</v>
+        <v>0.04141014888834691</v>
       </c>
       <c r="M9">
-        <v>0.8125498385202237</v>
+        <v>435.6938360112447</v>
       </c>
       <c r="N9">
-        <v>0.0001999884421727933</v>
+        <v>3.397690724693333E-28</v>
       </c>
       <c r="O9">
-        <v>295.6488980037444</v>
+        <v>-252.4305730012158</v>
       </c>
       <c r="P9">
-        <v>207.3508081258908</v>
+        <v>-2.55878366849068</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10">
-        <v>119.4372438025613</v>
+        <v>1.400688136228056</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0.348446407457455</v>
+        <v>30.00000007969707</v>
       </c>
       <c r="D10">
-        <v>0.09500605982315469</v>
+        <v>0.01670841275708275</v>
       </c>
       <c r="E10">
-        <v>0.006550475281539251</v>
+        <v>-0.07404306037784376</v>
       </c>
       <c r="F10">
-        <v>-1.811515325952283</v>
+        <v>-1.074194612272204</v>
       </c>
       <c r="G10">
-        <v>0.01199838432866765</v>
+        <v>-0.05513820570028236</v>
       </c>
       <c r="H10">
-        <v>-2.648850144351273E-06</v>
+        <v>85.36326045051545</v>
       </c>
       <c r="I10">
-        <v>42.11953792437455</v>
+        <v>85.54569530579924</v>
       </c>
       <c r="J10">
-        <v>52.07720324443369</v>
+        <v>94.95612502138002</v>
       </c>
       <c r="K10">
-        <v>112.3939510164194</v>
+        <v>98.68606607510506</v>
       </c>
       <c r="L10">
-        <v>-0.01276187022363004</v>
+        <v>0.03499138696120417</v>
       </c>
       <c r="M10">
-        <v>0.0004657674008989858</v>
+        <v>419.8284899575024</v>
       </c>
       <c r="N10">
-        <v>-3.810925854385568</v>
+        <v>-8.498488252749848E-28</v>
       </c>
       <c r="O10">
-        <v>-300.638014615855</v>
+        <v>-260.2069833423311</v>
       </c>
       <c r="P10">
-        <v>-206.2067003091486</v>
+        <v>31.20546562955481</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11">
-        <v>137.2956881221491</v>
+        <v>1.575807398538395</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0.2432973981317768</v>
+        <v>29.99999935710484</v>
       </c>
       <c r="D11">
-        <v>-0.1077259475834896</v>
+        <v>0.02474974397563092</v>
       </c>
       <c r="E11">
-        <v>-0.003178181679021966</v>
+        <v>-0.05839563646757716</v>
       </c>
       <c r="F11">
-        <v>-1.862095585250477</v>
+        <v>-1.283714728661302</v>
       </c>
       <c r="G11">
-        <v>-0.01763443214393483</v>
+        <v>-0.06671870525157461</v>
       </c>
       <c r="H11">
-        <v>171.428574089508</v>
+        <v>85.6783545595397</v>
       </c>
       <c r="I11">
-        <v>39.75443197357352</v>
+        <v>86.11039198869005</v>
       </c>
       <c r="J11">
-        <v>35.92085714001773</v>
+        <v>93.58315209973553</v>
       </c>
       <c r="K11">
-        <v>90.54014521880822</v>
+        <v>106.1526174173784</v>
       </c>
       <c r="L11">
-        <v>0.01034660684897255</v>
+        <v>0.06612957526612506</v>
       </c>
       <c r="M11">
-        <v>0.5867728999864386</v>
+        <v>602.5223596407133</v>
       </c>
       <c r="N11">
-        <v>0.0001999897121510085</v>
+        <v>-1.003094263682719E-26</v>
       </c>
       <c r="O11">
-        <v>279.8518285477558</v>
+        <v>-156.4814604077547</v>
       </c>
       <c r="P11">
-        <v>200.403803047832</v>
+        <v>-35.85592561121008</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12">
-        <v>155.6058664413082</v>
+        <v>1.751514699071341</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0.3306704419765834</v>
+        <v>29.78046720144491</v>
       </c>
       <c r="D12">
-        <v>0.1190956446651706</v>
+        <v>0.03963229130727886</v>
       </c>
       <c r="E12">
-        <v>0.005652149574822848</v>
+        <v>-0.03692606382483118</v>
       </c>
       <c r="F12">
-        <v>-1.860896014627843</v>
+        <v>-1.48682977130751</v>
       </c>
       <c r="G12">
-        <v>0.006838408287800813</v>
+        <v>-0.07494811591239135</v>
       </c>
       <c r="H12">
-        <v>-2.644852230977505E-06</v>
+        <v>84.80847347443027</v>
       </c>
       <c r="I12">
-        <v>4.4939003124283E-06</v>
+        <v>84.87367933722267</v>
       </c>
       <c r="J12">
-        <v>49.58864315989902</v>
+        <v>144.1261167807237</v>
       </c>
       <c r="K12">
-        <v>100.9450379392323</v>
+        <v>155.2172238812166</v>
       </c>
       <c r="L12">
-        <v>-0.01118138088745468</v>
+        <v>0.1080290974616526</v>
       </c>
       <c r="M12">
-        <v>0.0007276294021526524</v>
+        <v>-4.02182987857733E-26</v>
       </c>
       <c r="N12">
-        <v>-2.504703120999076</v>
+        <v>-0.0002382656986221379</v>
       </c>
       <c r="O12">
-        <v>-283.4349036461788</v>
+        <v>-212.6353441050444</v>
       </c>
       <c r="P12">
-        <v>-198.347993369127</v>
+        <v>-2.115484282094079</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13">
-        <v>174.8705402406503</v>
+        <v>1.928533916696793</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0.2181416187822255</v>
+        <v>29.58636800451441</v>
       </c>
       <c r="D13">
-        <v>-0.1303072562652417</v>
+        <v>0.05198737876893288</v>
       </c>
       <c r="E13">
-        <v>-0.002811659095833143</v>
+        <v>-0.009316364016207605</v>
       </c>
       <c r="F13">
-        <v>-1.924758861120675</v>
+        <v>-1.646705559141833</v>
       </c>
       <c r="G13">
-        <v>-0.01919774733012335</v>
+        <v>-0.079189460141976</v>
       </c>
       <c r="H13">
-        <v>171.4285740670998</v>
+        <v>84.36464466957358</v>
       </c>
       <c r="I13">
-        <v>32.89205036648492</v>
+        <v>84.50027406909025</v>
       </c>
       <c r="J13">
-        <v>37.32033605657825</v>
+        <v>92.39613089078176</v>
       </c>
       <c r="K13">
-        <v>84.21569039773586</v>
+        <v>105.9985875005506</v>
       </c>
       <c r="L13">
-        <v>0.01014406456756129</v>
+        <v>0.125055788493705</v>
       </c>
       <c r="M13">
-        <v>0.04884707979865765</v>
+        <v>358.7102237865072</v>
       </c>
       <c r="N13">
-        <v>0.0001999898061446215</v>
+        <v>1.763242668763301E-27</v>
       </c>
       <c r="O13">
-        <v>265.7252839472441</v>
+        <v>-198.1511343810747</v>
       </c>
       <c r="P13">
-        <v>192.0209892855251</v>
+        <v>-25.67060757642481</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14">
-        <v>194.5708491398933</v>
+        <v>2.106471973778904</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0.3153452456384909</v>
+        <v>29.44312662709868</v>
       </c>
       <c r="D14">
-        <v>0.1413529311354088</v>
+        <v>0.05392145412454036</v>
       </c>
       <c r="E14">
-        <v>0.005102029399164593</v>
+        <v>0.02951284708389866</v>
       </c>
       <c r="F14">
-        <v>-1.933491280951562</v>
+        <v>-1.780294036945668</v>
       </c>
       <c r="G14">
-        <v>0.004849643679055799</v>
+        <v>-0.07733963114756436</v>
       </c>
       <c r="H14">
-        <v>-2.634802071011128E-06</v>
+        <v>83.93184197797147</v>
       </c>
       <c r="I14">
-        <v>3.259514865542934E-05</v>
+        <v>83.72652645860553</v>
       </c>
       <c r="J14">
-        <v>40.09997527399352</v>
+        <v>95.4105724811533</v>
       </c>
       <c r="K14">
-        <v>85.45314163150074</v>
+        <v>109.3552215878401</v>
       </c>
       <c r="L14">
-        <v>-0.01028656772373162</v>
+        <v>0.1399931318186446</v>
       </c>
       <c r="M14">
-        <v>0.0009849736797253276</v>
+        <v>332.4299846781488</v>
       </c>
       <c r="N14">
-        <v>-1.733198907526684</v>
+        <v>1.742212466640867E-26</v>
       </c>
       <c r="O14">
-        <v>-266.8581442464447</v>
+        <v>-201.9918137635009</v>
       </c>
       <c r="P14">
-        <v>-188.6696935025203</v>
+        <v>-32.03204122763687</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15">
-        <v>215.241035636062</v>
+        <v>2.285254239181182</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0.2172318002830219</v>
+        <v>29.3029106111724</v>
       </c>
       <c r="D15">
-        <v>-0.1517266841022214</v>
+        <v>0.0506311188972042</v>
       </c>
       <c r="E15">
-        <v>-0.001359309453988036</v>
+        <v>0.06772207249900106</v>
       </c>
       <c r="F15">
-        <v>-2.000000047124283</v>
+        <v>-1.88922668367108</v>
       </c>
       <c r="G15">
-        <v>-0.01915642205621851</v>
+        <v>-0.06864072030209249</v>
       </c>
       <c r="H15">
-        <v>171.4285740656412</v>
+        <v>83.55584881772363</v>
       </c>
       <c r="I15">
-        <v>60.34250758024622</v>
+        <v>83.28289370661173</v>
       </c>
       <c r="J15">
-        <v>30.17447759289516</v>
+        <v>93.79356953687916</v>
       </c>
       <c r="K15">
-        <v>71.83643069055907</v>
+        <v>108.1983496077264</v>
       </c>
       <c r="L15">
-        <v>0.01105248700126392</v>
+        <v>0.1423112275103812</v>
       </c>
       <c r="M15">
-        <v>0.00466052912367589</v>
+        <v>329.907777830612</v>
       </c>
       <c r="N15">
-        <v>0.0001999893984333511</v>
+        <v>2.76763683728454E-27</v>
       </c>
       <c r="O15">
-        <v>254.4952117319014</v>
+        <v>-209.7973436063861</v>
       </c>
       <c r="P15">
-        <v>185.1235313495935</v>
+        <v>-35.79826427394634</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16">
-        <v>234.2600612864648</v>
+        <v>2.464797532383591</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0.3355937445858249</v>
+        <v>29.18972401618702</v>
       </c>
       <c r="D16">
-        <v>0.1635592339564484</v>
+        <v>0.04077829581824167</v>
       </c>
       <c r="E16">
-        <v>0.004025959163593364</v>
+        <v>0.1054925840237673</v>
       </c>
       <c r="F16">
-        <v>-2.000000049238839</v>
+        <v>-1.969198158422217</v>
       </c>
       <c r="G16">
-        <v>0.007181053429153064</v>
+        <v>-0.05308098356623071</v>
       </c>
       <c r="H16">
-        <v>-2.63705673708372E-06</v>
+        <v>83.27617455107935</v>
       </c>
       <c r="I16">
-        <v>60.82563948865756</v>
+        <v>82.73570952619457</v>
       </c>
       <c r="J16">
-        <v>26.85014957610545</v>
+        <v>90.23952510250032</v>
       </c>
       <c r="K16">
-        <v>71.16344417470708</v>
+        <v>104.5485520835698</v>
       </c>
       <c r="L16">
-        <v>0.0005381018871598624</v>
+        <v>0.5734386587331688</v>
       </c>
       <c r="M16">
-        <v>0.002593121483481037</v>
+        <v>412.5678104075254</v>
       </c>
       <c r="N16">
-        <v>-0.1334470676374061</v>
+        <v>2.279472509395758E-27</v>
       </c>
       <c r="O16">
-        <v>-258.8158308891711</v>
+        <v>-23.39852531058329</v>
       </c>
       <c r="P16">
-        <v>-184.8240808970149</v>
+        <v>-71.71965438736433</v>
       </c>
     </row>
     <row r="17" spans="1:16">
       <c r="A17">
-        <v>253.5832688564677</v>
+        <v>2.646304900532903</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>0.2618695535562728</v>
+        <v>28.64392812222416</v>
       </c>
       <c r="D17">
-        <v>-0.1622469234658728</v>
+        <v>0.03254825729389917</v>
       </c>
       <c r="E17">
-        <v>-0.002487856170210536</v>
+        <v>0.1349440177524654</v>
       </c>
       <c r="F17">
-        <v>-1.956241394345466</v>
+        <v>-1.999999810693658</v>
       </c>
       <c r="G17">
-        <v>0.008770027441980318</v>
+        <v>-0.03113979509410816</v>
       </c>
       <c r="H17">
-        <v>171.428574344364</v>
+        <v>65.71787633436971</v>
       </c>
       <c r="I17">
-        <v>120.5437313802238</v>
+        <v>66.16579388110144</v>
       </c>
       <c r="J17">
-        <v>25.29774045053272</v>
+        <v>121.5395205622169</v>
       </c>
       <c r="K17">
-        <v>68.82992519743624</v>
+        <v>128.4402575183722</v>
       </c>
       <c r="L17">
-        <v>0.008960281225997589</v>
+        <v>0.1321209100411237</v>
       </c>
       <c r="M17">
-        <v>0.00271460981676947</v>
+        <v>0.001939280818943257</v>
       </c>
       <c r="N17">
-        <v>0.0001999970018960722</v>
+        <v>7.66398330006273E-25</v>
       </c>
       <c r="O17">
-        <v>250.0632659773441</v>
+        <v>-68.40302639663129</v>
       </c>
       <c r="P17">
-        <v>181.6915601401241</v>
+        <v>-57.67629934326195</v>
       </c>
     </row>
     <row r="18" spans="1:16">
       <c r="A18">
-        <v>269.1871442783465</v>
+        <v>2.830603326154852</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>0.4114353482725129</v>
+        <v>28.34394403757355</v>
       </c>
       <c r="D18">
-        <v>0.1717321646737955</v>
+        <v>0.02286746195829881</v>
       </c>
       <c r="E18">
-        <v>0.004978138829117581</v>
+        <v>0.1716769414562861</v>
       </c>
       <c r="F18">
-        <v>-1.829222331675156</v>
+        <v>-1.941931444187555</v>
       </c>
       <c r="G18">
-        <v>0.02992207522772276</v>
+        <v>-0.003014252561297861</v>
       </c>
       <c r="H18">
-        <v>-2.849877287823442E-06</v>
+        <v>94.09696873531539</v>
       </c>
       <c r="I18">
-        <v>-2.13884299098005E-06</v>
+        <v>91.87932625864471</v>
       </c>
       <c r="J18">
-        <v>26.73780922235307</v>
+        <v>79.99472038654166</v>
       </c>
       <c r="K18">
-        <v>69.20319530570514</v>
+        <v>79.80041194766807</v>
       </c>
       <c r="L18">
-        <v>0.00815364843837431</v>
+        <v>0.121119769646981</v>
       </c>
       <c r="M18">
-        <v>0.002636220285335493</v>
+        <v>-3.279916929011744E-24</v>
       </c>
       <c r="N18">
-        <v>0.000199991225148401</v>
+        <v>-0.00294914023710311</v>
       </c>
       <c r="O18">
-        <v>-253.6365632449449</v>
+        <v>256.187546612053</v>
       </c>
       <c r="P18">
-        <v>-182.4214296008324</v>
+        <v>-100.8695702955812</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19">
-        <v>284.8086591298096</v>
+        <v>3.018736632587401</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>0.3702912562479955</v>
+        <v>27.52529179726817</v>
       </c>
       <c r="D19">
-        <v>-0.1618283944874649</v>
+        <v>0.02043185750597484</v>
       </c>
       <c r="E19">
-        <v>0.00169021460883954</v>
+        <v>0.2209513005327868</v>
       </c>
       <c r="F19">
-        <v>-1.595913021717977</v>
+        <v>-1.74833029082763</v>
       </c>
       <c r="G19">
-        <v>0.0498148844357296</v>
+        <v>0.03393054705061835</v>
       </c>
       <c r="H19">
-        <v>171.4285743461716</v>
+        <v>67.32405371162919</v>
       </c>
       <c r="I19">
-        <v>88.78309554005817</v>
+        <v>67.77763150691243</v>
       </c>
       <c r="J19">
-        <v>26.11769188959753</v>
+        <v>78.52319294319351</v>
       </c>
       <c r="K19">
-        <v>68.20060876669073</v>
+        <v>79.54585574299591</v>
       </c>
       <c r="L19">
-        <v>0.0117873395639554</v>
+        <v>0.1191978778303996</v>
       </c>
       <c r="M19">
-        <v>0.004295489607545928</v>
+        <v>503.9356604045615</v>
       </c>
       <c r="N19">
-        <v>0.0001999968699617555</v>
+        <v>5.318210895122265E-28</v>
       </c>
       <c r="O19">
-        <v>250.0615280100172</v>
+        <v>-332.7536131185527</v>
       </c>
       <c r="P19">
-        <v>182.4272166150001</v>
+        <v>-103.0542606003206</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20">
-        <v>295.7725276897305</v>
+        <v>3.209489361479243</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>0.656522460249566</v>
+        <v>27.64652984520336</v>
       </c>
       <c r="D20">
-        <v>0.1734211685786633</v>
+        <v>-0.008330811044512188</v>
       </c>
       <c r="E20">
-        <v>0.00669865785399826</v>
+        <v>0.2380682547519472</v>
       </c>
       <c r="F20">
-        <v>-1.226376666578598</v>
+        <v>-1.428809801732096</v>
       </c>
       <c r="G20">
-        <v>0.0781407524891182</v>
+        <v>0.07796339368739101</v>
       </c>
       <c r="H20">
-        <v>-2.889993843088816E-06</v>
+        <v>87.52022694410493</v>
       </c>
       <c r="I20">
-        <v>-2.686520688912521E-06</v>
+        <v>83.43484896976381</v>
       </c>
       <c r="J20">
-        <v>15.72786600503182</v>
+        <v>102.2377175346772</v>
       </c>
       <c r="K20">
-        <v>65.78688326562006</v>
+        <v>85.58423591373686</v>
       </c>
       <c r="L20">
-        <v>0.01492236708512812</v>
+        <v>0.09087146402773645</v>
       </c>
       <c r="M20">
-        <v>0.00605690987693816</v>
+        <v>4.129029810154228E-30</v>
       </c>
       <c r="N20">
-        <v>0.0001999853523934024</v>
+        <v>-340.5057285290218</v>
       </c>
       <c r="O20">
-        <v>-254.7295076785167</v>
+        <v>262.4399918949118</v>
       </c>
       <c r="P20">
-        <v>-183.9055357435065</v>
+        <v>-171.8350549962871</v>
       </c>
     </row>
     <row r="21" spans="1:16">
       <c r="A21">
-        <v>305.4770220440475</v>
+        <v>3.40324726950419</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0.4587012334363274</v>
+        <v>26.75426692319439</v>
       </c>
       <c r="D21">
-        <v>-0.1550155039255171</v>
+        <v>-0.01524613692329107</v>
       </c>
       <c r="E21">
-        <v>0.003356509518256488</v>
+        <v>0.2760300333001882</v>
       </c>
       <c r="F21">
-        <v>-0.6745565889967078</v>
+        <v>-0.9511877451839259</v>
       </c>
       <c r="G21">
-        <v>0.1146179938937624</v>
+        <v>0.1279110609036712</v>
       </c>
       <c r="H21">
-        <v>171.4285743590031</v>
+        <v>68.32492373140883</v>
       </c>
       <c r="I21">
-        <v>113.6141856175414</v>
+        <v>69.4524457427579</v>
       </c>
       <c r="J21">
-        <v>18.59209596466039</v>
+        <v>85.56676236461699</v>
       </c>
       <c r="K21">
-        <v>70.26780160428</v>
+        <v>75.72387214062176</v>
       </c>
       <c r="L21">
-        <v>0.01200226614513192</v>
+        <v>0.106271284886993</v>
       </c>
       <c r="M21">
-        <v>0.01100641330067549</v>
+        <v>7.00789265528821E-05</v>
       </c>
       <c r="N21">
-        <v>0.0001999966264942684</v>
+        <v>-1.17434611415472E-24</v>
       </c>
       <c r="O21">
-        <v>253.419809273886</v>
+        <v>-106.3855923017031</v>
       </c>
       <c r="P21">
-        <v>184.6751269290639</v>
+        <v>-207.2497389191921</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="A22">
-        <v>314.4846013004699</v>
+        <v>3.604119813775911</v>
       </c>
       <c r="B22">
         <v>0.003183098861837901</v>
       </c>
       <c r="C22">
-        <v>0.888680728703259</v>
+        <v>26.00634421883393</v>
       </c>
       <c r="D22">
-        <v>0.1661144116921349</v>
+        <v>-0.028085495899735</v>
       </c>
       <c r="E22">
-        <v>0.01033063794965093</v>
+        <v>0.2764568842117314</v>
       </c>
       <c r="F22">
-        <v>0.01230785083917473</v>
+        <v>-0.2760139041835133</v>
       </c>
       <c r="G22">
-        <v>0.1271137204221079</v>
+        <v>0.1666787013563632</v>
       </c>
       <c r="H22">
-        <v>-2.921930451875139E-06</v>
+        <v>81.43306235505052</v>
       </c>
       <c r="I22">
-        <v>-2.777202218570391E-06</v>
+        <v>77.1717678403068</v>
       </c>
       <c r="J22">
-        <v>4.596166679722756</v>
+        <v>72.85539721410859</v>
       </c>
       <c r="K22">
-        <v>67.19869455017742</v>
+        <v>75.59838168285037</v>
       </c>
       <c r="L22">
-        <v>0.02188793713707414</v>
+        <v>0.07135646548253842</v>
       </c>
       <c r="M22">
-        <v>0.02649208092763519</v>
+        <v>-9.544694409049545E-30</v>
       </c>
       <c r="N22">
-        <v>0.0001999194820420282</v>
+        <v>-1335.892709540615</v>
       </c>
       <c r="O22">
-        <v>-261.0023984752552</v>
+        <v>327.0166767702015</v>
       </c>
       <c r="P22">
-        <v>-188.7108235847481</v>
+        <v>-169.2842546171157</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="A23">
-        <v>321.4890358289551</v>
+        <v>3.813986636381685</v>
       </c>
       <c r="B23">
         <v>0.009708451528605597</v>
       </c>
       <c r="C23">
-        <v>0.6154758125602243</v>
+        <v>24.45368675157986</v>
       </c>
       <c r="D23">
-        <v>-0.138666585104283</v>
+        <v>-0.03880062472196966</v>
       </c>
       <c r="E23">
-        <v>0.006388057961833128</v>
+        <v>0.3122155920487815</v>
       </c>
       <c r="F23">
-        <v>0.7686169701497171</v>
+        <v>0.46861965900346</v>
       </c>
       <c r="G23">
-        <v>0.1297141077183976</v>
+        <v>0.1775396088560895</v>
       </c>
       <c r="H23">
-        <v>171.4285743805366</v>
+        <v>60.42025166434669</v>
       </c>
       <c r="I23">
-        <v>134.3447457761123</v>
+        <v>59.92394348416438</v>
       </c>
       <c r="J23">
-        <v>9.327762002679201</v>
+        <v>46.18691910975839</v>
       </c>
       <c r="K23">
-        <v>74.57505498767885</v>
+        <v>67.49396245266546</v>
       </c>
       <c r="L23">
-        <v>0.01282677856362168</v>
+        <v>0.08093771193798818</v>
       </c>
       <c r="M23">
-        <v>1.684952743416839</v>
+        <v>4.177142603132374E-05</v>
       </c>
       <c r="N23">
-        <v>0.0001999962208929666</v>
+        <v>-2.047357458758156E-25</v>
       </c>
       <c r="O23">
-        <v>261.3313800531331</v>
+        <v>-137.4727861493442</v>
       </c>
       <c r="P23">
-        <v>189.966028143527</v>
+        <v>-223.9283384094417</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24">
-        <v>328.2314819470565</v>
+        <v>4.031927964921906</v>
       </c>
       <c r="B24">
         <v>0.01639295913846519</v>
       </c>
       <c r="C24">
-        <v>1.033089376885512</v>
+        <v>23.54491119809519</v>
       </c>
       <c r="D24">
-        <v>0.149180665874344</v>
+        <v>-0.04880884224298262</v>
       </c>
       <c r="E24">
-        <v>0.01815686256805184</v>
+        <v>0.306428747886173</v>
       </c>
       <c r="F24">
-        <v>1.348164390776472</v>
+        <v>1.1270084947225</v>
       </c>
       <c r="G24">
-        <v>0.07461102117586228</v>
+        <v>0.1594283793624685</v>
       </c>
       <c r="H24">
-        <v>-2.951966116626071E-06</v>
+        <v>76.05838811512807</v>
       </c>
       <c r="I24">
-        <v>-1.871614698420237E-06</v>
+        <v>72.31711816135441</v>
       </c>
       <c r="J24">
-        <v>0.09678923606466314</v>
+        <v>64.88454155099977</v>
       </c>
       <c r="K24">
-        <v>81.1227813880764</v>
+        <v>69.35343767710854</v>
       </c>
       <c r="L24">
-        <v>0.03291373387411867</v>
+        <v>0.06217117779341732</v>
       </c>
       <c r="M24">
-        <v>0.03558776008919132</v>
+        <v>-1.121288683062752E-28</v>
       </c>
       <c r="N24">
-        <v>0.0001989843292765865</v>
+        <v>-339.9507502921666</v>
       </c>
       <c r="O24">
-        <v>-275.3045187253791</v>
+        <v>275.3206488217727</v>
       </c>
       <c r="P24">
-        <v>-198.7228724399485</v>
+        <v>-193.6760403331835</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c r="A25">
-        <v>333.7952521358886</v>
+        <v>4.254212962298838</v>
       </c>
       <c r="B25">
         <v>0.01986760647169749</v>
       </c>
       <c r="C25">
-        <v>0.79381099390087</v>
+        <v>22.59126197695183</v>
       </c>
       <c r="D25">
-        <v>-0.1081914460731947</v>
+        <v>-0.05467298210836744</v>
       </c>
       <c r="E25">
-        <v>0.01253052892215573</v>
+        <v>0.3435125175454988</v>
       </c>
       <c r="F25">
-        <v>1.757522423515591</v>
+        <v>1.594959641935798</v>
       </c>
       <c r="G25">
-        <v>0.04854325114322183</v>
+        <v>0.1273950904415034</v>
       </c>
       <c r="H25">
-        <v>171.428574386137</v>
+        <v>56.388549796456</v>
       </c>
       <c r="I25">
-        <v>171.4285714467678</v>
+        <v>56.63439290133422</v>
       </c>
       <c r="J25">
-        <v>1.301308841704538</v>
+        <v>60.96788944995595</v>
       </c>
       <c r="K25">
-        <v>82.91764999928708</v>
+        <v>64.51840229927424</v>
       </c>
       <c r="L25">
-        <v>0.01765796195142317</v>
+        <v>0.07148982424466999</v>
       </c>
       <c r="M25">
-        <v>16.84390559239931</v>
+        <v>4.124450162148068E-05</v>
       </c>
       <c r="N25">
-        <v>0.0001999956203532667</v>
+        <v>-4.964718211583831E-24</v>
       </c>
       <c r="O25">
-        <v>269.779755455377</v>
+        <v>-144.333003941144</v>
       </c>
       <c r="P25">
-        <v>193.3878960471683</v>
+        <v>-237.1809739169186</v>
       </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26">
-        <v>339.0810327987595</v>
+        <v>4.482652804149417</v>
       </c>
       <c r="B26">
         <v>0.02</v>
       </c>
       <c r="C26">
-        <v>1.118019419921428</v>
+        <v>21.85315022846399</v>
       </c>
       <c r="D26">
-        <v>0.1222204094400906</v>
+        <v>-0.05990869498501382</v>
       </c>
       <c r="E26">
-        <v>0.05244359118300083</v>
+        <v>0.3261467804699089</v>
       </c>
       <c r="F26">
-        <v>1.891270765280587</v>
+        <v>1.876354003335981</v>
       </c>
       <c r="G26">
-        <v>-0.01422445674307088</v>
+        <v>0.09894187404917255</v>
       </c>
       <c r="H26">
-        <v>-2.958332313885664E-06</v>
+        <v>70.34173864295875</v>
       </c>
       <c r="I26">
-        <v>103.428846709922</v>
+        <v>66.02293561445649</v>
       </c>
       <c r="J26">
-        <v>54.99045067199155</v>
+        <v>62.22500730921784</v>
       </c>
       <c r="K26">
-        <v>159.8264313210843</v>
+        <v>63.58001218990383</v>
       </c>
       <c r="L26">
-        <v>0.04858570872906419</v>
+        <v>0.05567684862949855</v>
       </c>
       <c r="M26">
-        <v>1.393607267550474E-05</v>
+        <v>-2.669437567255827E-28</v>
       </c>
       <c r="N26">
-        <v>-50.59488761407561</v>
+        <v>-285.8759741480189</v>
       </c>
       <c r="O26">
-        <v>-305.9030366082042</v>
+        <v>258.0428116068421</v>
       </c>
       <c r="P26">
-        <v>-211.6377623197678</v>
+        <v>-204.0327083042688</v>
       </c>
     </row>
     <row r="27" spans="1:16">
       <c r="A27">
-        <v>343.6838936747593</v>
+        <v>4.718413167775238</v>
       </c>
       <c r="B27">
         <v>0.02</v>
       </c>
       <c r="C27">
-        <v>1.058329766453057</v>
+        <v>20.9587226103786</v>
       </c>
       <c r="D27">
-        <v>-0.05690972704156464</v>
+        <v>-0.06397206409210804</v>
       </c>
       <c r="E27">
-        <v>0.01802489696765177</v>
+        <v>0.3616505122086126</v>
       </c>
       <c r="F27">
-        <v>2.000000049198159</v>
+        <v>1.999999890945066</v>
       </c>
       <c r="G27">
-        <v>0.0003179395310395035</v>
+        <v>0.07501339881310645</v>
       </c>
       <c r="H27">
-        <v>171.428574392333</v>
+        <v>52.74375469392419</v>
       </c>
       <c r="I27">
-        <v>-1.130636519702664E-06</v>
+        <v>53.36088471995214</v>
       </c>
       <c r="J27">
-        <v>0.02520905350446062</v>
+        <v>57.17252085368987</v>
       </c>
       <c r="K27">
-        <v>87.79389609971304</v>
+        <v>60.13441786971049</v>
       </c>
       <c r="L27">
-        <v>0.02259688567885212</v>
+        <v>0.06298101072657836</v>
       </c>
       <c r="M27">
-        <v>15.75325024294949</v>
+        <v>1.568764306202474E-25</v>
       </c>
       <c r="N27">
-        <v>0.0001999951357830614</v>
+        <v>-5.367531465370823E-05</v>
       </c>
       <c r="O27">
-        <v>298.1243837404094</v>
+        <v>-138.9509047335262</v>
       </c>
       <c r="P27">
-        <v>203.8595111834251</v>
+        <v>-240.9259860860476</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28">
-        <v>347.9048297120319</v>
+        <v>4.963023535182331</v>
       </c>
       <c r="B28">
         <v>0.02</v>
       </c>
       <c r="C28">
-        <v>1.327017432663145</v>
+        <v>20.25710807129565</v>
       </c>
       <c r="D28">
-        <v>0.07589798474770515</v>
+        <v>-0.06617149478998177</v>
       </c>
       <c r="E28">
-        <v>0.04002605094503976</v>
+        <v>0.3421130304013377</v>
       </c>
       <c r="F28">
-        <v>1.933563927507374</v>
+        <v>1.999999498710614</v>
       </c>
       <c r="G28">
-        <v>-0.05057406156855061</v>
+        <v>0.05611899938720128</v>
       </c>
       <c r="H28">
-        <v>-2.961310528341408E-06</v>
+        <v>65.15825179911336</v>
       </c>
       <c r="I28">
-        <v>-2.175712204485554E-06</v>
+        <v>60.6424258199774</v>
       </c>
       <c r="J28">
-        <v>32.48018507158981</v>
+        <v>57.4461050429945</v>
       </c>
       <c r="K28">
-        <v>146.1378839056372</v>
+        <v>58.92615039693928</v>
       </c>
       <c r="L28">
-        <v>0.03368323206949987</v>
+        <v>0.05132264680241373</v>
       </c>
       <c r="M28">
-        <v>3.47787717596384E-05</v>
+        <v>2.830983595433104E-28</v>
       </c>
       <c r="N28">
-        <v>-29.28021047089428</v>
+        <v>-28.62000192897993</v>
       </c>
       <c r="O28">
-        <v>-301.3860848256655</v>
+        <v>224.1530884898876</v>
       </c>
       <c r="P28">
-        <v>-184.6913196339694</v>
+        <v>-215.3147127432239</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c r="A29">
-        <v>351.7838196390722</v>
+        <v>5.216391358850169</v>
       </c>
       <c r="B29">
         <v>0.02</v>
       </c>
       <c r="C29">
-        <v>1.276641886751603</v>
+        <v>19.56986153668406</v>
       </c>
       <c r="D29">
-        <v>-0.03026005628584125</v>
+        <v>-0.0666321352467568</v>
       </c>
       <c r="E29">
-        <v>0.01883992507947921</v>
+        <v>0.3755668045678391</v>
       </c>
       <c r="F29">
-        <v>1.723839738318365</v>
+        <v>1.909801751400547</v>
       </c>
       <c r="G29">
-        <v>0.05968003560393236</v>
+        <v>0.04204554436509146</v>
       </c>
       <c r="H29">
-        <v>171.4285743897674</v>
+        <v>50.04380040419706</v>
       </c>
       <c r="I29">
-        <v>-2.594230685574422E-06</v>
+        <v>51.01071316721705</v>
       </c>
       <c r="J29">
-        <v>0.1943252489873309</v>
+        <v>55.19162123256464</v>
       </c>
       <c r="K29">
-        <v>103.850073730754</v>
+        <v>56.66425996408394</v>
       </c>
       <c r="L29">
-        <v>0.02427553839522184</v>
+        <v>0.06332210453117473</v>
       </c>
       <c r="M29">
-        <v>15.63296892205036</v>
+        <v>1.59989329059248E-26</v>
       </c>
       <c r="N29">
-        <v>0.0001999934466598271</v>
+        <v>2.426879561172013E-07</v>
       </c>
       <c r="O29">
-        <v>282.0032639314232</v>
+        <v>-118.7746998057287</v>
       </c>
       <c r="P29">
-        <v>176.0627292231166</v>
+        <v>-244.3834921872013</v>
       </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30">
-        <v>355.4215195172922</v>
+        <v>5.479401382938831</v>
       </c>
       <c r="B30">
         <v>0.02</v>
       </c>
       <c r="C30">
-        <v>1.502300650304962</v>
+        <v>18.90566457868778</v>
       </c>
       <c r="D30">
-        <v>0.05225687843390924</v>
+        <v>-0.0656040060246442</v>
       </c>
       <c r="E30">
-        <v>0.03652927614555809</v>
+        <v>0.3568248022896389</v>
       </c>
       <c r="F30">
-        <v>1.971801869695252</v>
+        <v>1.763105826308185</v>
       </c>
       <c r="G30">
-        <v>0.01245174436666112</v>
+        <v>0.03335066998658347</v>
       </c>
       <c r="H30">
-        <v>-2.953260079981019E-06</v>
+        <v>60.35793359666894</v>
       </c>
       <c r="I30">
-        <v>-2.476691795817937E-06</v>
+        <v>55.66827258623834</v>
       </c>
       <c r="J30">
-        <v>31.16980258046534</v>
+        <v>53.10798433878568</v>
       </c>
       <c r="K30">
-        <v>151.9245538799877</v>
+        <v>54.87485800965162</v>
       </c>
       <c r="L30">
-        <v>0.02427849587366249</v>
+        <v>0.0522304813512872</v>
       </c>
       <c r="M30">
-        <v>3.963478217760007E-05</v>
+        <v>91.41256820290248</v>
       </c>
       <c r="N30">
-        <v>-26.95479607823283</v>
+        <v>2.236481725476671E-24</v>
       </c>
       <c r="O30">
-        <v>-255.7835745633932</v>
+        <v>127.3548453895466</v>
       </c>
       <c r="P30">
-        <v>-142.2748380888008</v>
+        <v>-217.4153173629903</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31">
-        <v>358.8171772747159</v>
+        <v>5.750999871292233</v>
       </c>
       <c r="B31">
         <v>0.02</v>
       </c>
       <c r="C31">
-        <v>1.461633913731184</v>
+        <v>18.49700693031129</v>
       </c>
       <c r="D31">
-        <v>-0.01856597247728323</v>
+        <v>-0.06329929296912493</v>
       </c>
       <c r="E31">
-        <v>0.01701379535939716</v>
+        <v>0.3800973215982708</v>
       </c>
       <c r="F31">
-        <v>2.000000049641876</v>
+        <v>1.591762018829999</v>
       </c>
       <c r="G31">
-        <v>-0.03144914128015154</v>
+        <v>0.02841764661952779</v>
       </c>
       <c r="H31">
-        <v>171.4285743718356</v>
+        <v>48.01169906866211</v>
       </c>
       <c r="I31">
-        <v>57.46679067473682</v>
+        <v>49.07286240900848</v>
       </c>
       <c r="J31">
-        <v>0.1542633083456333</v>
+        <v>58.09786346314313</v>
       </c>
       <c r="K31">
-        <v>112.6619578987169</v>
+        <v>54.94336917923483</v>
       </c>
       <c r="L31">
-        <v>0.02348097546284098</v>
+        <v>0.06939279321942551</v>
       </c>
       <c r="M31">
-        <v>7.158342810607756</v>
+        <v>-5.957587782203527E-29</v>
       </c>
       <c r="N31">
-        <v>0.0001999902651772596</v>
+        <v>1.677535141814168E-05</v>
       </c>
       <c r="O31">
-        <v>244.6562394080815</v>
+        <v>-66.04634201202123</v>
       </c>
       <c r="P31">
-        <v>139.2720250617973</v>
+        <v>-244.3730092245467</v>
       </c>
     </row>
     <row r="32" spans="1:16">
       <c r="A32">
-        <v>362.0551415401488</v>
+        <v>6.030808714007093</v>
       </c>
       <c r="B32">
         <v>0.02</v>
       </c>
       <c r="C32">
-        <v>1.659464663848217</v>
+        <v>17.90056985576439</v>
       </c>
       <c r="D32">
-        <v>0.04092789256184379</v>
+        <v>-0.05867408132330796</v>
       </c>
       <c r="E32">
-        <v>0.02832343158355989</v>
+        <v>0.3682562603721562</v>
       </c>
       <c r="F32">
-        <v>1.776863818126263</v>
+        <v>1.42129742159429</v>
       </c>
       <c r="G32">
-        <v>-0.08149317204961917</v>
+        <v>0.02802251492798536</v>
       </c>
       <c r="H32">
-        <v>-2.938688058958549E-06</v>
+        <v>56.69189764168556</v>
       </c>
       <c r="I32">
-        <v>14.45191930055176</v>
+        <v>52.00463748034964</v>
       </c>
       <c r="J32">
-        <v>8.307570489194399</v>
+        <v>49.12241722812717</v>
       </c>
       <c r="K32">
-        <v>129.2083313462189</v>
+        <v>51.33806932408342</v>
       </c>
       <c r="L32">
-        <v>0.02181167886918744</v>
+        <v>0.06197848919785732</v>
       </c>
       <c r="M32">
-        <v>7.977459785151058</v>
+        <v>68.92316978135646</v>
       </c>
       <c r="N32">
-        <v>0.000199864075601082</v>
+        <v>3.11855260816492E-25</v>
       </c>
       <c r="O32">
-        <v>-213.9240847723869</v>
+        <v>121.056377388412</v>
       </c>
       <c r="P32">
-        <v>-113.7610134748317</v>
+        <v>-222.0389915312417</v>
       </c>
     </row>
     <row r="33" spans="1:16">
       <c r="A33">
-        <v>365.1638489836643</v>
+        <v>6.320028452627537</v>
       </c>
       <c r="B33">
         <v>0.02</v>
       </c>
       <c r="C33">
-        <v>1.625582917253973</v>
+        <v>17.45987373387959</v>
       </c>
       <c r="D33">
-        <v>-0.01273038082837005</v>
+        <v>-0.05271370901780061</v>
       </c>
       <c r="E33">
-        <v>0.01472717558567554</v>
+        <v>0.3905904597524811</v>
       </c>
       <c r="F33">
-        <v>1.297372152897303</v>
+        <v>1.290376152413829</v>
       </c>
       <c r="G33">
-        <v>-0.1323918098790651</v>
+        <v>0.03280378142384666</v>
       </c>
       <c r="H33">
-        <v>171.4285742934214</v>
+        <v>45.86854625080127</v>
       </c>
       <c r="I33">
-        <v>171.4285741221187</v>
+        <v>46.80838075915286</v>
       </c>
       <c r="J33">
-        <v>17.68033896057787</v>
+        <v>51.8006688142414</v>
       </c>
       <c r="K33">
-        <v>134.2326690355763</v>
+        <v>51.9675529646732</v>
       </c>
       <c r="L33">
-        <v>0.02152180303315001</v>
+        <v>0.07501908524007181</v>
       </c>
       <c r="M33">
-        <v>1.581620754370884</v>
+        <v>261.7167072585108</v>
       </c>
       <c r="N33">
-        <v>0.0001999847464276984</v>
+        <v>-9.598535298243677E-31</v>
       </c>
       <c r="O33">
-        <v>203.4016984827308</v>
+        <v>-247.3352899442067</v>
       </c>
       <c r="P33">
-        <v>109.2483861128341</v>
+        <v>-221.0784672431397</v>
       </c>
     </row>
     <row r="34" spans="1:16">
       <c r="A34">
-        <v>368.2045912450644</v>
+        <v>6.611466678105559</v>
       </c>
       <c r="B34">
         <v>0.02</v>
       </c>
       <c r="C34">
-        <v>1.801506079998902</v>
+        <v>17.68452854028479</v>
       </c>
       <c r="D34">
-        <v>0.03374411492090467</v>
+        <v>-0.05277535762174398</v>
       </c>
       <c r="E34">
-        <v>0.02189995110211204</v>
+        <v>0.3598096460151987</v>
       </c>
       <c r="F34">
-        <v>0.5274608441792159</v>
+        <v>1.203009380508814</v>
       </c>
       <c r="G34">
-        <v>-0.1862692065447703</v>
+        <v>0.03704144584465612</v>
       </c>
       <c r="H34">
-        <v>-2.883323264055616E-06</v>
+        <v>55.3170429663875</v>
       </c>
       <c r="I34">
-        <v>87.72442731358301</v>
+        <v>50.67718014078041</v>
       </c>
       <c r="J34">
-        <v>14.39861538125679</v>
+        <v>56.83232653198873</v>
       </c>
       <c r="K34">
-        <v>134.7382593024339</v>
+        <v>53.18848044892403</v>
       </c>
       <c r="L34">
-        <v>0.02058822699095207</v>
+        <v>0.06866613363868762</v>
       </c>
       <c r="M34">
-        <v>0.3208649184350714</v>
+        <v>43.3831044343839</v>
       </c>
       <c r="N34">
-        <v>0.000199945536750804</v>
+        <v>-1.651680962403308E-26</v>
       </c>
       <c r="O34">
-        <v>-183.8144761536342</v>
+        <v>171.3099134863379</v>
       </c>
       <c r="P34">
-        <v>-95.39638960489245</v>
+        <v>-225.9957916261661</v>
       </c>
     </row>
     <row r="35" spans="1:16">
       <c r="A35">
-        <v>371.1984544463602</v>
+        <v>6.905138940281997</v>
       </c>
       <c r="B35">
         <v>0.02</v>
       </c>
       <c r="C35">
-        <v>1.777658155516802</v>
+        <v>17.23401778798979</v>
       </c>
       <c r="D35">
-        <v>-0.008665054664186964</v>
+        <v>-0.04580828679797188</v>
       </c>
       <c r="E35">
-        <v>0.01652353012017592</v>
+        <v>0.3915808318291374</v>
       </c>
       <c r="F35">
-        <v>-0.5440211802652701</v>
+        <v>1.151114730230537</v>
       </c>
       <c r="G35">
-        <v>-0.2394817762118191</v>
+        <v>0.04242575900457433</v>
       </c>
       <c r="H35">
-        <v>48.32547105896449</v>
+        <v>45.92504654053485</v>
       </c>
       <c r="I35">
-        <v>171.4285742023826</v>
+        <v>46.83243496698204</v>
       </c>
       <c r="J35">
-        <v>8.283212327689206</v>
+        <v>51.47095802622008</v>
       </c>
       <c r="K35">
-        <v>126.6720054807343</v>
+        <v>49.92742206220482</v>
       </c>
       <c r="L35">
-        <v>0.01513165157237306</v>
+        <v>0.08329081763892782</v>
       </c>
       <c r="M35">
-        <v>20.07256326739708</v>
+        <v>280.1664486362501</v>
       </c>
       <c r="N35">
-        <v>0.0001999765356002858</v>
+        <v>2.567646184633904E-29</v>
       </c>
       <c r="O35">
-        <v>31.47237693223547</v>
+        <v>-265.7739080861951</v>
       </c>
       <c r="P35">
-        <v>25.68974933550225</v>
+        <v>-213.8737271608356</v>
       </c>
     </row>
     <row r="36" spans="1:16">
       <c r="A36">
-        <v>374.2239507181678</v>
+        <v>7.200296208691094</v>
       </c>
       <c r="B36">
         <v>0.02</v>
       </c>
       <c r="C36">
-        <v>1.902121033193476</v>
+        <v>17.53188097188578</v>
       </c>
       <c r="D36">
-        <v>0.02299553303131527</v>
+        <v>-0.04720362886079962</v>
       </c>
       <c r="E36">
-        <v>0.4772008638492212</v>
+        <v>0.3589701590505832</v>
       </c>
       <c r="F36">
-        <v>-2.000000049768825</v>
+        <v>1.149069956547078</v>
       </c>
       <c r="G36">
-        <v>-0.3048187110169432</v>
+        <v>0.04804723048819105</v>
       </c>
       <c r="H36">
-        <v>-2.902631722834846E-06</v>
+        <v>54.22641023152722</v>
       </c>
       <c r="I36">
-        <v>171.4285740033698</v>
+        <v>49.72164211795151</v>
       </c>
       <c r="J36">
-        <v>51.7215908871168</v>
+        <v>56.59770943834998</v>
       </c>
       <c r="K36">
-        <v>171.4285706970392</v>
+        <v>53.5163566059118</v>
       </c>
       <c r="L36">
-        <v>0.118695261913302</v>
+        <v>0.07150070286149632</v>
       </c>
       <c r="M36">
-        <v>264.7336158699712</v>
+        <v>59.16893691467783</v>
       </c>
       <c r="N36">
-        <v>-491.7553598311159</v>
+        <v>-1.453888720114538E-25</v>
       </c>
       <c r="O36">
-        <v>-221.0228088134109</v>
+        <v>154.8998612278962</v>
       </c>
       <c r="P36">
-        <v>-128.2331304978224</v>
+        <v>-227.1009672237715</v>
       </c>
     </row>
     <row r="37" spans="1:16">
       <c r="A37">
-        <v>376.0546544168142</v>
+        <v>7.496085728932864</v>
       </c>
       <c r="B37">
         <v>0.02</v>
       </c>
       <c r="C37">
-        <v>3.977888568276782</v>
+        <v>17.1431139479808</v>
       </c>
       <c r="D37">
-        <v>0.03834973784790086</v>
+        <v>-0.04082649287382356</v>
       </c>
       <c r="E37">
-        <v>0.2148393726893207</v>
+        <v>0.3900412960272182</v>
       </c>
       <c r="F37">
-        <v>-1.805915678483411</v>
+        <v>1.182521595426026</v>
       </c>
       <c r="G37">
-        <v>0.1209905938377209</v>
+        <v>0.05388224042737847</v>
       </c>
       <c r="H37">
-        <v>171.42857426433</v>
+        <v>46.31727679658388</v>
       </c>
       <c r="I37">
-        <v>-2.834215377080956E-06</v>
+        <v>47.09303475600134</v>
       </c>
       <c r="J37">
-        <v>152.0069759107495</v>
+        <v>52.73515869816585</v>
       </c>
       <c r="K37">
-        <v>171.4285515947262</v>
+        <v>49.45763745343412</v>
       </c>
       <c r="L37">
-        <v>0.04143753457643821</v>
+        <v>0.1830028358104935</v>
       </c>
       <c r="M37">
-        <v>34.47948396533056</v>
+        <v>238.5727406092965</v>
       </c>
       <c r="N37">
-        <v>-388.8832265075421</v>
+        <v>-3.786883064217709E-29</v>
       </c>
       <c r="O37">
-        <v>-118.7594280774801</v>
+        <v>-191.6909737606789</v>
       </c>
       <c r="P37">
-        <v>-60.50391698307328</v>
+        <v>-220.1070107144204</v>
       </c>
     </row>
     <row r="38" spans="1:16">
       <c r="A38">
-        <v>377.2989801105899</v>
+        <v>7.793938959118723</v>
       </c>
       <c r="B38">
         <v>0.02</v>
       </c>
       <c r="C38">
-        <v>4.754166510182819</v>
+        <v>17.2569442584117</v>
       </c>
       <c r="D38">
-        <v>0.01105672481320672</v>
+        <v>-0.04450722972638575</v>
       </c>
       <c r="E38">
-        <v>0.1025970988266143</v>
+        <v>0.3647261767296222</v>
       </c>
       <c r="F38">
-        <v>-0.7760956436413973</v>
+        <v>1.260403551929532</v>
       </c>
       <c r="G38">
-        <v>0.1872238157825133</v>
+        <v>0.06122746719624157</v>
       </c>
       <c r="H38">
-        <v>171.428574368873</v>
+        <v>51.3643419549745</v>
       </c>
       <c r="I38">
-        <v>-2.919701165139602E-06</v>
+        <v>47.30676760082309</v>
       </c>
       <c r="J38">
-        <v>1.039546254646192</v>
+        <v>54.88863585206523</v>
       </c>
       <c r="K38">
-        <v>2.081270048997986E-07</v>
+        <v>52.54830344708554</v>
       </c>
       <c r="L38">
-        <v>0.0295173129475529</v>
+        <v>0.06497434698849419</v>
       </c>
       <c r="M38">
-        <v>221.5369485367968</v>
+        <v>141.005231303369</v>
       </c>
       <c r="N38">
-        <v>0.0001998753840946112</v>
+        <v>4.115314585031116E-25</v>
       </c>
       <c r="O38">
-        <v>-22.52059033976505</v>
+        <v>-3.721436148868396</v>
       </c>
       <c r="P38">
-        <v>-11.06638168497132</v>
+        <v>-232.7946857549203</v>
       </c>
     </row>
     <row r="39" spans="1:16">
       <c r="A39">
-        <v>378.3702587848759</v>
+        <v>8.091122931133524</v>
       </c>
       <c r="B39">
         <v>0.02</v>
       </c>
       <c r="C39">
-        <v>5.254159172433778</v>
+        <v>17.15579617263688</v>
       </c>
       <c r="D39">
-        <v>0.01395247005557099</v>
+        <v>-0.04030892298840084</v>
       </c>
       <c r="E39">
-        <v>0.0757927419418279</v>
+        <v>0.3724066999441362</v>
       </c>
       <c r="F39">
-        <v>0.2732431060815674</v>
+        <v>1.368312054915998</v>
       </c>
       <c r="G39">
-        <v>0.1730869302551418</v>
+        <v>0.06578103394254267</v>
       </c>
       <c r="H39">
-        <v>171.4285737283847</v>
+        <v>48.38540008525107</v>
       </c>
       <c r="I39">
-        <v>76.52673769605225</v>
+        <v>48.7111656481016</v>
       </c>
       <c r="J39">
-        <v>166.0554239689108</v>
+        <v>54.2810219180784</v>
       </c>
       <c r="K39">
-        <v>164.4678350515972</v>
+        <v>50.12603376177968</v>
       </c>
       <c r="L39">
-        <v>0.02147626711792422</v>
+        <v>0.08554277063520478</v>
       </c>
       <c r="M39">
-        <v>25.88335224619073</v>
+        <v>231.1489103499916</v>
       </c>
       <c r="N39">
-        <v>0.0001998994722095968</v>
+        <v>4.228808392912525E-30</v>
       </c>
       <c r="O39">
-        <v>-43.17984304639459</v>
+        <v>-187.4406879674974</v>
       </c>
       <c r="P39">
-        <v>-21.26991846151348</v>
+        <v>-224.8106749389978</v>
       </c>
     </row>
     <row r="40" spans="1:16">
       <c r="A40">
-        <v>379.3429533001744</v>
+        <v>8.386889961011637</v>
       </c>
       <c r="B40">
         <v>0.02</v>
       </c>
       <c r="C40">
-        <v>5.526152435038922</v>
+        <v>17.33977792713401</v>
       </c>
       <c r="D40">
-        <v>0.007568644962309433</v>
+        <v>-0.03835916300840144</v>
       </c>
       <c r="E40">
-        <v>0.05903805790634745</v>
+        <v>0.3530006922999765</v>
       </c>
       <c r="F40">
-        <v>1.127986440594383</v>
+        <v>1.510366809876015</v>
       </c>
       <c r="G40">
-        <v>0.1314970836254192</v>
+        <v>0.06803105745413768</v>
       </c>
       <c r="H40">
-        <v>171.4285736709441</v>
+        <v>51.24712558420509</v>
       </c>
       <c r="I40">
-        <v>110.7119989847646</v>
+        <v>47.66051586194631</v>
       </c>
       <c r="J40">
-        <v>155.848686232725</v>
+        <v>54.21574631735587</v>
       </c>
       <c r="K40">
-        <v>152.4974943205549</v>
+        <v>52.25928490430933</v>
       </c>
       <c r="L40">
-        <v>0.01538534438478167</v>
+        <v>0.05894958667273837</v>
       </c>
       <c r="M40">
-        <v>38.13335607332485</v>
+        <v>178.9547673504247</v>
       </c>
       <c r="N40">
-        <v>0.0001999128852347269</v>
+        <v>-1.26899371976994E-30</v>
       </c>
       <c r="O40">
-        <v>-25.57193255483217</v>
+        <v>-58.39929240621525</v>
       </c>
       <c r="P40">
-        <v>-12.34065099612679</v>
+        <v>-222.4604197367706</v>
       </c>
     </row>
     <row r="41" spans="1:16">
       <c r="A41">
-        <v>380.2547684225888</v>
+        <v>8.679912998813574</v>
       </c>
       <c r="B41">
         <v>0.02</v>
       </c>
       <c r="C41">
-        <v>5.717419241253554</v>
+        <v>17.37181633112408</v>
       </c>
       <c r="D41">
-        <v>0.006059370227518984</v>
+        <v>-0.03565586879593829</v>
       </c>
       <c r="E41">
-        <v>0.06024880258579402</v>
+        <v>0.3532485738191174</v>
       </c>
       <c r="F41">
-        <v>1.690711245448674</v>
+        <v>1.665432468019806</v>
       </c>
       <c r="G41">
-        <v>0.07275638098365574</v>
+        <v>0.06649472865838951</v>
       </c>
       <c r="H41">
-        <v>171.428573926316</v>
+        <v>49.35596465950109</v>
       </c>
       <c r="I41">
-        <v>128.5495886312783</v>
+        <v>49.37339572028718</v>
       </c>
       <c r="J41">
-        <v>160.7097053986691</v>
+        <v>54.98363176134757</v>
       </c>
       <c r="K41">
-        <v>156.5968356754166</v>
+        <v>51.2147836187531</v>
       </c>
       <c r="L41">
-        <v>0.02032316487778606</v>
+        <v>0.07010805522273364</v>
       </c>
       <c r="M41">
-        <v>27.16577487064418</v>
+        <v>232.8721175334108</v>
       </c>
       <c r="N41">
-        <v>0.0001999285238911662</v>
+        <v>8.75580444618351E-30</v>
       </c>
       <c r="O41">
-        <v>-18.5132944883605</v>
+        <v>-175.3403837717839</v>
       </c>
       <c r="P41">
-        <v>-8.611321593481827</v>
+        <v>-218.5827306315371</v>
       </c>
     </row>
     <row r="42" spans="1:16">
       <c r="A42">
-        <v>381.1193026107814</v>
+        <v>8.970032173345627</v>
       </c>
       <c r="B42">
         <v>0.02</v>
       </c>
       <c r="C42">
-        <v>5.981907658553395</v>
+        <v>17.57525092731254</v>
       </c>
       <c r="D42">
-        <v>0.009478465703786841</v>
+        <v>-0.03373530975851145</v>
       </c>
       <c r="E42">
-        <v>0.1001419930353323</v>
+        <v>0.3380644137788796</v>
       </c>
       <c r="F42">
-        <v>1.965344683833926</v>
+        <v>1.816043997584537</v>
       </c>
       <c r="G42">
-        <v>0.01775191993219125</v>
+        <v>0.06176038018371807</v>
       </c>
       <c r="H42">
-        <v>16.56482213723607</v>
+        <v>51.69476284908245</v>
       </c>
       <c r="I42">
-        <v>-2.674605207773841E-06</v>
+        <v>48.51230848719851</v>
       </c>
       <c r="J42">
-        <v>162.5804756510469</v>
+        <v>54.78041270453804</v>
       </c>
       <c r="K42">
-        <v>158.1948540565109</v>
+        <v>52.62006601679167</v>
       </c>
       <c r="L42">
-        <v>0.01675487733444195</v>
+        <v>0.0460562270289034</v>
       </c>
       <c r="M42">
-        <v>73.28694592025991</v>
+        <v>204.9067526621295</v>
       </c>
       <c r="N42">
-        <v>0.0001998846137043633</v>
+        <v>1.042014786473643E-30</v>
       </c>
       <c r="O42">
-        <v>-45.04224645676251</v>
+        <v>-96.28246823869799</v>
       </c>
       <c r="P42">
-        <v>-22.08878878410075</v>
+        <v>-210.0498392475159</v>
       </c>
     </row>
     <row r="43" spans="1:16">
       <c r="A43">
-        <v>381.9370155204589</v>
+        <v>9.256564707387838</v>
       </c>
       <c r="B43">
         <v>0.02</v>
       </c>
       <c r="C43">
-        <v>6.330431678887159</v>
+        <v>17.70055364537248</v>
       </c>
       <c r="D43">
-        <v>0.0051170627011792</v>
+        <v>-0.03405187191906311</v>
       </c>
       <c r="E43">
-        <v>0.08779113903198772</v>
+        <v>0.3315416378786687</v>
       </c>
       <c r="F43">
-        <v>2.000000049471945</v>
+        <v>1.934703061322355</v>
       </c>
       <c r="G43">
-        <v>-0.02143753089946938</v>
+        <v>0.05268192102089887</v>
       </c>
       <c r="H43">
-        <v>171.4285735604942</v>
+        <v>50.52265550655499</v>
       </c>
       <c r="I43">
-        <v>171.4285738647595</v>
+        <v>50.33060267106741</v>
       </c>
       <c r="J43">
-        <v>164.4092968314938</v>
+        <v>55.57729762065753</v>
       </c>
       <c r="K43">
-        <v>157.1127758461759</v>
+        <v>52.44158949040104</v>
       </c>
       <c r="L43">
-        <v>0.02348423847781038</v>
+        <v>0.05012939732648833</v>
       </c>
       <c r="M43">
-        <v>55.87574092098637</v>
+        <v>239.2709021790526</v>
       </c>
       <c r="N43">
-        <v>0.0001999182603059054</v>
+        <v>1.107546326902022E-26</v>
       </c>
       <c r="O43">
-        <v>0.7154276828146691</v>
+        <v>-171.7392613533504</v>
       </c>
       <c r="P43">
-        <v>-1.676288888033395</v>
+        <v>-208.1299181206844</v>
       </c>
     </row>
     <row r="44" spans="1:16">
       <c r="A44">
-        <v>382.7073812169757</v>
+        <v>9.539675302571187</v>
       </c>
       <c r="B44">
         <v>0.02</v>
       </c>
       <c r="C44">
-        <v>6.752369202727333</v>
+        <v>17.92702921776986</v>
       </c>
       <c r="D44">
-        <v>0.009849008413409145</v>
+        <v>-0.03265342238335223</v>
       </c>
       <c r="E44">
-        <v>0.3012305668534642</v>
+        <v>0.316265148381986</v>
       </c>
       <c r="F44">
-        <v>1.834190011641778</v>
+        <v>1.999999864931711</v>
       </c>
       <c r="G44">
-        <v>-0.0632777622729922</v>
+        <v>0.03936629053902025</v>
       </c>
       <c r="H44">
-        <v>-2.887083871084747E-06</v>
+        <v>52.53312949785076</v>
       </c>
       <c r="I44">
-        <v>30.86810830068822</v>
+        <v>49.71993067741214</v>
       </c>
       <c r="J44">
-        <v>171.4201995094965</v>
+        <v>55.68799698598681</v>
       </c>
       <c r="K44">
-        <v>164.6005763717414</v>
+        <v>53.48212057534185</v>
       </c>
       <c r="L44">
-        <v>0.03745068456376621</v>
+        <v>0.03379423605154323</v>
       </c>
       <c r="M44">
-        <v>3.263872276429288E-06</v>
+        <v>223.5503920599814</v>
       </c>
       <c r="N44">
-        <v>-108.9857890138413</v>
+        <v>2.352401576515773E-31</v>
       </c>
       <c r="O44">
-        <v>-127.4587917401681</v>
+        <v>-120.0131847962945</v>
       </c>
       <c r="P44">
-        <v>-66.4428057494016</v>
+        <v>-197.2597895081246</v>
       </c>
     </row>
     <row r="45" spans="1:16">
       <c r="A45">
-        <v>383.3919308562669</v>
+        <v>9.819407762522172</v>
       </c>
       <c r="B45">
         <v>0.02</v>
       </c>
       <c r="C45">
-        <v>8.055989276549292</v>
+        <v>18.10547760821647</v>
       </c>
       <c r="D45">
-        <v>0.008608498043274019</v>
+        <v>-0.03396394063563473</v>
       </c>
       <c r="E45">
-        <v>0.2176023916043388</v>
+        <v>0.3043746259104375</v>
       </c>
       <c r="F45">
-        <v>1.7672614527405</v>
+        <v>1.984962779664668</v>
       </c>
       <c r="G45">
-        <v>0.005308992473549387</v>
+        <v>0.02115319309012525</v>
       </c>
       <c r="H45">
-        <v>88.98680437041249</v>
+        <v>51.78285227705366</v>
       </c>
       <c r="I45">
-        <v>171.4285739642258</v>
+        <v>51.47577498699793</v>
       </c>
       <c r="J45">
-        <v>35.51508616904943</v>
+        <v>56.55507094433766</v>
       </c>
       <c r="K45">
-        <v>5.393714556615848</v>
+        <v>53.76339575335403</v>
       </c>
       <c r="L45">
-        <v>0.02863371391730217</v>
+        <v>0.02756209752023485</v>
       </c>
       <c r="M45">
-        <v>405.1222665474241</v>
+        <v>255.0793967543425</v>
       </c>
       <c r="N45">
-        <v>0.0001994820815969802</v>
+        <v>-1.216987510771085E-30</v>
       </c>
       <c r="O45">
-        <v>-115.323038554969</v>
+        <v>-180.4669891039564</v>
       </c>
       <c r="P45">
-        <v>-58.52872855414194</v>
+        <v>-190.0125905030407</v>
       </c>
     </row>
     <row r="46" spans="1:16">
       <c r="A46">
-        <v>383.9845267389514</v>
+        <v>10.09617809614165</v>
       </c>
       <c r="B46">
         <v>0.02</v>
       </c>
       <c r="C46">
-        <v>9.028602572064788</v>
+        <v>18.37587661309</v>
       </c>
       <c r="D46">
-        <v>0.004889796292154015</v>
+        <v>-0.03444662946367001</v>
       </c>
       <c r="E46">
-        <v>0.1738396328522046</v>
+        <v>0.2840196943296125</v>
       </c>
       <c r="F46">
-        <v>1.861824344012618</v>
+        <v>1.860194615692348</v>
       </c>
       <c r="G46">
-        <v>0.01473537134974662</v>
+        <v>-0.002449160335722087</v>
       </c>
       <c r="H46">
-        <v>37.87585709231951</v>
+        <v>53.68630402839651</v>
       </c>
       <c r="I46">
-        <v>171.4285733652439</v>
+        <v>51.23899152109929</v>
       </c>
       <c r="J46">
-        <v>171.3645108788047</v>
+        <v>57.24831629396588</v>
       </c>
       <c r="K46">
-        <v>127.7242671851465</v>
+        <v>54.79040116336819</v>
       </c>
       <c r="L46">
-        <v>0.01758619282455282</v>
+        <v>0.0105274321386805</v>
       </c>
       <c r="M46">
-        <v>137.4568833783262</v>
+        <v>244.5411071237461</v>
       </c>
       <c r="N46">
-        <v>0.0001996529719345974</v>
+        <v>-9.30583052841991E-30</v>
       </c>
       <c r="O46">
-        <v>-100.3212393374474</v>
+        <v>-141.0928793981904</v>
       </c>
       <c r="P46">
-        <v>-50.40392103546151</v>
+        <v>-174.5798692089672</v>
       </c>
     </row>
     <row r="47" spans="1:16">
       <c r="A47">
-        <v>384.5236715130082</v>
+        <v>10.37058164915373</v>
       </c>
       <c r="B47">
         <v>0.02</v>
       </c>
       <c r="C47">
-        <v>9.725713536445353</v>
+        <v>18.61104172838906</v>
       </c>
       <c r="D47">
-        <v>0.0003698205632270834</v>
+        <v>-0.03789585827521252</v>
       </c>
       <c r="E47">
-        <v>0.1383874013566217</v>
+        <v>0.2622089044107401</v>
       </c>
       <c r="F47">
-        <v>1.89633036154025</v>
+        <v>1.586827175290384</v>
       </c>
       <c r="G47">
-        <v>-0.006953650377699439</v>
+        <v>-0.03255404080890677</v>
       </c>
       <c r="H47">
-        <v>16.65149387051026</v>
+        <v>53.24441312161098</v>
       </c>
       <c r="I47">
-        <v>171.4285731657336</v>
+        <v>52.95110200559144</v>
       </c>
       <c r="J47">
-        <v>171.1894133134</v>
+        <v>58.26542181642778</v>
       </c>
       <c r="K47">
-        <v>117.8126710842341</v>
+        <v>55.3661261253029</v>
       </c>
       <c r="L47">
-        <v>0.01050199670059428</v>
+        <v>0.005360065039212361</v>
       </c>
       <c r="M47">
-        <v>121.7760529062457</v>
+        <v>272.1752115071617</v>
       </c>
       <c r="N47">
-        <v>0.0001997093264230432</v>
+        <v>-9.437179747590532E-31</v>
       </c>
       <c r="O47">
-        <v>-83.56828454328904</v>
+        <v>-190.0481416090455</v>
       </c>
       <c r="P47">
-        <v>-41.59461881304307</v>
+        <v>-165.6302451048647</v>
       </c>
     </row>
     <row r="48" spans="1:16">
       <c r="A48">
-        <v>385.0307635338429</v>
+        <v>10.64375626276973</v>
       </c>
       <c r="B48">
         <v>0.01991830220998726</v>
       </c>
       <c r="C48">
-        <v>10.23258814852241</v>
+        <v>18.91926512013778</v>
       </c>
       <c r="D48">
-        <v>-0.00189341310996009</v>
+        <v>-0.03720035898949309</v>
       </c>
       <c r="E48">
-        <v>0.1089926021670921</v>
+        <v>0.23470033260237</v>
       </c>
       <c r="F48">
-        <v>1.751320840640777</v>
+        <v>1.134233650033034</v>
       </c>
       <c r="G48">
-        <v>-0.04934821295063403</v>
+        <v>-0.06929197920200716</v>
       </c>
       <c r="H48">
-        <v>7.601835771059378</v>
+        <v>55.06600667091554</v>
       </c>
       <c r="I48">
-        <v>171.4285727235387</v>
+        <v>53.02558516164466</v>
       </c>
       <c r="J48">
-        <v>171.2563094115709</v>
+        <v>59.14145391038939</v>
       </c>
       <c r="K48">
-        <v>111.0120448500262</v>
+        <v>56.4042149913326</v>
       </c>
       <c r="L48">
-        <v>0.006246432045545776</v>
+        <v>-0.0077463281846291</v>
       </c>
       <c r="M48">
-        <v>103.5285300361086</v>
+        <v>271.9467120228146</v>
       </c>
       <c r="N48">
-        <v>0.0001997418775560964</v>
+        <v>7.294076685247619E-30</v>
       </c>
       <c r="O48">
-        <v>-67.97649481127708</v>
+        <v>-164.486285531264</v>
       </c>
       <c r="P48">
-        <v>-33.54496094159587</v>
+        <v>-145.5832846930768</v>
       </c>
     </row>
     <row r="49" spans="1:16">
       <c r="A49">
-        <v>385.5231693221205</v>
+        <v>10.91728605354176</v>
       </c>
       <c r="B49">
         <v>0.01649435061504471</v>
       </c>
       <c r="C49">
-        <v>10.5838560986007</v>
+        <v>19.22058985590987</v>
       </c>
       <c r="D49">
-        <v>-0.002781462428249359</v>
+        <v>-0.03859596754771999</v>
       </c>
       <c r="E49">
-        <v>0.08481473246016291</v>
+        <v>0.2045581682624821</v>
       </c>
       <c r="F49">
-        <v>1.372507159837443</v>
+        <v>0.4915141992219205</v>
       </c>
       <c r="G49">
-        <v>-0.08861207917973049</v>
+        <v>-0.09586886879412186</v>
       </c>
       <c r="H49">
-        <v>3.613384762751696</v>
+        <v>54.9355867617726</v>
       </c>
       <c r="I49">
-        <v>171.4285719898419</v>
+        <v>54.76806918576017</v>
       </c>
       <c r="J49">
-        <v>171.172971775934</v>
+        <v>60.28574355370315</v>
       </c>
       <c r="K49">
-        <v>106.2382889625225</v>
+        <v>57.29226541078476</v>
       </c>
       <c r="L49">
-        <v>0.003720060442982321</v>
+        <v>-0.01145590098799235</v>
       </c>
       <c r="M49">
-        <v>83.62357939964056</v>
+        <v>302.382786048038</v>
       </c>
       <c r="N49">
-        <v>0.0001997627473227951</v>
+        <v>-7.413824476071486E-31</v>
       </c>
       <c r="O49">
-        <v>-53.93265230056954</v>
+        <v>-206.7726729348484</v>
       </c>
       <c r="P49">
-        <v>-26.42388440454391</v>
+        <v>-131.301250648508</v>
       </c>
     </row>
     <row r="50" spans="1:16">
       <c r="A50">
-        <v>386.0109212494555</v>
+        <v>11.18979201538024</v>
       </c>
       <c r="B50">
         <v>0.009809843005185111</v>
       </c>
       <c r="C50">
-        <v>10.80251214440495</v>
+        <v>19.60062225845789</v>
       </c>
       <c r="D50">
-        <v>-0.002894853749762275</v>
+        <v>-0.03551467540361967</v>
       </c>
       <c r="E50">
-        <v>0.06519857980062542</v>
+        <v>0.1713465552052831</v>
       </c>
       <c r="F50">
-        <v>0.8432682463758998</v>
+        <v>-0.2233307246219464</v>
       </c>
       <c r="G50">
-        <v>-0.1038154187969173</v>
+        <v>-0.09619850324199698</v>
       </c>
       <c r="H50">
-        <v>1.817437972777156</v>
+        <v>56.81260921575408</v>
       </c>
       <c r="I50">
-        <v>171.4285704780864</v>
+        <v>55.21912616879638</v>
       </c>
       <c r="J50">
-        <v>170.2908036876566</v>
+        <v>61.41483650969563</v>
       </c>
       <c r="K50">
-        <v>102.2812029480785</v>
+        <v>58.5178634365199</v>
       </c>
       <c r="L50">
-        <v>0.002262226864125965</v>
+        <v>-0.02193531581744311</v>
       </c>
       <c r="M50">
-        <v>57.82534271762061</v>
+        <v>313.5115482953804</v>
       </c>
       <c r="N50">
-        <v>0.0001997745287455976</v>
+        <v>2.428808427027646E-31</v>
       </c>
       <c r="O50">
-        <v>-41.86865787479469</v>
+        <v>-194.7837204811747</v>
       </c>
       <c r="P50">
-        <v>-20.40180903239728</v>
+        <v>-106.4830237513414</v>
       </c>
     </row>
     <row r="51" spans="1:16">
       <c r="A51">
-        <v>386.4959033344862</v>
+        <v>11.45734382909261</v>
       </c>
       <c r="B51">
         <v>0.003233794600127655</v>
       </c>
       <c r="C51">
-        <v>10.90775409613783</v>
+        <v>19.99378005686687</v>
       </c>
       <c r="D51">
-        <v>-0.002611252663796164</v>
+        <v>-0.03455940870307408</v>
       </c>
       <c r="E51">
-        <v>0.04966362439551574</v>
+        <v>0.1362198362502424</v>
       </c>
       <c r="F51">
-        <v>0.2982196609155605</v>
+        <v>-0.866589804777582</v>
       </c>
       <c r="G51">
-        <v>-0.0931538123689617</v>
+        <v>-0.07209005550940069</v>
       </c>
       <c r="H51">
-        <v>0.9898575977976396</v>
+        <v>57.05344889906311</v>
       </c>
       <c r="I51">
-        <v>171.4285660541739</v>
+        <v>57.08606609375592</v>
       </c>
       <c r="J51">
-        <v>165.4813939015812</v>
+        <v>62.78037732534976</v>
       </c>
       <c r="K51">
-        <v>95.55260585199477</v>
+        <v>59.80607084570988</v>
       </c>
       <c r="L51">
-        <v>0.001450095435172325</v>
+        <v>-0.02340240964807794</v>
       </c>
       <c r="M51">
-        <v>43.34927383714518</v>
+        <v>344.8597562577993</v>
       </c>
       <c r="N51">
-        <v>0.0001997792276190203</v>
+        <v>-6.572276610274761E-30</v>
       </c>
       <c r="O51">
-        <v>-31.96765559778959</v>
+        <v>-229.3808801869622</v>
       </c>
       <c r="P51">
-        <v>-15.51828735437315</v>
+        <v>-88.69013583422591</v>
       </c>
     </row>
     <row r="52" spans="1:16">
       <c r="A52">
-        <v>386.9784472961992</v>
+        <v>11.71797598337239</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52">
-        <v>10.92076081929019</v>
+        <v>20.45153614189159</v>
       </c>
       <c r="D52">
-        <v>-0.002166861164070132</v>
+        <v>-0.02980111408246361</v>
       </c>
       <c r="E52">
-        <v>0.03761935623202067</v>
+        <v>0.1023881967446281</v>
       </c>
       <c r="F52">
-        <v>-0.1477303146634473</v>
+        <v>-1.330283582595182</v>
       </c>
       <c r="G52">
-        <v>-0.07225410287297838</v>
+        <v>-0.0410563103650491</v>
       </c>
       <c r="H52">
-        <v>0.5878311635972819</v>
+        <v>59.02630543832731</v>
       </c>
       <c r="I52">
-        <v>171.4284854879963</v>
+        <v>57.89317031525459</v>
       </c>
       <c r="J52">
-        <v>160.8784359337548</v>
+        <v>64.15931887715459</v>
       </c>
       <c r="K52">
-        <v>89.80045186901765</v>
+        <v>61.28380372892499</v>
       </c>
       <c r="L52">
-        <v>0.001025179005282881</v>
+        <v>-0.0296431275454726</v>
       </c>
       <c r="M52">
-        <v>33.5216254755444</v>
+        <v>362.9837397638042</v>
       </c>
       <c r="N52">
-        <v>0.0001997802964525157</v>
+        <v>1.553884969042059E-29</v>
       </c>
       <c r="O52">
-        <v>-24.11188566969494</v>
+        <v>-227.8503562528336</v>
       </c>
       <c r="P52">
-        <v>-11.67571992858589</v>
+        <v>-63.65573791435528</v>
       </c>
     </row>
     <row r="53" spans="1:16">
       <c r="A53">
-        <v>387.4613426542454</v>
+        <v>11.97214748785181</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53">
-        <v>10.86233879859392</v>
+        <v>20.92891599224533</v>
       </c>
       <c r="D53">
-        <v>-0.001689320628887865</v>
+        <v>-0.02675311687018086</v>
       </c>
       <c r="E53">
-        <v>0.02840862272140857</v>
+        <v>0.06953685504965307</v>
       </c>
       <c r="F53">
-        <v>-0.494593342608816</v>
+        <v>-1.635005788406454</v>
       </c>
       <c r="G53">
-        <v>-0.05643139062821931</v>
+        <v>-0.01927449436217221</v>
       </c>
       <c r="H53">
-        <v>1.054233932755379E-05</v>
+        <v>59.6266075985923</v>
       </c>
       <c r="I53">
-        <v>171.0689628100801</v>
+        <v>59.86082576464671</v>
       </c>
       <c r="J53">
-        <v>157.443452151944</v>
+        <v>65.72881313786736</v>
       </c>
       <c r="K53">
-        <v>85.69632134516318</v>
+        <v>62.96952920945337</v>
       </c>
       <c r="L53">
-        <v>0.0007646463787985297</v>
+        <v>-0.02608121989660552</v>
       </c>
       <c r="M53">
-        <v>26.51595291811233</v>
+        <v>390.6272278688153</v>
       </c>
       <c r="N53">
-        <v>0.0001997790584360903</v>
+        <v>1.754837716188897E-29</v>
       </c>
       <c r="O53">
-        <v>-18.00062019867099</v>
+        <v>-254.0555690094482</v>
       </c>
       <c r="P53">
-        <v>-8.703171236428629</v>
+        <v>-47.30003107700363</v>
       </c>
     </row>
     <row r="54" spans="1:16">
       <c r="A54">
-        <v>387.9476983486949</v>
+        <v>12.22006230863698</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54">
-        <v>10.74940455838039</v>
+        <v>21.45086250124922</v>
       </c>
       <c r="D54">
-        <v>-0.001273509830267965</v>
+        <v>-0.02084018743828562</v>
       </c>
       <c r="E54">
-        <v>0.02137001379297698</v>
+        <v>0.04239728626678527</v>
       </c>
       <c r="F54">
-        <v>-0.7660984240537432</v>
+        <v>-1.821084291450236</v>
       </c>
       <c r="G54">
-        <v>-0.04441804797409896</v>
+        <v>-0.005477968580721022</v>
       </c>
       <c r="H54">
-        <v>3.905913536239828E-06</v>
+        <v>61.67863659980172</v>
       </c>
       <c r="I54">
-        <v>171.1902715275834</v>
+        <v>60.95624172203545</v>
       </c>
       <c r="J54">
-        <v>155.3032416594431</v>
+        <v>67.32495865425422</v>
       </c>
       <c r="K54">
-        <v>83.17349368215338</v>
+        <v>64.72162965213079</v>
       </c>
       <c r="L54">
-        <v>0.0006242295439325173</v>
+        <v>-0.02549734842109723</v>
       </c>
       <c r="M54">
-        <v>21.61862917967242</v>
+        <v>407.7695549652397</v>
       </c>
       <c r="N54">
-        <v>0.0001997756266513288</v>
+        <v>2.138316141107261E-29</v>
       </c>
       <c r="O54">
-        <v>-13.33094574457206</v>
+        <v>-257.1210426905168</v>
       </c>
       <c r="P54">
-        <v>-6.43950264548321</v>
+        <v>-27.98035286826806</v>
       </c>
     </row>
     <row r="55" spans="1:16">
       <c r="A55">
-        <v>388.439902728492</v>
+        <v>12.4618641413827</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55">
-        <v>10.59633005167963</v>
+        <v>21.98102523013781</v>
       </c>
       <c r="D55">
-        <v>-0.0009194054039673202</v>
+        <v>-0.01632475671977554</v>
       </c>
       <c r="E55">
-        <v>0.01604220419506138</v>
+        <v>0.02003675377682059</v>
       </c>
       <c r="F55">
-        <v>-0.9801867607194868</v>
+        <v>-1.924829173039639</v>
       </c>
       <c r="G55">
-        <v>-0.03528172045530424</v>
+        <v>0.001994820734094132</v>
       </c>
       <c r="H55">
-        <v>1.895729608163532E-06</v>
+        <v>62.57403605493435</v>
       </c>
       <c r="I55">
-        <v>171.2672268842661</v>
+        <v>62.93356289575028</v>
       </c>
       <c r="J55">
-        <v>154.47553741282</v>
+        <v>69.04403538169329</v>
       </c>
       <c r="K55">
-        <v>82.13092140428995</v>
+        <v>66.74689690956677</v>
       </c>
       <c r="L55">
-        <v>0.0005352667094880269</v>
+        <v>-0.01796466441569363</v>
       </c>
       <c r="M55">
-        <v>16.8641398886169</v>
+        <v>426.1651608657469</v>
       </c>
       <c r="N55">
-        <v>0.0001997699855437323</v>
+        <v>-6.624582539336354E-29</v>
       </c>
       <c r="O55">
-        <v>-9.823416271014077</v>
+        <v>-273.9243793050162</v>
       </c>
       <c r="P55">
-        <v>-4.742690815982626</v>
+        <v>-16.95334649250927</v>
       </c>
     </row>
     <row r="56" spans="1:16">
       <c r="A56">
-        <v>388.9398426543783</v>
+        <v>12.69780102770439</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56">
-        <v>10.41419329716213</v>
+        <v>22.52282477820338</v>
       </c>
       <c r="D56">
-        <v>-0.000641254732964019</v>
+        <v>-0.01077731604276446</v>
       </c>
       <c r="E56">
-        <v>0.01203065834577294</v>
+        <v>0.005091053568056193</v>
       </c>
       <c r="F56">
-        <v>-1.150521440806501</v>
+        <v>-1.974623342200836</v>
       </c>
       <c r="G56">
-        <v>-0.02831959598955932</v>
+        <v>0.00488581305245185</v>
       </c>
       <c r="H56">
-        <v>9.383162734491275E-07</v>
+        <v>64.59154998711496</v>
       </c>
       <c r="I56">
-        <v>171.3186808947778</v>
+        <v>64.16249780497749</v>
       </c>
       <c r="J56">
-        <v>154.2304371166763</v>
+        <v>70.78371992988001</v>
       </c>
       <c r="K56">
-        <v>81.76668310681198</v>
+        <v>68.75421185934624</v>
       </c>
       <c r="L56">
-        <v>0.0004683507003417708</v>
+        <v>-0.01589649410062524</v>
       </c>
       <c r="M56">
-        <v>13.70726701677308</v>
+        <v>436.5805068569553</v>
       </c>
       <c r="N56">
-        <v>0.0001997618083345029</v>
+        <v>1.537391592796668E-27</v>
       </c>
       <c r="O56">
-        <v>-7.215808033424183</v>
+        <v>-275.7730645575422</v>
       </c>
       <c r="P56">
-        <v>-3.482728399756915</v>
+        <v>-4.318040816968792</v>
       </c>
     </row>
     <row r="57" spans="1:16">
       <c r="A57">
-        <v>389.4490399866193</v>
+        <v>12.92820008680493</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
       <c r="C57">
-        <v>10.21175428861547</v>
+        <v>23.04876388770719</v>
       </c>
       <c r="D57">
-        <v>-0.000432851353353996</v>
+        <v>-0.007254018003740477</v>
       </c>
       <c r="E57">
-        <v>0.009020077754621715</v>
+        <v>-0.005741199020544688</v>
       </c>
       <c r="F57">
-        <v>-1.287504645593823</v>
+        <v>-1.994620451105244</v>
       </c>
       <c r="G57">
-        <v>-0.02300347003089997</v>
+        <v>0.004755735290799788</v>
       </c>
       <c r="H57">
-        <v>3.84113850708343E-07</v>
+        <v>65.62154947119235</v>
       </c>
       <c r="I57">
-        <v>171.3538938989614</v>
+        <v>66.00181693176427</v>
       </c>
       <c r="J57">
-        <v>154.6427913556667</v>
+        <v>72.64410300182259</v>
       </c>
       <c r="K57">
-        <v>82.11353761754978</v>
+        <v>71.23148013850066</v>
       </c>
       <c r="L57">
-        <v>0.0004110237084717464</v>
+        <v>-0.007644599035413526</v>
       </c>
       <c r="M57">
-        <v>10.47720131606968</v>
+        <v>443.0433176791869</v>
       </c>
       <c r="N57">
-        <v>0.0001997507128386661</v>
+        <v>1.084809255320042E-28</v>
       </c>
       <c r="O57">
-        <v>-5.291341242239641</v>
+        <v>-283.0594031137477</v>
       </c>
       <c r="P57">
-        <v>-2.55347139176565</v>
+        <v>-0.4392686744444267</v>
       </c>
     </row>
     <row r="58" spans="1:16">
       <c r="A58">
-        <v>389.9687470974291</v>
+        <v>13.15348202580292</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58">
-        <v>9.995753403456565</v>
+        <v>23.55598631415235</v>
       </c>
       <c r="D58">
-        <v>-0.0002821446417660446</v>
+        <v>-0.003204549737869117</v>
       </c>
       <c r="E58">
-        <v>0.006765103456664595</v>
+        <v>-0.01058228958997999</v>
       </c>
       <c r="F58">
-        <v>-1.399045488322683</v>
+        <v>-1.99999946949124</v>
       </c>
       <c r="G58">
-        <v>-0.01893588395654465</v>
+        <v>0.002877153098402982</v>
       </c>
       <c r="H58">
-        <v>2.703544833358558E-08</v>
+        <v>67.44982549663361</v>
       </c>
       <c r="I58">
-        <v>171.3781308645132</v>
+        <v>67.19564481840062</v>
       </c>
       <c r="J58">
-        <v>155.1498187859613</v>
+        <v>74.39803962934799</v>
       </c>
       <c r="K58">
-        <v>82.58474692368466</v>
+        <v>73.32689799248394</v>
       </c>
       <c r="L58">
-        <v>0.0003586436656713179</v>
+        <v>-0.0009191491256197496</v>
       </c>
       <c r="M58">
-        <v>9.308304849218029</v>
+        <v>441.4123915148464</v>
       </c>
       <c r="N58">
-        <v>0.000199735861223443</v>
+        <v>3.578564923998964E-29</v>
       </c>
       <c r="O58">
-        <v>-3.877896021660475</v>
+        <v>-280.1324257312623</v>
       </c>
       <c r="P58">
-        <v>-1.871217866220606</v>
+        <v>2.239121827019806</v>
       </c>
     </row>
     <row r="59" spans="1:16">
       <c r="A59">
-        <v>390.5000169499079</v>
+        <v>13.37413336798776</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
       <c r="C59">
-        <v>9.77129267316943</v>
+        <v>24.02649350523733</v>
       </c>
       <c r="D59">
-        <v>-0.0001763478095069599</v>
+        <v>4.405031059662506E-05</v>
       </c>
       <c r="E59">
-        <v>0.005077634176713114</v>
+        <v>-0.01095113528741443</v>
       </c>
       <c r="F59">
-        <v>-1.49115539982555</v>
+        <v>-1.997995329610591</v>
       </c>
       <c r="G59">
-        <v>-0.01581723797702659</v>
+        <v>0.0004784570750179082</v>
       </c>
       <c r="H59">
-        <v>-2.176000434619272E-07</v>
+        <v>68.4561102559819</v>
       </c>
       <c r="I59">
-        <v>171.3947595608326</v>
+        <v>68.77283412519076</v>
       </c>
       <c r="J59">
-        <v>156.3284418691475</v>
+        <v>75.73425010866306</v>
       </c>
       <c r="K59">
-        <v>83.74384007102272</v>
+        <v>75.21427560366803</v>
       </c>
       <c r="L59">
-        <v>0.0003100361929419782</v>
+        <v>0.007027812333839</v>
       </c>
       <c r="M59">
-        <v>8.404986337823424</v>
+        <v>442.252938730777</v>
       </c>
       <c r="N59">
-        <v>0.0001997162200303187</v>
+        <v>2.191776469345094E-30</v>
       </c>
       <c r="O59">
-        <v>-2.842783032315081</v>
+        <v>-282.9434481013639</v>
       </c>
       <c r="P59">
-        <v>-1.371678821845765</v>
+        <v>0.8022067544612832</v>
       </c>
     </row>
     <row r="60" spans="1:16">
       <c r="A60">
-        <v>391.0437547542587</v>
+        <v>13.5906368690226</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
       <c r="C60">
-        <v>9.542185160218212</v>
+        <v>24.46761562216563</v>
       </c>
       <c r="D60">
-        <v>-0.0001040576466395266</v>
+        <v>0.002819398856350751</v>
       </c>
       <c r="E60">
-        <v>0.003814991261665513</v>
+        <v>-0.00697825805773308</v>
       </c>
       <c r="F60">
-        <v>-1.568404325568113</v>
+        <v>-1.991915840225344</v>
       </c>
       <c r="G60">
-        <v>-0.01342131266299415</v>
+        <v>-0.001476632088750429</v>
       </c>
       <c r="H60">
-        <v>-3.895385580098317E-07</v>
+        <v>70.01351034320673</v>
       </c>
       <c r="I60">
-        <v>171.4060894700621</v>
+        <v>69.82217409422954</v>
       </c>
       <c r="J60">
-        <v>158.0092911519104</v>
+        <v>77.06231528739983</v>
       </c>
       <c r="K60">
-        <v>85.41405181126223</v>
+        <v>76.71743044463342</v>
       </c>
       <c r="L60">
-        <v>0.0002653131898195549</v>
+        <v>0.008126363465820035</v>
       </c>
       <c r="M60">
-        <v>7.232496905739414</v>
+        <v>440.3382749522</v>
       </c>
       <c r="N60">
-        <v>0.0001996900955445323</v>
+        <v>1.377542464860059E-29</v>
       </c>
       <c r="O60">
-        <v>-2.085826436919751</v>
+        <v>-280.5187919297882</v>
       </c>
       <c r="P60">
-        <v>-1.006414101369191</v>
+        <v>1.662760382008889</v>
       </c>
     </row>
     <row r="61" spans="1:16">
       <c r="A61">
-        <v>391.6007564176062</v>
+        <v>13.80341810626703</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
       <c r="C61">
-        <v>9.3112500561269</v>
+        <v>24.87521503496018</v>
       </c>
       <c r="D61">
-        <v>-5.597786537648866E-05</v>
+        <v>0.003543112282022477</v>
       </c>
       <c r="E61">
-        <v>0.002869775765872218</v>
+        <v>-0.002313108320789624</v>
       </c>
       <c r="F61">
-        <v>-1.634268855483865</v>
+        <v>-1.985297196179395</v>
       </c>
       <c r="G61">
-        <v>-0.01157699030132441</v>
+        <v>-0.002465031085992346</v>
       </c>
       <c r="H61">
-        <v>-5.082780520796796E-07</v>
+        <v>70.94535293757322</v>
       </c>
       <c r="I61">
-        <v>171.4137483967926</v>
+        <v>71.14887505158923</v>
       </c>
       <c r="J61">
-        <v>159.8254556877939</v>
+        <v>78.17084037526534</v>
       </c>
       <c r="K61">
-        <v>87.22442044955559</v>
+        <v>78.16785417738534</v>
       </c>
       <c r="L61">
-        <v>0.0002248575064516223</v>
+        <v>0.007716898444950014</v>
       </c>
       <c r="M61">
-        <v>7.816262441656634</v>
+        <v>441.2140416227772</v>
       </c>
       <c r="N61">
-        <v>0.0001996545838521818</v>
+        <v>2.155968690372191E-30</v>
       </c>
       <c r="O61">
-        <v>-1.532481511433951</v>
+        <v>-282.6656477069695</v>
       </c>
       <c r="P61">
-        <v>-0.7394153097146714</v>
+        <v>0.5524195406049585</v>
       </c>
     </row>
     <row r="62" spans="1:16">
       <c r="A62">
-        <v>392.1717373846776</v>
+        <v>14.01284566600077</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
       <c r="C62">
-        <v>9.080551401623079</v>
+        <v>25.25806698070437</v>
       </c>
       <c r="D62">
-        <v>-2.494462106945585E-05</v>
+        <v>0.003151679616284214</v>
       </c>
       <c r="E62">
-        <v>0.002161562881917182</v>
+        <v>0.001936889933207007</v>
       </c>
       <c r="F62">
-        <v>-1.691396914352508</v>
+        <v>-1.98094711372665</v>
       </c>
       <c r="G62">
-        <v>-0.01015457848468331</v>
+        <v>-0.002498123699927706</v>
       </c>
       <c r="H62">
-        <v>-5.823621552858303E-07</v>
+        <v>72.25773869875196</v>
       </c>
       <c r="I62">
-        <v>171.4188868335516</v>
+        <v>72.08578514915888</v>
       </c>
       <c r="J62">
-        <v>162.5133873914778</v>
+        <v>79.31966045630027</v>
       </c>
       <c r="K62">
-        <v>89.90919011771156</v>
+        <v>79.42812534255813</v>
       </c>
       <c r="L62">
-        <v>0.0001889236247864851</v>
+        <v>0.003984338939220324</v>
       </c>
       <c r="M62">
-        <v>10.4910320464884</v>
+        <v>440.2218583029254</v>
       </c>
       <c r="N62">
-        <v>0.0001996049599964377</v>
+        <v>-4.418836325438934E-29</v>
       </c>
       <c r="O62">
-        <v>-1.127810932579923</v>
+        <v>-281.2314556765193</v>
       </c>
       <c r="P62">
-        <v>-0.5441599616818351</v>
+        <v>0.6271506802736259</v>
       </c>
     </row>
     <row r="63" spans="1:16">
       <c r="A63">
-        <v>392.7573544005883</v>
+        <v>14.21923162541453</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="C63">
-        <v>8.851585524261271</v>
+        <v>25.61434011708347</v>
       </c>
       <c r="D63">
-        <v>-5.646993185429463E-06</v>
+        <v>0.001760153631069652</v>
       </c>
       <c r="E63">
-        <v>0.001630317959076604</v>
+        <v>0.004158240509543088</v>
       </c>
       <c r="F63">
-        <v>-1.741808361599838</v>
+        <v>-1.980065096117542</v>
       </c>
       <c r="G63">
-        <v>-0.009055571004820819</v>
+        <v>-0.001858931070325327</v>
       </c>
       <c r="H63">
-        <v>-6.127360462332639E-07</v>
+        <v>73.10693578129042</v>
       </c>
       <c r="I63">
-        <v>171.4223112663841</v>
+        <v>73.22403316458468</v>
       </c>
       <c r="J63">
-        <v>167.0985304221826</v>
+        <v>80.37793374019853</v>
       </c>
       <c r="K63">
-        <v>94.4926046109792</v>
+        <v>80.61156602101046</v>
       </c>
       <c r="L63">
-        <v>0.0001575363143056968</v>
+        <v>0.001209228178324576</v>
       </c>
       <c r="M63">
-        <v>8.181244610761585</v>
+        <v>440.7849745155056</v>
       </c>
       <c r="N63">
-        <v>0.0001995341108780757</v>
+        <v>-5.297878702402491E-30</v>
       </c>
       <c r="O63">
-        <v>-0.8315786841067161</v>
+        <v>-282.6993987681153</v>
       </c>
       <c r="P63">
-        <v>-0.4012286358433014</v>
+        <v>-0.4635818549206762</v>
       </c>
     </row>
     <row r="64" spans="1:16">
       <c r="A64">
-        <v>393.3582220216385</v>
+        <v>14.42285139068643</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
       <c r="C64">
-        <v>8.625425098893372</v>
+        <v>25.949387934466</v>
       </c>
       <c r="D64">
-        <v>5.74213086144677E-06</v>
+        <v>0.0004163902762145762</v>
       </c>
       <c r="E64">
-        <v>0.001231299726642224</v>
+        <v>0.004767708811659001</v>
       </c>
       <c r="F64">
-        <v>-1.787046680340905</v>
+        <v>-1.982229727911674</v>
       </c>
       <c r="G64">
-        <v>-0.008204979862981963</v>
+        <v>-0.0009419263301016941</v>
       </c>
       <c r="H64">
-        <v>-5.928441409179228E-07</v>
+        <v>74.21283367017635</v>
       </c>
       <c r="I64">
-        <v>171.4245804701144</v>
+        <v>74.07448620573456</v>
       </c>
       <c r="J64">
-        <v>170.8192393054927</v>
+        <v>81.47474165363556</v>
       </c>
       <c r="K64">
-        <v>98.21236625036269</v>
+        <v>81.61787564299281</v>
       </c>
       <c r="L64">
-        <v>0.0001305140869346155</v>
+        <v>-0.001963827259961594</v>
       </c>
       <c r="M64">
-        <v>1.909988756214035</v>
+        <v>439.8754243026239</v>
       </c>
       <c r="N64">
-        <v>0.0001994272530047032</v>
+        <v>-2.961536548127957E-30</v>
       </c>
       <c r="O64">
-        <v>-0.6144265338082043</v>
+        <v>-281.5575462053598</v>
       </c>
       <c r="P64">
-        <v>-0.2964540540581682</v>
+        <v>-0.3285367685865132</v>
       </c>
     </row>
     <row r="65" spans="1:16">
       <c r="A65">
-        <v>393.9749252113708</v>
+        <v>14.62394765235881</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="C65">
-        <v>8.402828228634046</v>
+        <v>26.26162163751965</v>
       </c>
       <c r="D65">
-        <v>1.19202139149539E-05</v>
+        <v>-0.0007950274280725685</v>
       </c>
       <c r="E65">
-        <v>0.0009311807337273499</v>
+        <v>0.00373024822120531</v>
       </c>
       <c r="F65">
-        <v>-1.828293562124868</v>
+        <v>-1.986361849852085</v>
       </c>
       <c r="G65">
-        <v>-0.007545588942431365</v>
+        <v>-8.14858420235277E-05</v>
       </c>
       <c r="H65">
-        <v>-5.052588358815846E-07</v>
+        <v>74.97953087159206</v>
       </c>
       <c r="I65">
-        <v>171.4260770743564</v>
+        <v>75.05760147901722</v>
       </c>
       <c r="J65">
-        <v>171.3028513515576</v>
+        <v>82.48447334663639</v>
       </c>
       <c r="K65">
-        <v>98.69545775755171</v>
+        <v>82.56403194703815</v>
       </c>
       <c r="L65">
-        <v>0.000107531351706215</v>
+        <v>-0.003008505676550867</v>
       </c>
       <c r="M65">
-        <v>0.878598996686098</v>
+        <v>440.0529158358166</v>
       </c>
       <c r="N65">
-        <v>0.000199251683531927</v>
+        <v>7.239456466319677E-31</v>
       </c>
       <c r="O65">
-        <v>-0.4549764558209604</v>
+        <v>-282.4967468467839</v>
       </c>
       <c r="P65">
-        <v>-0.2195206974945897</v>
+        <v>-0.8685256198183162</v>
       </c>
     </row>
     <row r="66" spans="1:16">
       <c r="A66">
-        <v>394.6080290086285</v>
+        <v>14.82273851727173</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66">
-        <v>8.184320217448974</v>
+        <v>26.55508450395694</v>
       </c>
       <c r="D66">
-        <v>1.475342967888158E-05</v>
+        <v>-0.001354133202986988</v>
       </c>
       <c r="E66">
-        <v>0.0007051279545345824</v>
+        <v>0.00210608957344559</v>
       </c>
       <c r="F66">
-        <v>-1.866455467089181</v>
+        <v>-1.991098758059789</v>
       </c>
       <c r="G66">
-        <v>-0.007033642363963323</v>
+        <v>0.0005003984128530284</v>
       </c>
       <c r="H66">
-        <v>-3.109246577817797E-07</v>
+        <v>75.91701046340093</v>
       </c>
       <c r="I66">
-        <v>171.4270603640373</v>
+        <v>75.82659446642462</v>
       </c>
       <c r="J66">
-        <v>171.3630306959952</v>
+        <v>83.4807390392009</v>
       </c>
       <c r="K66">
-        <v>98.75535019423418</v>
+        <v>83.39388859602673</v>
       </c>
       <c r="L66">
-        <v>8.818135453328694E-05</v>
+        <v>-0.003558207949539017</v>
       </c>
       <c r="M66">
-        <v>0.5936882724959863</v>
+        <v>439.3727165189503</v>
       </c>
       <c r="N66">
-        <v>0.0001989337014573517</v>
+        <v>2.003180276175655E-25</v>
       </c>
       <c r="O66">
-        <v>-0.3376738781746061</v>
+        <v>-281.720427899179</v>
       </c>
       <c r="P66">
-        <v>-0.1629233199467273</v>
+        <v>-0.4623981423582945</v>
       </c>
     </row>
     <row r="67" spans="1:16">
       <c r="A67">
-        <v>395.2580859984504</v>
+        <v>15.01941638397542</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67">
-        <v>7.970254482932585</v>
+        <v>26.8292556215936</v>
       </c>
       <c r="D67">
-        <v>1.551093441176104E-05</v>
+        <v>-0.001491840966995927</v>
       </c>
       <c r="E67">
-        <v>0.0005346220957941419</v>
+        <v>0.0002549100499349298</v>
       </c>
       <c r="F67">
-        <v>-1.902229071863976</v>
+        <v>-1.995372416725188</v>
       </c>
       <c r="G67">
-        <v>-0.006635603505619162</v>
+        <v>0.0007319230745700741</v>
       </c>
       <c r="H67">
-        <v>8.398746372076246E-08</v>
+        <v>76.61083517407528</v>
       </c>
       <c r="I67">
-        <v>171.4277045237287</v>
+        <v>76.67591228483252</v>
       </c>
       <c r="J67">
-        <v>171.3775219643343</v>
+        <v>84.38182869155985</v>
       </c>
       <c r="K67">
-        <v>98.76968283265738</v>
+        <v>84.20825876198447</v>
       </c>
       <c r="L67">
-        <v>7.20263745884902E-05</v>
+        <v>-0.002423878090414986</v>
       </c>
       <c r="M67">
-        <v>0.420562868038233</v>
+        <v>439.5034026761299</v>
       </c>
       <c r="N67">
-        <v>0.0001982604817998707</v>
+        <v>-2.771650830179325E-30</v>
       </c>
       <c r="O67">
-        <v>-0.2512006972994641</v>
+        <v>-282.3991618850509</v>
       </c>
       <c r="P67">
-        <v>-0.1212009196221042</v>
+        <v>-0.6583232212184169</v>
       </c>
     </row>
     <row r="68" spans="1:16">
       <c r="A68">
-        <v>395.9256421285528</v>
+        <v>15.21415356732201</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="C68">
-        <v>7.76085776165798</v>
+        <v>27.08726181182552</v>
       </c>
       <c r="D68">
-        <v>1.504102035925825E-05</v>
+        <v>-0.00111611589486981</v>
       </c>
       <c r="E68">
-        <v>0.0004058358640371129</v>
+        <v>-0.001029550424399625</v>
       </c>
       <c r="F68">
-        <v>-1.936150828262598</v>
+        <v>-1.998439550382097</v>
       </c>
       <c r="G68">
-        <v>-0.006325713448382566</v>
+        <v>0.0006535240976610539</v>
       </c>
       <c r="H68">
-        <v>9.716438521626506E-07</v>
+        <v>77.41591893271378</v>
       </c>
       <c r="I68">
-        <v>171.4281258878046</v>
+        <v>77.36604057434529</v>
       </c>
       <c r="J68">
-        <v>171.3785875974138</v>
+        <v>85.25225262628889</v>
       </c>
       <c r="K68">
-        <v>98.77066047965519</v>
+        <v>84.95703433454239</v>
       </c>
       <c r="L68">
-        <v>5.863277957634517E-05</v>
+        <v>-0.001240881674720904</v>
       </c>
       <c r="M68">
-        <v>0.3058680980261133</v>
+        <v>439.0300490728508</v>
       </c>
       <c r="N68">
-        <v>0.0001964599286752743</v>
+        <v>1.574780678346522E-29</v>
       </c>
       <c r="O68">
-        <v>-0.1873159399746704</v>
+        <v>-281.8996399718433</v>
       </c>
       <c r="P68">
-        <v>-0.09037725187354977</v>
+        <v>-0.3343038851291994</v>
       </c>
     </row>
     <row r="69" spans="1:16">
       <c r="A69">
-        <v>396.6112412756376</v>
+        <v>15.40710306629226</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69">
-        <v>7.556263593442317</v>
+        <v>27.32895537111682</v>
       </c>
       <c r="D69">
-        <v>1.389979795403131E-05</v>
+        <v>-0.0005858524395284717</v>
       </c>
       <c r="E69">
-        <v>0.000308430666867994</v>
+        <v>-0.001679553049499067</v>
       </c>
       <c r="F69">
-        <v>-1.968634560728888</v>
+        <v>-1.999981877029894</v>
       </c>
       <c r="G69">
-        <v>-0.00608414715965624</v>
+        <v>0.0003889392242223858</v>
       </c>
       <c r="H69">
-        <v>3.221765016341848E-06</v>
+        <v>78.04686464195264</v>
       </c>
       <c r="I69">
-        <v>171.4284022068507</v>
+        <v>78.10011496271376</v>
       </c>
       <c r="J69">
-        <v>171.3769697587052</v>
+        <v>86.04696404102258</v>
       </c>
       <c r="K69">
-        <v>98.76899368055834</v>
+        <v>85.69178015169136</v>
       </c>
       <c r="L69">
-        <v>4.759327134020422E-05</v>
+        <v>0.00047885976984989</v>
       </c>
       <c r="M69">
-        <v>0.2265361824668302</v>
+        <v>439.0291929333104</v>
       </c>
       <c r="N69">
-        <v>0.0001893392485850571</v>
+        <v>-3.829987378389947E-31</v>
       </c>
       <c r="O69">
-        <v>-0.1400124910182405</v>
+        <v>-282.3165693347185</v>
       </c>
       <c r="P69">
-        <v>-0.06755391564618882</v>
+        <v>-0.5395691786072626</v>
       </c>
     </row>
     <row r="70" spans="1:16">
       <c r="A70">
-        <v>397.3154288634393</v>
+        <v>15.59840362962104</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="C70">
-        <v>7.356537110463023</v>
+        <v>27.55644293163924</v>
       </c>
       <c r="D70">
-        <v>1.244348670121387E-05</v>
+        <v>3.199070130129252E-05</v>
       </c>
       <c r="E70">
-        <v>0.0002346651002253361</v>
+        <v>-0.00149072459056563</v>
       </c>
       <c r="F70">
-        <v>-2.000000048262731</v>
+        <v>-1.999986857351332</v>
       </c>
       <c r="G70">
-        <v>-0.005895617306052557</v>
+        <v>8.264284133753508E-05</v>
       </c>
       <c r="H70">
-        <v>-2.952691669241955E-06</v>
+        <v>78.74533055573271</v>
       </c>
       <c r="I70">
-        <v>171.4285743810969</v>
+        <v>78.71558281461846</v>
       </c>
       <c r="J70">
-        <v>171.3763995832639</v>
+        <v>86.81777224625216</v>
       </c>
       <c r="K70">
-        <v>98.76839617254761</v>
+        <v>86.36455145499291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>